<commit_message>
Refactor MOGWO algorithm to MOMGO with new search strategy
- Rename algorithm from MOGWO (Grey Wolf Optimizer) to MOMGO (modified optimization approach)
- Replace wolf pack hunting mechanism with new randomized search strategy
- Implement new position update logic using coefficient vectors and random solutions
- Add multi-location update approach with boundary checking
- Include dynamic herd management with new solution additions
- Update visualization and leader selection process

The changes introduce a fundamentally different optimization approach while maintaining the multi-objective framework.
</commit_message>
<xml_diff>
--- a/Optimal.xlsx
+++ b/Optimal.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="6">
   <si>
     <t>X1</t>
   </si>
@@ -76,18 +76,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="true"/>
-    <col min="2" max="2" width="12.5546875" customWidth="true"/>
+    <col min="1" max="1" width="13.5546875" customWidth="true"/>
+    <col min="2" max="2" width="14.5546875" customWidth="true"/>
     <col min="3" max="3" width="13.5546875" customWidth="true"/>
-    <col min="4" max="4" width="13.5546875" customWidth="true"/>
-    <col min="5" max="5" width="14.5546875" customWidth="true"/>
-    <col min="6" max="6" width="11.5546875" customWidth="true"/>
+    <col min="4" max="4" width="14.5546875" customWidth="true"/>
+    <col min="5" max="5" width="13.5546875" customWidth="true"/>
+    <col min="6" max="6" width="12.5546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -112,762 +112,982 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.23275606037585905</v>
+        <v>0.29150969148882722</v>
       </c>
       <c r="B2" s="0">
-        <v>0.62429497362449737</v>
+        <v>0.15021372056613569</v>
       </c>
       <c r="C2" s="0">
-        <v>0.18477715127186933</v>
+        <v>0.055921997167276749</v>
       </c>
       <c r="D2" s="0">
-        <v>0.064433510320585752</v>
+        <v>0.068352401695925935</v>
       </c>
       <c r="E2" s="0">
-        <v>0.23275606037585905</v>
+        <v>0.29150969148882722</v>
       </c>
       <c r="F2" s="0">
-        <v>2.7025314746752405</v>
+        <v>1.0943844363827335</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.59226501429759171</v>
+        <v>0.077189113646382146</v>
       </c>
       <c r="B3" s="0">
-        <v>0.78768067613275916</v>
+        <v>0.077189113646382146</v>
       </c>
       <c r="C3" s="0">
-        <v>0.05368240643228217</v>
+        <v>0.077189113646382146</v>
       </c>
       <c r="D3" s="0">
-        <v>0.1364286393297075</v>
+        <v>0.077189113646382146</v>
       </c>
       <c r="E3" s="0">
-        <v>0.59226501429759171</v>
+        <v>0.29150969148882722</v>
       </c>
       <c r="F3" s="0">
-        <v>2.4070722800348183</v>
+        <v>1.0943844363827335</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.84322393817237284</v>
       </c>
       <c r="B4" s="0">
-        <v>0.1035295990612185</v>
+        <v>0.84322393817237284</v>
       </c>
       <c r="C4" s="0">
-        <v>0.19187604844290351</v>
+        <v>0.84322393817237284</v>
       </c>
       <c r="D4" s="0">
-        <v>0.236923268229007</v>
+        <v>0.84322393817237284</v>
       </c>
       <c r="E4" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.29150969148882722</v>
       </c>
       <c r="F4" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.0943844363827335</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.11498199876870274</v>
+        <v>0</v>
       </c>
       <c r="B5" s="0">
-        <v>0.4303761828434064</v>
+        <v>0.23658895007515812</v>
       </c>
       <c r="C5" s="0">
-        <v>0.20458692422542668</v>
+        <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>0.48676739162024529</v>
+        <v>0.073247606412435107</v>
       </c>
       <c r="E5" s="0">
-        <v>0.11498199876870274</v>
+        <v>0.077189113646382146</v>
       </c>
       <c r="F5" s="0">
-        <v>3.6567294694024635</v>
+        <v>1.3330218505159859</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0.89893981332804307</v>
       </c>
       <c r="B6" s="0">
-        <v>0.26758722415481262</v>
+        <v>0.89893981332804307</v>
       </c>
       <c r="C6" s="0">
-        <v>0.62753472454918635</v>
+        <v>0.89893981332804307</v>
       </c>
       <c r="D6" s="0">
-        <v>0.67557004386782837</v>
+        <v>0.89893981332804307</v>
       </c>
       <c r="E6" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0</v>
       </c>
       <c r="F6" s="0">
-        <v>5.4884618200815289</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.74693206205889351</v>
+        <v>0.71955589370827833</v>
       </c>
       <c r="B7" s="0">
-        <v>0.1384817810454122</v>
+        <v>0.71955589370827833</v>
       </c>
       <c r="C7" s="0">
-        <v>0.12170853114703628</v>
+        <v>0.71955589370827833</v>
       </c>
       <c r="D7" s="0">
-        <v>0.38770186764823156</v>
+        <v>0.71955589370827833</v>
       </c>
       <c r="E7" s="0">
-        <v>0.74693206205889351</v>
+        <v>0</v>
       </c>
       <c r="F7" s="0">
-        <v>1.4608662388768145</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.83842961795480531</v>
+        <v>1</v>
       </c>
       <c r="B8" s="0">
-        <v>0.1035295990612185</v>
+        <v>0.6807751271799658</v>
       </c>
       <c r="C8" s="0">
-        <v>0.19187604844290351</v>
+        <v>1</v>
       </c>
       <c r="D8" s="0">
-        <v>0.236923268229007</v>
+        <v>0.84754181853670918</v>
       </c>
       <c r="E8" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.077189113646382146</v>
       </c>
       <c r="F8" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.3330218505159859</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0.0087539612024455371</v>
+        <v>1</v>
       </c>
       <c r="B9" s="0">
-        <v>0.26758722415481262</v>
+        <v>0.93419071587248204</v>
       </c>
       <c r="C9" s="0">
-        <v>0.62753472454918635</v>
+        <v>1</v>
       </c>
       <c r="D9" s="0">
-        <v>0.67557004386782837</v>
+        <v>0</v>
       </c>
       <c r="E9" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0.29150969148882722</v>
       </c>
       <c r="F9" s="0">
-        <v>5.4884618200815289</v>
+        <v>1.0943844363827335</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.74693206205889351</v>
+        <v>0.13335881945498218</v>
       </c>
       <c r="B10" s="0">
-        <v>0.1384817810454122</v>
+        <v>0.13335881945498218</v>
       </c>
       <c r="C10" s="0">
-        <v>0.12170853114703628</v>
+        <v>0.13335881945498218</v>
       </c>
       <c r="D10" s="0">
-        <v>0.38770186764823156</v>
+        <v>0.13335881945498218</v>
       </c>
       <c r="E10" s="0">
-        <v>0.74693206205889351</v>
+        <v>0</v>
       </c>
       <c r="F10" s="0">
-        <v>1.4608662388768145</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.20152531051941514</v>
       </c>
       <c r="B11" s="0">
-        <v>0.1035295990612185</v>
+        <v>0.20152531051941514</v>
       </c>
       <c r="C11" s="0">
-        <v>0.19187604844290351</v>
+        <v>0.20152531051941514</v>
       </c>
       <c r="D11" s="0">
-        <v>0.236923268229007</v>
+        <v>0.20152531051941514</v>
       </c>
       <c r="E11" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F11" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0.82407977286481915</v>
       </c>
       <c r="B12" s="0">
-        <v>0.26758722415481262</v>
+        <v>0.82407977286481915</v>
       </c>
       <c r="C12" s="0">
-        <v>0.62753472454918635</v>
+        <v>0.82407977286481915</v>
       </c>
       <c r="D12" s="0">
-        <v>0.67557004386782837</v>
+        <v>0.82407977286481915</v>
       </c>
       <c r="E12" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0</v>
       </c>
       <c r="F12" s="0">
-        <v>5.4884618200815289</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.83842961795480531</v>
+        <v>1</v>
       </c>
       <c r="B13" s="0">
-        <v>0.1035295990612185</v>
+        <v>1</v>
       </c>
       <c r="C13" s="0">
-        <v>0.19187604844290351</v>
+        <v>1</v>
       </c>
       <c r="D13" s="0">
-        <v>0.236923268229007</v>
+        <v>1</v>
       </c>
       <c r="E13" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.077189113646382146</v>
       </c>
       <c r="F13" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.3330218505159859</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.0087539612024455371</v>
+        <v>1</v>
       </c>
       <c r="B14" s="0">
-        <v>0.26758722415481262</v>
+        <v>1</v>
       </c>
       <c r="C14" s="0">
-        <v>0.62753472454918635</v>
+        <v>1</v>
       </c>
       <c r="D14" s="0">
-        <v>0.67557004386782837</v>
+        <v>1</v>
       </c>
       <c r="E14" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0</v>
       </c>
       <c r="F14" s="0">
-        <v>5.4884618200815289</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.30189286053120012</v>
       </c>
       <c r="B15" s="0">
-        <v>0.1035295990612185</v>
+        <v>0.94109380406463461</v>
       </c>
       <c r="C15" s="0">
-        <v>0.19187604844290351</v>
+        <v>0.8965035496044933</v>
       </c>
       <c r="D15" s="0">
-        <v>0.236923268229007</v>
+        <v>0.33792901932329156</v>
       </c>
       <c r="E15" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F15" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.0087539612024455371</v>
+        <v>1</v>
       </c>
       <c r="B16" s="0">
-        <v>0.26758722415481262</v>
+        <v>0.93124453542360486</v>
       </c>
       <c r="C16" s="0">
-        <v>0.62753472454918635</v>
+        <v>0.61945306940279166</v>
       </c>
       <c r="D16" s="0">
-        <v>0.67557004386782837</v>
+        <v>0.78227178659946506</v>
       </c>
       <c r="E16" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0</v>
       </c>
       <c r="F16" s="0">
-        <v>5.4884618200815289</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.83842961795480531</v>
+        <v>1</v>
       </c>
       <c r="B17" s="0">
-        <v>0.1035295990612185</v>
+        <v>1</v>
       </c>
       <c r="C17" s="0">
-        <v>0.19187604844290351</v>
+        <v>1</v>
       </c>
       <c r="D17" s="0">
-        <v>0.236923268229007</v>
+        <v>0.98636367948592119</v>
       </c>
       <c r="E17" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F17" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0.55185278833681684</v>
       </c>
       <c r="B18" s="0">
-        <v>0.26758722415481262</v>
+        <v>0.4667311079084242</v>
       </c>
       <c r="C18" s="0">
-        <v>0.62753472454918635</v>
+        <v>0.29582532268418543</v>
       </c>
       <c r="D18" s="0">
-        <v>0.67557004386782837</v>
+        <v>0</v>
       </c>
       <c r="E18" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0.62589639308841771</v>
       </c>
       <c r="F18" s="0">
-        <v>5.4884618200815289</v>
+        <v>0.65426847911508668</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="B19" s="0">
-        <v>0.1035295990612185</v>
+        <v>1</v>
       </c>
       <c r="C19" s="0">
-        <v>0.19187604844290351</v>
+        <v>0</v>
       </c>
       <c r="D19" s="0">
-        <v>0.236923268229007</v>
+        <v>0.36100432451725162</v>
       </c>
       <c r="E19" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F19" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0</v>
       </c>
       <c r="B20" s="0">
-        <v>0.26758722415481262</v>
+        <v>0</v>
       </c>
       <c r="C20" s="0">
-        <v>0.62753472454918635</v>
+        <v>0</v>
       </c>
       <c r="D20" s="0">
-        <v>0.67557004386782837</v>
+        <v>0</v>
       </c>
       <c r="E20" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0</v>
       </c>
       <c r="F20" s="0">
-        <v>5.4884618200815289</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.99179998526696</v>
       </c>
       <c r="B21" s="0">
-        <v>0.1035295990612185</v>
+        <v>0.64903151508563017</v>
       </c>
       <c r="C21" s="0">
-        <v>0.19187604844290351</v>
+        <v>1</v>
       </c>
       <c r="D21" s="0">
-        <v>0.236923268229007</v>
+        <v>0.7583541282064753</v>
       </c>
       <c r="E21" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F21" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0</v>
       </c>
       <c r="B22" s="0">
-        <v>0.26758722415481262</v>
+        <v>0.9707716350527823</v>
       </c>
       <c r="C22" s="0">
-        <v>0.62753472454918635</v>
+        <v>0</v>
       </c>
       <c r="D22" s="0">
-        <v>0.67557004386782837</v>
+        <v>0.88388994263013598</v>
       </c>
       <c r="E22" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0</v>
       </c>
       <c r="F22" s="0">
-        <v>5.4884618200815289</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.66728677516521773</v>
       </c>
       <c r="B23" s="0">
-        <v>0.1035295990612185</v>
+        <v>0.68026336522163799</v>
       </c>
       <c r="C23" s="0">
-        <v>0.19187604844290351</v>
+        <v>0</v>
       </c>
       <c r="D23" s="0">
-        <v>0.236923268229007</v>
+        <v>0</v>
       </c>
       <c r="E23" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F23" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0.88994481199442155</v>
       </c>
       <c r="B24" s="0">
-        <v>0.26758722415481262</v>
+        <v>0.90682858633178776</v>
       </c>
       <c r="C24" s="0">
-        <v>0.62753472454918635</v>
+        <v>0.50865495247334269</v>
       </c>
       <c r="D24" s="0">
-        <v>0.67557004386782837</v>
+        <v>0.29257977307463567</v>
       </c>
       <c r="E24" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0</v>
       </c>
       <c r="F24" s="0">
-        <v>5.4884618200815289</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.83842961795480531</v>
+        <v>1</v>
       </c>
       <c r="B25" s="0">
-        <v>0.1035295990612185</v>
+        <v>0.78820031079388286</v>
       </c>
       <c r="C25" s="0">
-        <v>0.19187604844290351</v>
+        <v>1</v>
       </c>
       <c r="D25" s="0">
-        <v>0.236923268229007</v>
+        <v>1</v>
       </c>
       <c r="E25" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F25" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0</v>
       </c>
       <c r="B26" s="0">
-        <v>0.26758722415481262</v>
+        <v>0</v>
       </c>
       <c r="C26" s="0">
-        <v>0.62753472454918635</v>
+        <v>0</v>
       </c>
       <c r="D26" s="0">
-        <v>0.67557004386782837</v>
+        <v>0</v>
       </c>
       <c r="E26" s="0">
-        <v>0.0087539612024455371</v>
+        <v>0</v>
       </c>
       <c r="F26" s="0">
-        <v>5.4884618200815289</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.55616370047907149</v>
       </c>
       <c r="B27" s="0">
-        <v>0.1035295990612185</v>
+        <v>0.84436781473935107</v>
       </c>
       <c r="C27" s="0">
-        <v>0.19187604844290351</v>
+        <v>0.69366182334053672</v>
       </c>
       <c r="D27" s="0">
-        <v>0.236923268229007</v>
+        <v>0.7969283804409355</v>
       </c>
       <c r="E27" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F27" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.83842961795480531</v>
+        <v>1</v>
       </c>
       <c r="B28" s="0">
-        <v>0.1035295990612185</v>
+        <v>1</v>
       </c>
       <c r="C28" s="0">
-        <v>0.19187604844290351</v>
+        <v>1</v>
       </c>
       <c r="D28" s="0">
-        <v>0.236923268229007</v>
+        <v>0.26765306442105102</v>
       </c>
       <c r="E28" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F28" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>0.83842961795480531</v>
+        <v>1</v>
       </c>
       <c r="B29" s="0">
-        <v>0.1035295990612185</v>
+        <v>1</v>
       </c>
       <c r="C29" s="0">
-        <v>0.19187604844290351</v>
+        <v>0</v>
       </c>
       <c r="D29" s="0">
-        <v>0.236923268229007</v>
+        <v>0</v>
       </c>
       <c r="E29" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F29" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0.83842961795480531</v>
+        <v>1</v>
       </c>
       <c r="B30" s="0">
-        <v>0.1035295990612185</v>
+        <v>0.27966283451250251</v>
       </c>
       <c r="C30" s="0">
-        <v>0.19187604844290351</v>
+        <v>0</v>
       </c>
       <c r="D30" s="0">
-        <v>0.236923268229007</v>
+        <v>0.050059440791189611</v>
       </c>
       <c r="E30" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F30" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="B31" s="0">
-        <v>0.1035295990612185</v>
+        <v>0</v>
       </c>
       <c r="C31" s="0">
-        <v>0.19187604844290351</v>
+        <v>0</v>
       </c>
       <c r="D31" s="0">
-        <v>0.236923268229007</v>
+        <v>0</v>
       </c>
       <c r="E31" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F31" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.37383848887580456</v>
       </c>
       <c r="B32" s="0">
-        <v>0.1035295990612185</v>
+        <v>0.43956474371474069</v>
       </c>
       <c r="C32" s="0">
-        <v>0.19187604844290351</v>
+        <v>0.26435198278410665</v>
       </c>
       <c r="D32" s="0">
-        <v>0.236923268229007</v>
+        <v>0</v>
       </c>
       <c r="E32" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F32" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.44991443863782377</v>
       </c>
       <c r="B33" s="0">
-        <v>0.1035295990612185</v>
+        <v>0.48255259095290598</v>
       </c>
       <c r="C33" s="0">
-        <v>0.19187604844290351</v>
+        <v>0.41273234313763635</v>
       </c>
       <c r="D33" s="0">
-        <v>0.236923268229007</v>
+        <v>0.19030396392451202</v>
       </c>
       <c r="E33" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F33" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.60337240665257497</v>
       </c>
       <c r="B34" s="0">
-        <v>0.1035295990612185</v>
+        <v>0.79043307979119626</v>
       </c>
       <c r="C34" s="0">
-        <v>0.19187604844290351</v>
+        <v>0.64718160604492214</v>
       </c>
       <c r="D34" s="0">
-        <v>0.236923268229007</v>
+        <v>0.025490857145197655</v>
       </c>
       <c r="E34" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F34" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>0.83842961795480531</v>
+        <v>0.076211500955900124</v>
       </c>
       <c r="B35" s="0">
-        <v>0.1035295990612185</v>
+        <v>0</v>
       </c>
       <c r="C35" s="0">
-        <v>0.19187604844290351</v>
+        <v>0.053942058463242806</v>
       </c>
       <c r="D35" s="0">
-        <v>0.236923268229007</v>
+        <v>0</v>
       </c>
       <c r="E35" s="0">
-        <v>0.83842961795480531</v>
+        <v>0</v>
       </c>
       <c r="F35" s="0">
-        <v>1.1213883579728081</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.26534948483764864</v>
+        <v>0.5497932757823405</v>
       </c>
       <c r="B36" s="0">
-        <v>0.80258777917942647</v>
+        <v>0.63210698787651698</v>
       </c>
       <c r="C36" s="0">
-        <v>0.031949916894432606</v>
+        <v>0.77682075784954119</v>
       </c>
       <c r="D36" s="0">
-        <v>0.12373934270314957</v>
+        <v>0.44182461108858473</v>
       </c>
       <c r="E36" s="0">
-        <v>0.26534948483764864</v>
+        <v>0</v>
       </c>
       <c r="F36" s="0">
-        <v>2.8608368162724265</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.26534948483764864</v>
+        <v>0.36202218259607749</v>
       </c>
       <c r="B37" s="0">
-        <v>0.80258777917942647</v>
+        <v>0.72556999344065309</v>
       </c>
       <c r="C37" s="0">
-        <v>0.031949916894432606</v>
+        <v>0.065100509595460571</v>
       </c>
       <c r="D37" s="0">
-        <v>0.12373934270314957</v>
+        <v>0.62247871914728981</v>
       </c>
       <c r="E37" s="0">
-        <v>0.26534948483764864</v>
+        <v>0</v>
       </c>
       <c r="F37" s="0">
-        <v>2.8608368162724265</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>0.26534948483764864</v>
+        <v>0.86616963721181561</v>
       </c>
       <c r="B38" s="0">
-        <v>0.80258777917942647</v>
+        <v>0</v>
       </c>
       <c r="C38" s="0">
-        <v>0.031949916894432606</v>
+        <v>1</v>
       </c>
       <c r="D38" s="0">
-        <v>0.12373934270314957</v>
+        <v>0</v>
       </c>
       <c r="E38" s="0">
-        <v>0.26534948483764864</v>
+        <v>0</v>
       </c>
       <c r="F38" s="0">
-        <v>2.8608368162724265</v>
+        <v>1.9295096694627798</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0.26534948483764864</v>
+        <v>0.27118206175103515</v>
       </c>
       <c r="B39" s="0">
-        <v>0.80258777917942647</v>
+        <v>0.33793538575048293</v>
       </c>
       <c r="C39" s="0">
-        <v>0.031949916894432606</v>
+        <v>0.27159601348696827</v>
       </c>
       <c r="D39" s="0">
-        <v>0.12373934270314957</v>
+        <v>0.31273979788675244</v>
       </c>
       <c r="E39" s="0">
-        <v>0.26534948483764864</v>
+        <v>0</v>
       </c>
       <c r="F39" s="0">
-        <v>2.8608368162724265</v>
+        <v>1.9295096694627798</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>0.3726830944684788</v>
+      </c>
+      <c r="B40" s="0">
+        <v>0</v>
+      </c>
+      <c r="C40" s="0">
+        <v>0.31784621087819043</v>
+      </c>
+      <c r="D40" s="0">
+        <v>0</v>
+      </c>
+      <c r="E40" s="0">
+        <v>0</v>
+      </c>
+      <c r="F40" s="0">
+        <v>1.9295096694627798</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>1</v>
+      </c>
+      <c r="B41" s="0">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0">
+        <v>1</v>
+      </c>
+      <c r="D41" s="0">
+        <v>1</v>
+      </c>
+      <c r="E41" s="0">
+        <v>0</v>
+      </c>
+      <c r="F41" s="0">
+        <v>1.9295096694627798</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>0.39331566717778699</v>
+      </c>
+      <c r="B42" s="0">
+        <v>0.8023440427901507</v>
+      </c>
+      <c r="C42" s="0">
+        <v>0</v>
+      </c>
+      <c r="D42" s="0">
+        <v>0.074096107482310269</v>
+      </c>
+      <c r="E42" s="0">
+        <v>0</v>
+      </c>
+      <c r="F42" s="0">
+        <v>1.9295096694627798</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>0.25210430483922869</v>
+      </c>
+      <c r="B43" s="0">
+        <v>1</v>
+      </c>
+      <c r="C43" s="0">
+        <v>1</v>
+      </c>
+      <c r="D43" s="0">
+        <v>1</v>
+      </c>
+      <c r="E43" s="0">
+        <v>0</v>
+      </c>
+      <c r="F43" s="0">
+        <v>1.9295096694627798</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>1</v>
+      </c>
+      <c r="B44" s="0">
+        <v>1</v>
+      </c>
+      <c r="C44" s="0">
+        <v>1</v>
+      </c>
+      <c r="D44" s="0">
+        <v>0.0054421490853886695</v>
+      </c>
+      <c r="E44" s="0">
+        <v>0</v>
+      </c>
+      <c r="F44" s="0">
+        <v>1.9295096694627798</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>0</v>
+      </c>
+      <c r="B45" s="0">
+        <v>0.0026598599078565544</v>
+      </c>
+      <c r="C45" s="0">
+        <v>0.18152555110511048</v>
+      </c>
+      <c r="D45" s="0">
+        <v>0.53969925371476823</v>
+      </c>
+      <c r="E45" s="0">
+        <v>0</v>
+      </c>
+      <c r="F45" s="0">
+        <v>1.9295096694627798</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>0.99597898046122069</v>
+      </c>
+      <c r="B46" s="0">
+        <v>0.79045788144483853</v>
+      </c>
+      <c r="C46" s="0">
+        <v>0.085727546061760473</v>
+      </c>
+      <c r="D46" s="0">
+        <v>0.57643881595177038</v>
+      </c>
+      <c r="E46" s="0">
+        <v>0</v>
+      </c>
+      <c r="F46" s="0">
+        <v>1.9295096694627798</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>0.72541144070463148</v>
+      </c>
+      <c r="B47" s="0">
+        <v>0.70577426394726284</v>
+      </c>
+      <c r="C47" s="0">
+        <v>0.44395219730245172</v>
+      </c>
+      <c r="D47" s="0">
+        <v>0.29142558632006482</v>
+      </c>
+      <c r="E47" s="0">
+        <v>0</v>
+      </c>
+      <c r="F47" s="0">
+        <v>1.9295096694627798</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>0.74076059672179462</v>
+      </c>
+      <c r="B48" s="0">
+        <v>0.68414918268037028</v>
+      </c>
+      <c r="C48" s="0">
+        <v>0.29822103612286888</v>
+      </c>
+      <c r="D48" s="0">
+        <v>0</v>
+      </c>
+      <c r="E48" s="0">
+        <v>0</v>
+      </c>
+      <c r="F48" s="0">
+        <v>1.9295096694627798</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>0.20800089814799622</v>
+      </c>
+      <c r="B49" s="0">
+        <v>1</v>
+      </c>
+      <c r="C49" s="0">
+        <v>0</v>
+      </c>
+      <c r="D49" s="0">
+        <v>0.18198427273283097</v>
+      </c>
+      <c r="E49" s="0">
+        <v>0</v>
+      </c>
+      <c r="F49" s="0">
+        <v>1.9295096694627798</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>0</v>
+      </c>
+      <c r="B50" s="0">
+        <v>0</v>
+      </c>
+      <c r="C50" s="0">
+        <v>0</v>
+      </c>
+      <c r="D50" s="0">
+        <v>1</v>
+      </c>
+      <c r="E50" s="0">
+        <v>0</v>
+      </c>
+      <c r="F50" s="0">
+        <v>1.9295096694627798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix measurement path and initialization in MOPSO, add MOGWS algorithm
- Update all runner scripts to use correct 'measurements' folder path instead of 'measurement'
- Fix MOPSO initialization by properly assigning return value from Initialization function
- Add new MOGWS algorithm files (MOGWS.m and runMOGWS.m)
- Update Optimal.xlsx with latest results
</commit_message>
<xml_diff>
--- a/Optimal.xlsx
+++ b/Optimal.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="30" uniqueCount="7">
   <si>
     <t>X1</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Y2</t>
+  </si>
+  <si>
+    <t>Y3</t>
   </si>
 </sst>
 </file>
@@ -76,18 +79,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="true"/>
-    <col min="2" max="2" width="14.5546875" customWidth="true"/>
-    <col min="3" max="3" width="13.5546875" customWidth="true"/>
-    <col min="4" max="4" width="14.5546875" customWidth="true"/>
-    <col min="5" max="5" width="13.5546875" customWidth="true"/>
-    <col min="6" max="6" width="12.5546875" customWidth="true"/>
+    <col min="1" max="1" width="11.5546875" customWidth="true"/>
+    <col min="2" max="2" width="11.5546875" customWidth="true"/>
+    <col min="3" max="3" width="12.5546875" customWidth="true"/>
+    <col min="4" max="4" width="12.21875" customWidth="true"/>
+    <col min="5" max="5" width="11.5546875" customWidth="true"/>
+    <col min="6" max="6" width="12.21875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -101,993 +104,2013 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.29150969148882722</v>
+        <v>23.503633910445178</v>
       </c>
       <c r="B2" s="0">
-        <v>0.15021372056613569</v>
+        <v>119.86173633906553</v>
       </c>
       <c r="C2" s="0">
-        <v>0.055921997167276749</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="0">
-        <v>0.068352401695925935</v>
+        <v>-72644.320442153359</v>
       </c>
       <c r="E2" s="0">
-        <v>0.29150969148882722</v>
+        <v>1928.9268240705633</v>
       </c>
       <c r="F2" s="0">
-        <v>1.0943844363827335</v>
+        <v>-170504.10044751273</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.077189113646382146</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0">
-        <v>0.077189113646382146</v>
+        <v>140</v>
       </c>
       <c r="C3" s="0">
-        <v>0.077189113646382146</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="D3" s="0">
-        <v>0.077189113646382146</v>
+        <v>-93642.095000000001</v>
       </c>
       <c r="E3" s="0">
-        <v>0.29150969148882722</v>
+        <v>2269.9360000000001</v>
       </c>
       <c r="F3" s="0">
-        <v>1.0943844363827335</v>
+        <v>-258190.205399</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.84322393817237284</v>
+        <v>26</v>
       </c>
       <c r="B4" s="0">
-        <v>0.84322393817237284</v>
+        <v>140</v>
       </c>
       <c r="C4" s="0">
-        <v>0.84322393817237284</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="D4" s="0">
-        <v>0.84322393817237284</v>
+        <v>-93642.095000000001</v>
       </c>
       <c r="E4" s="0">
-        <v>0.29150969148882722</v>
+        <v>2269.9360000000001</v>
       </c>
       <c r="F4" s="0">
-        <v>1.0943844363827335</v>
+        <v>-258190.205399</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0</v>
+        <v>25.999980170157144</v>
       </c>
       <c r="B5" s="0">
-        <v>0.23658895007515812</v>
+        <v>100.15824259477009</v>
       </c>
       <c r="C5" s="0">
-        <v>0</v>
+        <v>0.49891020237293587</v>
       </c>
       <c r="D5" s="0">
-        <v>0.073247606412435107</v>
+        <v>-67291.827038041665</v>
       </c>
       <c r="E5" s="0">
-        <v>0.077189113646382146</v>
+        <v>1712.5587099473578</v>
       </c>
       <c r="F5" s="0">
-        <v>1.3330218505159859</v>
+        <v>-132055.93137534091</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.89893981332804307</v>
+        <v>25.215035441292535</v>
       </c>
       <c r="B6" s="0">
-        <v>0.89893981332804307</v>
+        <v>109.93065366205062</v>
       </c>
       <c r="C6" s="0">
-        <v>0.89893981332804307</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="0">
-        <v>0.89893981332804307</v>
+        <v>-71539.074865915551</v>
       </c>
       <c r="E6" s="0">
-        <v>0</v>
+        <v>1830.2983521154706</v>
       </c>
       <c r="F6" s="0">
-        <v>1.9295096694627798</v>
+        <v>-154172.92920217643</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.71955589370827833</v>
+        <v>24.476255963325571</v>
       </c>
       <c r="B7" s="0">
-        <v>0.71955589370827833</v>
+        <v>126.0045303718743</v>
       </c>
       <c r="C7" s="0">
-        <v>0.71955589370827833</v>
+        <v>0.4847392472032469</v>
       </c>
       <c r="D7" s="0">
-        <v>0.71955589370827833</v>
+        <v>-79461.424584664215</v>
       </c>
       <c r="E7" s="0">
-        <v>0</v>
+        <v>2036.9855353397265</v>
       </c>
       <c r="F7" s="0">
-        <v>1.9295096694627798</v>
+        <v>-196497.11228706728</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>1</v>
+        <v>25.99996773756282</v>
       </c>
       <c r="B8" s="0">
-        <v>0.6807751271799658</v>
+        <v>139.99066609579342</v>
       </c>
       <c r="C8" s="0">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D8" s="0">
-        <v>0.84754181853670918</v>
+        <v>-93638.53540372428</v>
       </c>
       <c r="E8" s="0">
-        <v>0.077189113646382146</v>
+        <v>2266.2095157276008</v>
       </c>
       <c r="F8" s="0">
-        <v>1.3330218505159859</v>
+        <v>-258154.8610070048</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>1</v>
+        <v>25.999956568353113</v>
       </c>
       <c r="B9" s="0">
-        <v>0.93419071587248204</v>
+        <v>139.9410546151598</v>
       </c>
       <c r="C9" s="0">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D9" s="0">
-        <v>0</v>
+        <v>-93605.680358376922</v>
       </c>
       <c r="E9" s="0">
-        <v>0.29150969148882722</v>
+        <v>2265.5196589198936</v>
       </c>
       <c r="F9" s="0">
-        <v>1.0943844363827335</v>
+        <v>-257971.6471081374</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.13335881945498218</v>
+        <v>25.999832032398238</v>
       </c>
       <c r="B10" s="0">
-        <v>0.13335881945498218</v>
+        <v>139.99999843527786</v>
       </c>
       <c r="C10" s="0">
-        <v>0.13335881945498218</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="0">
-        <v>0.13335881945498218</v>
+        <v>-93644.221147790595</v>
       </c>
       <c r="E10" s="0">
-        <v>0</v>
+        <v>2266.3361099564941</v>
       </c>
       <c r="F10" s="0">
-        <v>1.9295096694627798</v>
+        <v>-258187.92408002037</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.20152531051941514</v>
+        <v>24.186710040060806</v>
       </c>
       <c r="B11" s="0">
-        <v>0.20152531051941514</v>
+        <v>139.99999999991675</v>
       </c>
       <c r="C11" s="0">
-        <v>0.20152531051941514</v>
+        <v>0.5</v>
       </c>
       <c r="D11" s="0">
-        <v>0.20152531051941514</v>
+        <v>-87137.126795622622</v>
       </c>
       <c r="E11" s="0">
-        <v>0</v>
+        <v>2224.5799322214434</v>
       </c>
       <c r="F11" s="0">
-        <v>1.9295096694627798</v>
+        <v>-239659.01232102094</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.82407977286481915</v>
+        <v>24.737846250937324</v>
       </c>
       <c r="B12" s="0">
-        <v>0.82407977286481915</v>
+        <v>122.24094179280534</v>
       </c>
       <c r="C12" s="0">
-        <v>0.82407977286481915</v>
+        <v>0.49609365302965164</v>
       </c>
       <c r="D12" s="0">
-        <v>0.82407977286481915</v>
+        <v>-77938.718247958561</v>
       </c>
       <c r="E12" s="0">
-        <v>0</v>
+        <v>1990.4919261976079</v>
       </c>
       <c r="F12" s="0">
-        <v>1.9295096694627798</v>
+        <v>-186960.85022738617</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>1</v>
+        <v>24.636845843702737</v>
       </c>
       <c r="B13" s="0">
-        <v>1</v>
+        <v>126.11957009981451</v>
       </c>
       <c r="C13" s="0">
-        <v>1</v>
+        <v>0.49779954163703583</v>
       </c>
       <c r="D13" s="0">
-        <v>1</v>
+        <v>-80052.867546223977</v>
       </c>
       <c r="E13" s="0">
-        <v>0.077189113646382146</v>
+        <v>2042.048148409262</v>
       </c>
       <c r="F13" s="0">
-        <v>1.3330218505159859</v>
+        <v>-198187.98372569526</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>1</v>
+        <v>24.635112822572228</v>
       </c>
       <c r="B14" s="0">
-        <v>1</v>
+        <v>126.11808920055184</v>
       </c>
       <c r="C14" s="0">
-        <v>1</v>
+        <v>0.49773604870144222</v>
       </c>
       <c r="D14" s="0">
-        <v>1</v>
+        <v>-80046.330913389393</v>
       </c>
       <c r="E14" s="0">
-        <v>0</v>
+        <v>2041.9887940358572</v>
       </c>
       <c r="F14" s="0">
-        <v>1.9295096694627798</v>
+        <v>-198168.9554369968</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.30189286053120012</v>
+        <v>25.207848894695875</v>
       </c>
       <c r="B15" s="0">
-        <v>0.94109380406463461</v>
+        <v>109.98278330432498</v>
       </c>
       <c r="C15" s="0">
-        <v>0.8965035496044933</v>
+        <v>0.5</v>
       </c>
       <c r="D15" s="0">
-        <v>0.33792901932329156</v>
+        <v>-71552.210688497405</v>
       </c>
       <c r="E15" s="0">
-        <v>0</v>
+        <v>1830.8574479749632</v>
       </c>
       <c r="F15" s="0">
-        <v>1.9295096694627798</v>
+        <v>-154274.03919795723</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>1</v>
+        <v>25.221617513215858</v>
       </c>
       <c r="B16" s="0">
-        <v>0.93124453542360486</v>
+        <v>109.98278315116404</v>
       </c>
       <c r="C16" s="0">
-        <v>0.61945306940279166</v>
+        <v>0.5</v>
       </c>
       <c r="D16" s="0">
-        <v>0.78227178659946506</v>
+        <v>-71591.11040733433</v>
       </c>
       <c r="E16" s="0">
-        <v>0</v>
+        <v>1831.1745371305415</v>
       </c>
       <c r="F16" s="0">
-        <v>1.9295096694627798</v>
+        <v>-154360.83845494653</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>1</v>
+        <v>24.233471524036883</v>
       </c>
       <c r="B17" s="0">
-        <v>1</v>
+        <v>139.89728201152161</v>
       </c>
       <c r="C17" s="0">
-        <v>1</v>
+        <v>0.46277224429232955</v>
       </c>
       <c r="D17" s="0">
-        <v>0.98636367948592119</v>
+        <v>-87241.114868897916</v>
       </c>
       <c r="E17" s="0">
-        <v>0</v>
+        <v>2224.8984242063439</v>
       </c>
       <c r="F17" s="0">
-        <v>1.9295096694627798</v>
+        <v>-239784.43153802038</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.55185278833681684</v>
+        <v>24.243492047898204</v>
       </c>
       <c r="B18" s="0">
-        <v>0.4667311079084242</v>
+        <v>139.99963893364816</v>
       </c>
       <c r="C18" s="0">
-        <v>0.29582532268418543</v>
+        <v>0.48442148171524357</v>
       </c>
       <c r="D18" s="0">
-        <v>0</v>
+        <v>-87340.475839731997</v>
       </c>
       <c r="E18" s="0">
-        <v>0.62589639308841771</v>
+        <v>2226.1627047995653</v>
       </c>
       <c r="F18" s="0">
-        <v>0.65426847911508668</v>
+        <v>-240238.08812697517</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0</v>
+        <v>24.233573832413228</v>
       </c>
       <c r="B19" s="0">
-        <v>1</v>
+        <v>139.99984964249674</v>
       </c>
       <c r="C19" s="0">
-        <v>0</v>
+        <v>0.48784636926144842</v>
       </c>
       <c r="D19" s="0">
-        <v>0.36100432451725162</v>
+        <v>-87305.057198630675</v>
       </c>
       <c r="E19" s="0">
-        <v>0</v>
+        <v>2225.8756376718607</v>
       </c>
       <c r="F19" s="0">
-        <v>1.9295096694627798</v>
+        <v>-240137.44540266096</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0</v>
+        <v>24.233394436398182</v>
       </c>
       <c r="B20" s="0">
-        <v>0</v>
+        <v>139.84403067240376</v>
       </c>
       <c r="C20" s="0">
-        <v>0</v>
+        <v>0.46577160842373727</v>
       </c>
       <c r="D20" s="0">
-        <v>0</v>
+        <v>-87208.050032265906</v>
       </c>
       <c r="E20" s="0">
-        <v>0</v>
+        <v>2224.1025266972038</v>
       </c>
       <c r="F20" s="0">
-        <v>1.9295096694627798</v>
+        <v>-239600.96924798458</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.99179998526696</v>
+        <v>24.723485726408992</v>
       </c>
       <c r="B21" s="0">
-        <v>0.64903151508563017</v>
+        <v>122.2444814546519</v>
       </c>
       <c r="C21" s="0">
-        <v>1</v>
+        <v>0.49891034410267648</v>
       </c>
       <c r="D21" s="0">
-        <v>0.7583541282064753</v>
+        <v>-77895.932625725181</v>
       </c>
       <c r="E21" s="0">
-        <v>0</v>
+        <v>1990.1597605118943</v>
       </c>
       <c r="F21" s="0">
-        <v>1.9295096694627798</v>
+        <v>-186859.81555496884</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0</v>
+        <v>24.728931627359248</v>
       </c>
       <c r="B22" s="0">
-        <v>0.9707716350527823</v>
+        <v>122.24466899336817</v>
       </c>
       <c r="C22" s="0">
-        <v>0</v>
+        <v>0.49999271605439022</v>
       </c>
       <c r="D22" s="0">
-        <v>0.88388994263013598</v>
+        <v>-77913.1502053312</v>
       </c>
       <c r="E22" s="0">
-        <v>0</v>
+        <v>1990.2683253512432</v>
       </c>
       <c r="F22" s="0">
-        <v>1.9295096694627798</v>
+        <v>-186902.80906410687</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.66728677516521773</v>
+        <v>24.727852451260183</v>
       </c>
       <c r="B23" s="0">
-        <v>0.68026336522163799</v>
+        <v>122.35026117672091</v>
       </c>
       <c r="C23" s="0">
-        <v>0</v>
+        <v>0.49993052751939276</v>
       </c>
       <c r="D23" s="0">
-        <v>0</v>
+        <v>-77976.189339403558</v>
       </c>
       <c r="E23" s="0">
-        <v>0</v>
+        <v>1991.712321424144</v>
       </c>
       <c r="F23" s="0">
-        <v>1.9295096694627798</v>
+        <v>-187217.73215312045</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.88994481199442155</v>
+        <v>24.72890615226035</v>
       </c>
       <c r="B24" s="0">
-        <v>0.90682858633178776</v>
+        <v>122.24742065116168</v>
       </c>
       <c r="C24" s="0">
-        <v>0.50865495247334269</v>
+        <v>0.49998368769329687</v>
       </c>
       <c r="D24" s="0">
-        <v>0.29257977307463567</v>
+        <v>-77914.801238954897</v>
       </c>
       <c r="E24" s="0">
-        <v>0</v>
+        <v>1990.3061490329778</v>
       </c>
       <c r="F24" s="0">
-        <v>1.9295096694627798</v>
+        <v>-186911.03320471465</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>1</v>
+        <v>24.728933381108028</v>
       </c>
       <c r="B25" s="0">
-        <v>0.78820031079388286</v>
+        <v>122.24448156685143</v>
       </c>
       <c r="C25" s="0">
-        <v>1</v>
+        <v>0.4999974537122418</v>
       </c>
       <c r="D25" s="0">
-        <v>1</v>
+        <v>-77913.037861067438</v>
       </c>
       <c r="E25" s="0">
-        <v>0</v>
+        <v>1990.2656753284068</v>
       </c>
       <c r="F25" s="0">
-        <v>1.9295096694627798</v>
+        <v>-186902.24902424208</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0</v>
+        <v>25.694940041256441</v>
       </c>
       <c r="B26" s="0">
-        <v>0</v>
+        <v>100.01419825226098</v>
       </c>
       <c r="C26" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D26" s="0">
-        <v>0</v>
+        <v>-66412.108481921532</v>
       </c>
       <c r="E26" s="0">
-        <v>0</v>
+        <v>1703.5118248565636</v>
       </c>
       <c r="F26" s="0">
-        <v>1.9295096694627798</v>
+        <v>-130086.00254883181</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>0.55616370047907149</v>
+        <v>25.695059224837454</v>
       </c>
       <c r="B27" s="0">
-        <v>0.84436781473935107</v>
+        <v>100.12809135297761</v>
       </c>
       <c r="C27" s="0">
-        <v>0.69366182334053672</v>
+        <v>0.33337349348275314</v>
       </c>
       <c r="D27" s="0">
-        <v>0.7969283804409355</v>
+        <v>-66484.590433498481</v>
       </c>
       <c r="E27" s="0">
-        <v>0</v>
+        <v>1708.0936283415754</v>
       </c>
       <c r="F27" s="0">
-        <v>1.9295096694627798</v>
+        <v>-130383.89202622641</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>1</v>
+        <v>25.695219533762163</v>
       </c>
       <c r="B28" s="0">
-        <v>1</v>
+        <v>100.01394851723779</v>
       </c>
       <c r="C28" s="0">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D28" s="0">
-        <v>0.26765306442105102</v>
+        <v>-66412.663990775749</v>
       </c>
       <c r="E28" s="0">
-        <v>0</v>
+        <v>1703.514790252148</v>
       </c>
       <c r="F28" s="0">
-        <v>1.9295096694627798</v>
+        <v>-130086.80884793536</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>1</v>
+        <v>24.579306293403857</v>
       </c>
       <c r="B29" s="0">
-        <v>1</v>
+        <v>136.40590491643599</v>
       </c>
       <c r="C29" s="0">
-        <v>0</v>
+        <v>0.49265709172725447</v>
       </c>
       <c r="D29" s="0">
-        <v>0</v>
+        <v>-86298.632474853948</v>
       </c>
       <c r="E29" s="0">
-        <v>0</v>
+        <v>2183.795527766295</v>
       </c>
       <c r="F29" s="0">
-        <v>1.9295096694627798</v>
+        <v>-231310.11383570003</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>1</v>
+        <v>24.60850064663331</v>
       </c>
       <c r="B30" s="0">
-        <v>0.27966283451250251</v>
+        <v>136.23360153508216</v>
       </c>
       <c r="C30" s="0">
-        <v>0</v>
+        <v>0.41020893557474247</v>
       </c>
       <c r="D30" s="0">
-        <v>0.050059440791189611</v>
+        <v>-86291.744176795051</v>
       </c>
       <c r="E30" s="0">
-        <v>0</v>
+        <v>2183.5552745679734</v>
       </c>
       <c r="F30" s="0">
-        <v>1.9295096694627798</v>
+        <v>-231008.3188969382</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0</v>
+        <v>24.582888934977557</v>
       </c>
       <c r="B31" s="0">
-        <v>0</v>
+        <v>136.49798664469765</v>
       </c>
       <c r="C31" s="0">
-        <v>0</v>
+        <v>0.49749303235876968</v>
       </c>
       <c r="D31" s="0">
-        <v>0</v>
+        <v>-86368.815489328801</v>
       </c>
       <c r="E31" s="0">
-        <v>0</v>
+        <v>2185.0710218120198</v>
       </c>
       <c r="F31" s="0">
-        <v>1.9295096694627798</v>
+        <v>-231657.57931472606</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.37383848887580456</v>
+        <v>24.601212278254078</v>
       </c>
       <c r="B32" s="0">
-        <v>0.43956474371474069</v>
+        <v>136.41737271296327</v>
       </c>
       <c r="C32" s="0">
-        <v>0.26435198278410665</v>
+        <v>0.49276475767192279</v>
       </c>
       <c r="D32" s="0">
-        <v>0</v>
+        <v>-86382.426343452113</v>
       </c>
       <c r="E32" s="0">
-        <v>0</v>
+        <v>2184.45748913544</v>
       </c>
       <c r="F32" s="0">
-        <v>1.9295096694627798</v>
+        <v>-231561.58763478536</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.44991443863782377</v>
+        <v>24.579481802690289</v>
       </c>
       <c r="B33" s="0">
-        <v>0.48255259095290598</v>
+        <v>136.49798658188055</v>
       </c>
       <c r="C33" s="0">
-        <v>0.41273234313763635</v>
+        <v>0.49999592201205201</v>
       </c>
       <c r="D33" s="0">
-        <v>0.19030396392451202</v>
+        <v>-86356.925337069813</v>
       </c>
       <c r="E33" s="0">
-        <v>0</v>
+        <v>2184.9475527263203</v>
       </c>
       <c r="F33" s="0">
-        <v>1.9295096694627798</v>
+        <v>-231624.47522783405</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.60337240665257497</v>
+        <v>25.994530605726482</v>
       </c>
       <c r="B34" s="0">
-        <v>0.79043307979119626</v>
+        <v>100.30469889742342</v>
       </c>
       <c r="C34" s="0">
-        <v>0.64718160604492214</v>
+        <v>0.49910169128620496</v>
       </c>
       <c r="D34" s="0">
-        <v>0.025490857145197655</v>
+        <v>-67374.646981768034</v>
       </c>
       <c r="E34" s="0">
-        <v>0</v>
+        <v>1714.4655061147407</v>
       </c>
       <c r="F34" s="0">
-        <v>1.9295096694627798</v>
+        <v>-132414.3108492014</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>0.076211500955900124</v>
+        <v>25.978064501392584</v>
       </c>
       <c r="B35" s="0">
-        <v>0</v>
+        <v>100.14705562844978</v>
       </c>
       <c r="C35" s="0">
-        <v>0.053942058463242806</v>
+        <v>0.49916226409750736</v>
       </c>
       <c r="D35" s="0">
-        <v>0</v>
+        <v>-67227.997448784212</v>
       </c>
       <c r="E35" s="0">
-        <v>0</v>
+        <v>1711.8939611940498</v>
       </c>
       <c r="F35" s="0">
-        <v>1.9295096694627798</v>
+        <v>-131911.86628422557</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.5497932757823405</v>
+        <v>25.993578391266716</v>
       </c>
       <c r="B36" s="0">
-        <v>0.63210698787651698</v>
+        <v>100.4030211607184</v>
       </c>
       <c r="C36" s="0">
-        <v>0.77682075784954119</v>
+        <v>0.49980059204840921</v>
       </c>
       <c r="D36" s="0">
-        <v>0.44182461108858473</v>
+        <v>-67437.218936462639</v>
       </c>
       <c r="E36" s="0">
-        <v>0</v>
+        <v>1715.7976898398279</v>
       </c>
       <c r="F36" s="0">
-        <v>1.9295096694627798</v>
+        <v>-132669.34379900459</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.36202218259607749</v>
+        <v>25.992807881840015</v>
       </c>
       <c r="B37" s="0">
-        <v>0.72556999344065309</v>
+        <v>100.40176846565717</v>
       </c>
       <c r="C37" s="0">
-        <v>0.065100509595460571</v>
+        <v>0.49969115575311296</v>
       </c>
       <c r="D37" s="0">
-        <v>0.62247871914728981</v>
+        <v>-67434.399986130622</v>
       </c>
       <c r="E37" s="0">
-        <v>0</v>
+        <v>1715.7645002109693</v>
       </c>
       <c r="F37" s="0">
-        <v>1.9295096694627798</v>
+        <v>-132661.98238107836</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>0.86616963721181561</v>
+        <v>25.99358137210012</v>
       </c>
       <c r="B38" s="0">
-        <v>0</v>
+        <v>100.40317827258617</v>
       </c>
       <c r="C38" s="0">
-        <v>1</v>
+        <v>0.49983723794568502</v>
       </c>
       <c r="D38" s="0">
-        <v>0</v>
+        <v>-67437.331026247382</v>
       </c>
       <c r="E38" s="0">
-        <v>0</v>
+        <v>1715.7992834501501</v>
       </c>
       <c r="F38" s="0">
-        <v>1.9295096694627798</v>
+        <v>-132669.77506136795</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0.27118206175103515</v>
+        <v>25.993594674229438</v>
       </c>
       <c r="B39" s="0">
-        <v>0.33793538575048293</v>
+        <v>100.40273182872063</v>
       </c>
       <c r="C39" s="0">
-        <v>0.27159601348696827</v>
+        <v>0.49982296508894447</v>
       </c>
       <c r="D39" s="0">
-        <v>0.31273979788675244</v>
+        <v>-67437.06994841127</v>
       </c>
       <c r="E39" s="0">
-        <v>0</v>
+        <v>1715.7936408544217</v>
       </c>
       <c r="F39" s="0">
-        <v>1.9295096694627798</v>
+        <v>-132668.66371294187</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>0.3726830944684788</v>
+        <v>25.993603664937506</v>
       </c>
       <c r="B40" s="0">
-        <v>0</v>
+        <v>100.40354684767328</v>
       </c>
       <c r="C40" s="0">
-        <v>0.31784621087819043</v>
+        <v>0.49983723794568502</v>
       </c>
       <c r="D40" s="0">
-        <v>0</v>
+        <v>-67437.632306581683</v>
       </c>
       <c r="E40" s="0">
-        <v>0</v>
+        <v>1715.8049200479063</v>
       </c>
       <c r="F40" s="0">
-        <v>1.9295096694627798</v>
+        <v>-132670.86739090137</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>1</v>
+        <v>25.993601850003284</v>
       </c>
       <c r="B41" s="0">
-        <v>1</v>
+        <v>100.40330838710769</v>
       </c>
       <c r="C41" s="0">
-        <v>1</v>
+        <v>0.49983638928189927</v>
       </c>
       <c r="D41" s="0">
-        <v>1</v>
+        <v>-67437.469921100143</v>
       </c>
       <c r="E41" s="0">
-        <v>0</v>
+        <v>1715.8015789070839</v>
       </c>
       <c r="F41" s="0">
-        <v>1.9295096694627798</v>
+        <v>-132670.22690529202</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0.39331566717778699</v>
+        <v>25.993616767257596</v>
       </c>
       <c r="B42" s="0">
-        <v>0.8023440427901507</v>
+        <v>100.40354684767119</v>
       </c>
       <c r="C42" s="0">
-        <v>0</v>
+        <v>0.49969097691714992</v>
       </c>
       <c r="D42" s="0">
-        <v>0.074096107482310269</v>
+        <v>-67437.664134493345</v>
       </c>
       <c r="E42" s="0">
-        <v>0</v>
+        <v>1715.8078515676018</v>
       </c>
       <c r="F42" s="0">
-        <v>1.9295096694627798</v>
+        <v>-132670.93662809281</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>0.25210430483922869</v>
+        <v>24.490026832697335</v>
       </c>
       <c r="B43" s="0">
-        <v>1</v>
+        <v>126.05239196412442</v>
       </c>
       <c r="C43" s="0">
-        <v>1</v>
+        <v>0.49995746219383258</v>
       </c>
       <c r="D43" s="0">
-        <v>1</v>
+        <v>-79535.970432872418</v>
       </c>
       <c r="E43" s="0">
-        <v>0</v>
+        <v>2037.694331088104</v>
       </c>
       <c r="F43" s="0">
-        <v>1.9295096694627798</v>
+        <v>-196760.58384421104</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>1</v>
+        <v>24.487798915820502</v>
       </c>
       <c r="B44" s="0">
-        <v>1</v>
+        <v>126.03568657269392</v>
       </c>
       <c r="C44" s="0">
-        <v>1</v>
+        <v>0.49995399467527657</v>
       </c>
       <c r="D44" s="0">
-        <v>0.0054421490853886695</v>
+        <v>-79518.358211241924</v>
       </c>
       <c r="E44" s="0">
-        <v>0</v>
+        <v>2037.4108795675302</v>
       </c>
       <c r="F44" s="0">
-        <v>1.9295096694627798</v>
+        <v>-196689.93580606443</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>0</v>
+        <v>24.635110122309499</v>
       </c>
       <c r="B45" s="0">
-        <v>0.0026598599078565544</v>
+        <v>126.11810200013151</v>
       </c>
       <c r="C45" s="0">
-        <v>0.18152555110511048</v>
+        <v>0.49774967733705539</v>
       </c>
       <c r="D45" s="0">
-        <v>0.53969925371476823</v>
+        <v>-80046.330383804569</v>
       </c>
       <c r="E45" s="0">
-        <v>0</v>
+        <v>2041.9886647200956</v>
       </c>
       <c r="F45" s="0">
-        <v>1.9295096694627798</v>
+        <v>-198168.97327293019</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>0.99597898046122069</v>
+        <v>24.629977178534578</v>
       </c>
       <c r="B46" s="0">
-        <v>0.79045788144483853</v>
+        <v>126.11811895020004</v>
       </c>
       <c r="C46" s="0">
-        <v>0.085727546061760473</v>
+        <v>0.497736126386634</v>
       </c>
       <c r="D46" s="0">
-        <v>0.57643881595177038</v>
+        <v>-80029.731976184761</v>
       </c>
       <c r="E46" s="0">
-        <v>0</v>
+        <v>2041.8709322770003</v>
       </c>
       <c r="F46" s="0">
-        <v>1.9295096694627798</v>
+        <v>-198126.4655429429</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>0.72541144070463148</v>
+        <v>24.635112822411642</v>
       </c>
       <c r="B47" s="0">
-        <v>0.70577426394726284</v>
+        <v>126.11808920061023</v>
       </c>
       <c r="C47" s="0">
-        <v>0.44395219730245172</v>
+        <v>0.49777184502965388</v>
       </c>
       <c r="D47" s="0">
-        <v>0.29142558632006482</v>
+        <v>-80046.331401526244</v>
       </c>
       <c r="E47" s="0">
-        <v>0</v>
+        <v>2041.9881504149891</v>
       </c>
       <c r="F47" s="0">
-        <v>1.9295096694627798</v>
+        <v>-198168.9553397464</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0.74076059672179462</v>
+        <v>25.987852089076881</v>
       </c>
       <c r="B48" s="0">
-        <v>0.68414918268037028</v>
+        <v>100.1430373766635</v>
       </c>
       <c r="C48" s="0">
-        <v>0.29822103612286888</v>
+        <v>0.49941987503950597</v>
       </c>
       <c r="D48" s="0">
-        <v>0</v>
+        <v>-67250.547717157999</v>
       </c>
       <c r="E48" s="0">
-        <v>0</v>
+        <v>1712.0588837938531</v>
       </c>
       <c r="F48" s="0">
-        <v>1.9295096694627798</v>
+        <v>-131952.41298954652</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0.20800089814799622</v>
+        <v>25.983250366214705</v>
       </c>
       <c r="B49" s="0">
-        <v>1</v>
+        <v>100.17980272200197</v>
       </c>
       <c r="C49" s="0">
-        <v>0</v>
+        <v>0.49890889240302139</v>
       </c>
       <c r="D49" s="0">
-        <v>0.18198427273283097</v>
+        <v>-67262.994037105731</v>
       </c>
       <c r="E49" s="0">
-        <v>0</v>
+        <v>1712.4731318843458</v>
       </c>
       <c r="F49" s="0">
-        <v>1.9295096694627798</v>
+        <v>-132025.37257573107</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>0</v>
+        <v>25.984691860246738</v>
       </c>
       <c r="B50" s="0">
-        <v>0</v>
+        <v>100.19287466913889</v>
       </c>
       <c r="C50" s="0">
-        <v>0</v>
+        <v>0.49881114885696226</v>
       </c>
       <c r="D50" s="0">
-        <v>1</v>
+        <v>-67275.347013738152</v>
       </c>
       <c r="E50" s="0">
-        <v>0</v>
+        <v>1712.6897869860647</v>
       </c>
       <c r="F50" s="0">
-        <v>1.9295096694627798</v>
+        <v>-132067.41166166583</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>25.989193062023944</v>
+      </c>
+      <c r="B51" s="0">
+        <v>100.17542320355184</v>
+      </c>
+      <c r="C51" s="0">
+        <v>0.49845312408693959</v>
+      </c>
+      <c r="D51" s="0">
+        <v>-67275.399808514077</v>
+      </c>
+      <c r="E51" s="0">
+        <v>1712.557311576699</v>
+      </c>
+      <c r="F51" s="0">
+        <v>-132044.89072354804</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>25.989611710353799</v>
+      </c>
+      <c r="B52" s="0">
+        <v>100.14281092340165</v>
+      </c>
+      <c r="C52" s="0">
+        <v>0.49892940710700751</v>
+      </c>
+      <c r="D52" s="0">
+        <v>-67254.922196499567</v>
+      </c>
+      <c r="E52" s="0">
+        <v>1712.105078784947</v>
+      </c>
+      <c r="F52" s="0">
+        <v>-131961.01184476897</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>25.970687880467295</v>
+      </c>
+      <c r="B53" s="0">
+        <v>100.14281109888539</v>
+      </c>
+      <c r="C53" s="0">
+        <v>0.49893693687600649</v>
+      </c>
+      <c r="D53" s="0">
+        <v>-67206.195008319584</v>
+      </c>
+      <c r="E53" s="0">
+        <v>1711.6691300366383</v>
+      </c>
+      <c r="F53" s="0">
+        <v>-131862.12516359915</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>25.989698744394708</v>
+      </c>
+      <c r="B54" s="0">
+        <v>100.2214533361803</v>
+      </c>
+      <c r="C54" s="0">
+        <v>0.49873748750026348</v>
+      </c>
+      <c r="D54" s="0">
+        <v>-67307.140310927774</v>
+      </c>
+      <c r="E54" s="0">
+        <v>1713.2036634310618</v>
+      </c>
+      <c r="F54" s="0">
+        <v>-132169.059760879</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>25.98969913278172</v>
+      </c>
+      <c r="B55" s="0">
+        <v>100.24398619192473</v>
+      </c>
+      <c r="C55" s="0">
+        <v>0.49902115360546762</v>
+      </c>
+      <c r="D55" s="0">
+        <v>-67322.043411091043</v>
+      </c>
+      <c r="E55" s="0">
+        <v>1713.5117787538904</v>
+      </c>
+      <c r="F55" s="0">
+        <v>-132228.57109881076</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>25.989419212691942</v>
+      </c>
+      <c r="B56" s="0">
+        <v>100.14294607680752</v>
+      </c>
+      <c r="C56" s="0">
+        <v>0.49902025129928684</v>
+      </c>
+      <c r="D56" s="0">
+        <v>-67254.517129333501</v>
+      </c>
+      <c r="E56" s="0">
+        <v>1712.100890817559</v>
+      </c>
+      <c r="F56" s="0">
+        <v>-131960.36230594668</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>25.989699135486454</v>
+      </c>
+      <c r="B57" s="0">
+        <v>100.14350609028087</v>
+      </c>
+      <c r="C57" s="0">
+        <v>0.49893197429535413</v>
+      </c>
+      <c r="D57" s="0">
+        <v>-67255.606973545466</v>
+      </c>
+      <c r="E57" s="0">
+        <v>1712.1167088473267</v>
+      </c>
+      <c r="F57" s="0">
+        <v>-131963.30299963412</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0">
+        <v>25.9889988526952</v>
+      </c>
+      <c r="B58" s="0">
+        <v>100.14281081184765</v>
+      </c>
+      <c r="C58" s="0">
+        <v>0.49892993414461151</v>
+      </c>
+      <c r="D58" s="0">
+        <v>-67253.344068590362</v>
+      </c>
+      <c r="E58" s="0">
+        <v>1712.0909536463328</v>
+      </c>
+      <c r="F58" s="0">
+        <v>-131957.8090402043</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0">
+        <v>22.13770774449247</v>
+      </c>
+      <c r="B59" s="0">
+        <v>100.00000130980764</v>
+      </c>
+      <c r="C59" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D59" s="0">
+        <v>-57256.152283997813</v>
+      </c>
+      <c r="E59" s="0">
+        <v>1621.3914275619879</v>
+      </c>
+      <c r="F59" s="0">
+        <v>-111513.62819203545</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0">
+        <v>22.105789939758711</v>
+      </c>
+      <c r="B60" s="0">
+        <v>100.00034022492359</v>
+      </c>
+      <c r="C60" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D60" s="0">
+        <v>-57174.272946933415</v>
+      </c>
+      <c r="E60" s="0">
+        <v>1620.6610714390811</v>
+      </c>
+      <c r="F60" s="0">
+        <v>-111348.07218196601</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0">
+        <v>22.117836587050856</v>
+      </c>
+      <c r="B61" s="0">
+        <v>100.00091211861616</v>
+      </c>
+      <c r="C61" s="0">
+        <v>0.4811458876712813</v>
+      </c>
+      <c r="D61" s="0">
+        <v>-57205.31290814704</v>
+      </c>
+      <c r="E61" s="0">
+        <v>1621.285451988216</v>
+      </c>
+      <c r="F61" s="0">
+        <v>-111412.16472985045</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0">
+        <v>22.038705244659095</v>
+      </c>
+      <c r="B62" s="0">
+        <v>100.00002206542131</v>
+      </c>
+      <c r="C62" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D62" s="0">
+        <v>-57001.599779841454</v>
+      </c>
+      <c r="E62" s="0">
+        <v>1619.1116884938551</v>
+      </c>
+      <c r="F62" s="0">
+        <v>-110997.80950023182</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0">
+        <v>22.000022956889616</v>
+      </c>
+      <c r="B63" s="0">
+        <v>100.00107563041888</v>
+      </c>
+      <c r="C63" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D63" s="0">
+        <v>-56902.72603828174</v>
+      </c>
+      <c r="E63" s="0">
+        <v>1618.2354799599905</v>
+      </c>
+      <c r="F63" s="0">
+        <v>-110798.58806048136</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0">
+        <v>22.018575875402306</v>
+      </c>
+      <c r="B64" s="0">
+        <v>100.00000009345632</v>
+      </c>
+      <c r="C64" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D64" s="0">
+        <v>-56949.829015013005</v>
+      </c>
+      <c r="E64" s="0">
+        <v>1618.647803709558</v>
+      </c>
+      <c r="F64" s="0">
+        <v>-110892.87408657809</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0">
+        <v>22.000239272706747</v>
+      </c>
+      <c r="B65" s="0">
+        <v>100.00038773544443</v>
+      </c>
+      <c r="C65" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D65" s="0">
+        <v>-56902.897249651855</v>
+      </c>
+      <c r="E65" s="0">
+        <v>1618.230899973114</v>
+      </c>
+      <c r="F65" s="0">
+        <v>-110798.18899677182</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0">
+        <v>22.01016505878248</v>
+      </c>
+      <c r="B66" s="0">
+        <v>100.00000000000254</v>
+      </c>
+      <c r="C66" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D66" s="0">
+        <v>-56928.202313998227</v>
+      </c>
+      <c r="E66" s="0">
+        <v>1618.4541013037961</v>
+      </c>
+      <c r="F66" s="0">
+        <v>-110849.04827527556</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0">
+        <v>24.490530511472393</v>
+      </c>
+      <c r="B67" s="0">
+        <v>125.94134567473044</v>
+      </c>
+      <c r="C67" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D67" s="0">
+        <v>-79468.413762547294</v>
+      </c>
+      <c r="E67" s="0">
+        <v>2036.1616225579623</v>
+      </c>
+      <c r="F67" s="0">
+        <v>-196417.89505988927</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0">
+        <v>24.476335251120368</v>
+      </c>
+      <c r="B68" s="0">
+        <v>125.9291672534882</v>
+      </c>
+      <c r="C68" s="0">
+        <v>0.47887972647746396</v>
+      </c>
+      <c r="D68" s="0">
+        <v>-79414.673973899087</v>
+      </c>
+      <c r="E68" s="0">
+        <v>2036.0451681747234</v>
+      </c>
+      <c r="F68" s="0">
+        <v>-196262.57904355676</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0">
+        <v>24.492293086119183</v>
+      </c>
+      <c r="B69" s="0">
+        <v>125.99973538556603</v>
+      </c>
+      <c r="C69" s="0">
+        <v>0.49095234451052144</v>
+      </c>
+      <c r="D69" s="0">
+        <v>-79510.367250789568</v>
+      </c>
+      <c r="E69" s="0">
+        <v>2037.1765084783935</v>
+      </c>
+      <c r="F69" s="0">
+        <v>-196614.85270604884</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0">
+        <v>24.522505081753227</v>
+      </c>
+      <c r="B70" s="0">
+        <v>126.04304056761703</v>
+      </c>
+      <c r="C70" s="0">
+        <v>0.49943343039304211</v>
+      </c>
+      <c r="D70" s="0">
+        <v>-79635.166086230514</v>
+      </c>
+      <c r="E70" s="0">
+        <v>2038.3217428441867</v>
+      </c>
+      <c r="F70" s="0">
+        <v>-197000.34502150188</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0">
+        <v>24.534974982673003</v>
+      </c>
+      <c r="B71" s="0">
+        <v>126.04307989342185</v>
+      </c>
+      <c r="C71" s="0">
+        <v>0.499943461255208</v>
+      </c>
+      <c r="D71" s="0">
+        <v>-79675.523070873911</v>
+      </c>
+      <c r="E71" s="0">
+        <v>2038.6003009361543</v>
+      </c>
+      <c r="F71" s="0">
+        <v>-197103.74088587437</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0">
+        <v>24.527352359731506</v>
+      </c>
+      <c r="B72" s="0">
+        <v>126.04308862311977</v>
+      </c>
+      <c r="C72" s="0">
+        <v>0.49533024250316371</v>
+      </c>
+      <c r="D72" s="0">
+        <v>-79650.815311664323</v>
+      </c>
+      <c r="E72" s="0">
+        <v>2038.5078189457745</v>
+      </c>
+      <c r="F72" s="0">
+        <v>-197040.65091718835</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="0">
+        <v>24.535379716770226</v>
+      </c>
+      <c r="B73" s="0">
+        <v>125.9829438607413</v>
+      </c>
+      <c r="C73" s="0">
+        <v>0.49936983007510977</v>
+      </c>
+      <c r="D73" s="0">
+        <v>-79639.288367949368</v>
+      </c>
+      <c r="E73" s="0">
+        <v>2037.7840449967719</v>
+      </c>
+      <c r="F73" s="0">
+        <v>-196918.87661426121</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="0">
+        <v>25.962282175168347</v>
+      </c>
+      <c r="B74" s="0">
+        <v>139.92724356070332</v>
+      </c>
+      <c r="C74" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D74" s="0">
+        <v>-93461.405669251792</v>
+      </c>
+      <c r="E74" s="0">
+        <v>2264.4600439879032</v>
+      </c>
+      <c r="F74" s="0">
+        <v>-257536.07936744922</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="0">
+        <v>25.99997430970501</v>
+      </c>
+      <c r="B75" s="0">
+        <v>139.99572210238904</v>
+      </c>
+      <c r="C75" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D75" s="0">
+        <v>-93641.903230557306</v>
+      </c>
+      <c r="E75" s="0">
+        <v>2266.2799455757145</v>
+      </c>
+      <c r="F75" s="0">
+        <v>-258173.59189031084</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="0">
+        <v>25.999999762613285</v>
+      </c>
+      <c r="B76" s="0">
+        <v>139.99999902456028</v>
+      </c>
+      <c r="C76" s="0">
+        <v>0.42623823501991642</v>
+      </c>
+      <c r="D76" s="0">
+        <v>-93643.816654758382</v>
+      </c>
+      <c r="E76" s="0">
+        <v>2267.666217508714</v>
+      </c>
+      <c r="F76" s="0">
+        <v>-258189.84794486852</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="0">
+        <v>25.999999999298375</v>
+      </c>
+      <c r="B77" s="0">
+        <v>139.9999999634727</v>
+      </c>
+      <c r="C77" s="0">
+        <v>0.31724978858842579</v>
+      </c>
+      <c r="D77" s="0">
+        <v>-93642.33043293556</v>
+      </c>
+      <c r="E77" s="0">
+        <v>2269.6258482772923</v>
+      </c>
+      <c r="F77" s="0">
+        <v>-258190.15752375964</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="0">
+        <v>25.999996791855111</v>
+      </c>
+      <c r="B78" s="0">
+        <v>139.99999999174244</v>
+      </c>
+      <c r="C78" s="0">
+        <v>0.30503473334623221</v>
+      </c>
+      <c r="D78" s="0">
+        <v>-93642.152204969199</v>
+      </c>
+      <c r="E78" s="0">
+        <v>2269.845401496078</v>
+      </c>
+      <c r="F78" s="0">
+        <v>-258190.15866071821</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="0">
+        <v>25.999999371342099</v>
+      </c>
+      <c r="B79" s="0">
+        <v>139.98156127054992</v>
+      </c>
+      <c r="C79" s="0">
+        <v>0.4966271822521755</v>
+      </c>
+      <c r="D79" s="0">
+        <v>-93632.580591941121</v>
+      </c>
+      <c r="E79" s="0">
+        <v>2266.1443304457584</v>
+      </c>
+      <c r="F79" s="0">
+        <v>-258121.58590944222</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0">
+        <v>25.999999890109095</v>
+      </c>
+      <c r="B80" s="0">
+        <v>139.99994823542772</v>
+      </c>
+      <c r="C80" s="0">
+        <v>0.43894729928865589</v>
+      </c>
+      <c r="D80" s="0">
+        <v>-93643.956997090398</v>
+      </c>
+      <c r="E80" s="0">
+        <v>2267.4370055004479</v>
+      </c>
+      <c r="F80" s="0">
+        <v>-258189.62610561858</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="0">
+        <v>25.999997130356387</v>
+      </c>
+      <c r="B81" s="0">
+        <v>139.99998507282064</v>
+      </c>
+      <c r="C81" s="0">
+        <v>0.38399714555848585</v>
+      </c>
+      <c r="D81" s="0">
+        <v>-93643.221388769191</v>
+      </c>
+      <c r="E81" s="0">
+        <v>2268.4254577471725</v>
+      </c>
+      <c r="F81" s="0">
+        <v>-258189.88767595438</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="0">
+        <v>24.561824864841739</v>
+      </c>
+      <c r="B82" s="0">
+        <v>126.14813795049663</v>
+      </c>
+      <c r="C82" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D82" s="0">
+        <v>-79827.99751211243</v>
+      </c>
+      <c r="E82" s="0">
+        <v>2040.6779441492088</v>
+      </c>
+      <c r="F82" s="0">
+        <v>-197655.50716051663</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="0">
+        <v>24.539819572276201</v>
+      </c>
+      <c r="B83" s="0">
+        <v>126.04308948967214</v>
+      </c>
+      <c r="C83" s="0">
+        <v>0.4930951915640841</v>
+      </c>
+      <c r="D83" s="0">
+        <v>-79691.102142452597</v>
+      </c>
+      <c r="E83" s="0">
+        <v>2038.8351371116416</v>
+      </c>
+      <c r="F83" s="0">
+        <v>-197143.91154284729</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="0">
+        <v>24.536564521677761</v>
+      </c>
+      <c r="B84" s="0">
+        <v>126.05375092934713</v>
+      </c>
+      <c r="C84" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D84" s="0">
+        <v>-79687.325104598247</v>
+      </c>
+      <c r="E84" s="0">
+        <v>2038.784218852164</v>
+      </c>
+      <c r="F84" s="0">
+        <v>-197150.31507526236</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="0">
+        <v>24.550846963956413</v>
+      </c>
+      <c r="B85" s="0">
+        <v>126.08290455993628</v>
+      </c>
+      <c r="C85" s="0">
+        <v>0.48183560717118606</v>
+      </c>
+      <c r="D85" s="0">
+        <v>-79751.476556870941</v>
+      </c>
+      <c r="E85" s="0">
+        <v>2039.8449747460927</v>
+      </c>
+      <c r="F85" s="0">
+        <v>-197360.0155075551</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0">
+        <v>24.560154658423048</v>
+      </c>
+      <c r="B86" s="0">
+        <v>126.04313508982501</v>
+      </c>
+      <c r="C86" s="0">
+        <v>0.49656591979165199</v>
+      </c>
+      <c r="D86" s="0">
+        <v>-79756.938143631793</v>
+      </c>
+      <c r="E86" s="0">
+        <v>2039.2416842941968</v>
+      </c>
+      <c r="F86" s="0">
+        <v>-197312.4578742185</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0">
+        <v>24.552687291661318</v>
+      </c>
+      <c r="B87" s="0">
+        <v>126.06559616093703</v>
+      </c>
+      <c r="C87" s="0">
+        <v>0.49955303990324595</v>
+      </c>
+      <c r="D87" s="0">
+        <v>-79746.860385334381</v>
+      </c>
+      <c r="E87" s="0">
+        <v>2039.3282113065247</v>
+      </c>
+      <c r="F87" s="0">
+        <v>-197320.98039840092</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="0">
+        <v>24.540138180366295</v>
+      </c>
+      <c r="B88" s="0">
+        <v>126.0430886299015</v>
+      </c>
+      <c r="C88" s="0">
+        <v>0.49163442469247437</v>
+      </c>
+      <c r="D88" s="0">
+        <v>-79692.111989417215</v>
+      </c>
+      <c r="E88" s="0">
+        <v>2038.8687272934962</v>
+      </c>
+      <c r="F88" s="0">
+        <v>-197146.55142926952</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="0">
+        <v>24.53655541949168</v>
+      </c>
+      <c r="B89" s="0">
+        <v>126.0430950079688</v>
+      </c>
+      <c r="C89" s="0">
+        <v>0.49994210837661363</v>
+      </c>
+      <c r="D89" s="0">
+        <v>-79680.643344658514</v>
+      </c>
+      <c r="E89" s="0">
+        <v>2038.6369328130484</v>
+      </c>
+      <c r="F89" s="0">
+        <v>-197116.87719236908</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="0">
+        <v>24.536621913989901</v>
+      </c>
+      <c r="B90" s="0">
+        <v>126.07201333717923</v>
+      </c>
+      <c r="C90" s="0">
+        <v>0.49992586340198203</v>
+      </c>
+      <c r="D90" s="0">
+        <v>-79698.909312898235</v>
+      </c>
+      <c r="E90" s="0">
+        <v>2039.0407210420112</v>
+      </c>
+      <c r="F90" s="0">
+        <v>-197207.97519771592</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="0">
+        <v>24.536593258949367</v>
+      </c>
+      <c r="B91" s="0">
+        <v>126.04308862565426</v>
+      </c>
+      <c r="C91" s="0">
+        <v>0.49818994837969771</v>
+      </c>
+      <c r="D91" s="0">
+        <v>-79680.737809998885</v>
+      </c>
+      <c r="E91" s="0">
+        <v>2038.6692193783313</v>
+      </c>
+      <c r="F91" s="0">
+        <v>-197117.17527956513</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="0">
+        <v>24.536953659401004</v>
+      </c>
+      <c r="B92" s="0">
+        <v>126.04925613106292</v>
+      </c>
+      <c r="C92" s="0">
+        <v>0.49986083612657128</v>
+      </c>
+      <c r="D92" s="0">
+        <v>-79685.77597088019</v>
+      </c>
+      <c r="E92" s="0">
+        <v>2038.7332051642238</v>
+      </c>
+      <c r="F92" s="0">
+        <v>-197139.46543330821</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="0">
+        <v>24.536557138800749</v>
+      </c>
+      <c r="B93" s="0">
+        <v>126.12237158753652</v>
+      </c>
+      <c r="C93" s="0">
+        <v>0.49996822604137581</v>
+      </c>
+      <c r="D93" s="0">
+        <v>-79730.134495922597</v>
+      </c>
+      <c r="E93" s="0">
+        <v>2039.7384472691151</v>
+      </c>
+      <c r="F93" s="0">
+        <v>-197365.16617737271</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="0">
+        <v>24.536555624889754</v>
+      </c>
+      <c r="B94" s="0">
+        <v>126.04308862652863</v>
+      </c>
+      <c r="C94" s="0">
+        <v>0.4999532461321064</v>
+      </c>
+      <c r="D94" s="0">
+        <v>-79680.640177551977</v>
+      </c>
+      <c r="E94" s="0">
+        <v>2038.636648584504</v>
+      </c>
+      <c r="F94" s="0">
+        <v>-197116.85888483888</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="0">
+        <v>25.999996457078737</v>
+      </c>
+      <c r="B95" s="0">
+        <v>139.96387174519316</v>
+      </c>
+      <c r="C95" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D95" s="0">
+        <v>-93620.915615242178</v>
+      </c>
+      <c r="E95" s="0">
+        <v>2265.8377356647088</v>
+      </c>
+      <c r="F95" s="0">
+        <v>-258056.25704211273</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="0">
+        <v>25.999996781176378</v>
+      </c>
+      <c r="B96" s="0">
+        <v>139.99998700339299</v>
+      </c>
+      <c r="C96" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D96" s="0">
+        <v>-93644.804851521418</v>
+      </c>
+      <c r="E96" s="0">
+        <v>2266.339745217655</v>
+      </c>
+      <c r="F96" s="0">
+        <v>-258189.56550271856</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="0">
+        <v>25.999988812838286</v>
+      </c>
+      <c r="B97" s="0">
+        <v>139.99465315847988</v>
+      </c>
+      <c r="C97" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D97" s="0">
+        <v>-93641.248237173844</v>
+      </c>
+      <c r="E97" s="0">
+        <v>2266.2654212625366</v>
+      </c>
+      <c r="F97" s="0">
+        <v>-258169.79413855355</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0">
+        <v>25.999994854670891</v>
+      </c>
+      <c r="B98" s="0">
+        <v>139.99999303642508</v>
+      </c>
+      <c r="C98" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D98" s="0">
+        <v>-93644.801927993729</v>
+      </c>
+      <c r="E98" s="0">
+        <v>2266.3397847093797</v>
+      </c>
+      <c r="F98" s="0">
+        <v>-258189.56808651844</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0">
+        <v>25.999711047051836</v>
+      </c>
+      <c r="B99" s="0">
+        <v>139.99999998621846</v>
+      </c>
+      <c r="C99" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D99" s="0">
+        <v>-93643.787970538309</v>
+      </c>
+      <c r="E99" s="0">
+        <v>2266.3333452220404</v>
+      </c>
+      <c r="F99" s="0">
+        <v>-258186.69341451887</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0">
+        <v>25.999996777236678</v>
+      </c>
+      <c r="B100" s="0">
+        <v>139.99999999173951</v>
+      </c>
+      <c r="C100" s="0">
+        <v>0.34952280276741265</v>
+      </c>
+      <c r="D100" s="0">
+        <v>-93642.759414650907</v>
+      </c>
+      <c r="E100" s="0">
+        <v>2269.0455056711817</v>
+      </c>
+      <c r="F100" s="0">
+        <v>-258190.03515117092</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="0">
+        <v>25.999996791630114</v>
+      </c>
+      <c r="B101" s="0">
+        <v>139.99997325117667</v>
+      </c>
+      <c r="C101" s="0">
+        <v>0.36169876463469786</v>
+      </c>
+      <c r="D101" s="0">
+        <v>-93642.907980911143</v>
+      </c>
+      <c r="E101" s="0">
+        <v>2268.8262105144654</v>
+      </c>
+      <c r="F101" s="0">
+        <v>-258189.90271534762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor MOGWS algorithm and add new MO optimization algorithms
- Rename MOWAO to MOGWS and update implementation to use glowworm swarm optimization
- Remove whale optimization references and logic
- Add new MO algorithms: MOBAT, MODOA, MOFF with corresponding runner files
- Add utility functions for new algorithms (Attack, EuclidDistance, etc.)
- Update Optimal.xlsx with new results
- Clean up documentation and remove unused references

The changes transition from whale optimization to glowworm swarm approach while maintaining the multi-objective optimization framework. New algorithms provide additional optimization methods.
</commit_message>
<xml_diff>
--- a/Optimal.xlsx
+++ b/Optimal.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="30" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="7">
   <si>
     <t>X1</t>
   </si>
@@ -85,12 +85,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="true"/>
-    <col min="2" max="2" width="11.5546875" customWidth="true"/>
-    <col min="3" max="3" width="12.5546875" customWidth="true"/>
-    <col min="4" max="4" width="12.21875" customWidth="true"/>
-    <col min="5" max="5" width="11.5546875" customWidth="true"/>
-    <col min="6" max="6" width="12.21875" customWidth="true"/>
+    <col min="1" max="1" width="14.5546875" customWidth="true"/>
+    <col min="2" max="2" width="14.5546875" customWidth="true"/>
+    <col min="3" max="3" width="14.5546875" customWidth="true"/>
+    <col min="4" max="4" width="14.5546875" customWidth="true"/>
+    <col min="5" max="5" width="14.5546875" customWidth="true"/>
+    <col min="6" max="6" width="13.5546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -104,2013 +104,2013 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>23.503633910445178</v>
+        <v>0.35111972542188447</v>
       </c>
       <c r="B2" s="0">
-        <v>119.86173633906553</v>
+        <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D2" s="0">
-        <v>-72644.320442153359</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0">
-        <v>1928.9268240705633</v>
+        <v>0.35111972542188447</v>
       </c>
       <c r="F2" s="0">
-        <v>-170504.10044751273</v>
+        <v>0.40744643666425862</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>26</v>
+        <v>0.65589331251858773</v>
       </c>
       <c r="B3" s="0">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0">
-        <v>0.29999999999999999</v>
+        <v>0</v>
       </c>
       <c r="D3" s="0">
-        <v>-93642.095000000001</v>
+        <v>0</v>
       </c>
       <c r="E3" s="0">
-        <v>2269.9360000000001</v>
+        <v>0.65589331251858773</v>
       </c>
       <c r="F3" s="0">
-        <v>-258190.205399</v>
+        <v>0.19012759491473741</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>26</v>
+        <v>0.65597693366699372</v>
       </c>
       <c r="B4" s="0">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="C4" s="0">
-        <v>0.29999999999999999</v>
+        <v>0</v>
       </c>
       <c r="D4" s="0">
-        <v>-93642.095000000001</v>
+        <v>0</v>
       </c>
       <c r="E4" s="0">
-        <v>2269.9360000000001</v>
+        <v>0.65597693366699372</v>
       </c>
       <c r="F4" s="0">
-        <v>-258190.205399</v>
+        <v>0.19007597043488478</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>25.999980170157144</v>
+        <v>0.34880903083467485</v>
       </c>
       <c r="B5" s="0">
-        <v>100.15824259477009</v>
+        <v>0</v>
       </c>
       <c r="C5" s="0">
-        <v>0.49891020237293587</v>
+        <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>-67291.827038041665</v>
+        <v>0</v>
       </c>
       <c r="E5" s="0">
-        <v>1712.5587099473578</v>
+        <v>0.34880903083467485</v>
       </c>
       <c r="F5" s="0">
-        <v>-132055.93137534091</v>
+        <v>0.40939943207386364</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>25.215035441292535</v>
+        <v>0.69989618528878328</v>
       </c>
       <c r="B6" s="0">
-        <v>109.93065366205062</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D6" s="0">
-        <v>-71539.074865915551</v>
+        <v>0</v>
       </c>
       <c r="E6" s="0">
-        <v>1830.2983521154706</v>
+        <v>0.69989618528878328</v>
       </c>
       <c r="F6" s="0">
-        <v>-154172.92920217643</v>
+        <v>0.16340201692283329</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>24.476255963325571</v>
+        <v>0.90919823802307265</v>
       </c>
       <c r="B7" s="0">
-        <v>126.0045303718743</v>
+        <v>0</v>
       </c>
       <c r="C7" s="0">
-        <v>0.4847392472032469</v>
+        <v>0</v>
       </c>
       <c r="D7" s="0">
-        <v>-79461.424584664215</v>
+        <v>0</v>
       </c>
       <c r="E7" s="0">
-        <v>2036.9855353397265</v>
+        <v>0.90919823802307265</v>
       </c>
       <c r="F7" s="0">
-        <v>-196497.11228706728</v>
+        <v>0.046481128648691805</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>25.99996773756282</v>
+        <v>0.65161580057967938</v>
       </c>
       <c r="B8" s="0">
-        <v>139.99066609579342</v>
+        <v>0</v>
       </c>
       <c r="C8" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D8" s="0">
-        <v>-93638.53540372428</v>
+        <v>0</v>
       </c>
       <c r="E8" s="0">
-        <v>2266.2095157276008</v>
+        <v>0.65161580057967938</v>
       </c>
       <c r="F8" s="0">
-        <v>-258154.8610070048</v>
+        <v>0.19277277016958883</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>25.999956568353113</v>
+        <v>0.64190087281693864</v>
       </c>
       <c r="B9" s="0">
-        <v>139.9410546151598</v>
+        <v>0</v>
       </c>
       <c r="C9" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D9" s="0">
-        <v>-93605.680358376922</v>
+        <v>0</v>
       </c>
       <c r="E9" s="0">
-        <v>2265.5196589198936</v>
+        <v>0.64190087281693864</v>
       </c>
       <c r="F9" s="0">
-        <v>-257971.6471081374</v>
+        <v>0.19881283533937055</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>25.999832032398238</v>
+        <v>0.89526633762802676</v>
       </c>
       <c r="B10" s="0">
-        <v>139.99999843527786</v>
+        <v>0</v>
       </c>
       <c r="C10" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D10" s="0">
-        <v>-93644.221147790595</v>
+        <v>0</v>
       </c>
       <c r="E10" s="0">
-        <v>2266.3361099564941</v>
+        <v>0.89526633762802676</v>
       </c>
       <c r="F10" s="0">
-        <v>-258187.92408002037</v>
+        <v>0.053814850239115808</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>24.186710040060806</v>
+        <v>0.33306554321145693</v>
       </c>
       <c r="B11" s="0">
-        <v>139.99999999991675</v>
+        <v>0</v>
       </c>
       <c r="C11" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D11" s="0">
-        <v>-87137.126795622622</v>
+        <v>0</v>
       </c>
       <c r="E11" s="0">
-        <v>2224.5799322214434</v>
+        <v>0.33306554321145693</v>
       </c>
       <c r="F11" s="0">
-        <v>-239659.01232102094</v>
+        <v>0.42288169045553847</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>24.737846250937324</v>
+        <v>0.33406842634584977</v>
       </c>
       <c r="B12" s="0">
-        <v>122.24094179280534</v>
+        <v>0</v>
       </c>
       <c r="C12" s="0">
-        <v>0.49609365302965164</v>
+        <v>0</v>
       </c>
       <c r="D12" s="0">
-        <v>-77938.718247958561</v>
+        <v>0</v>
       </c>
       <c r="E12" s="0">
-        <v>1990.4919261976079</v>
+        <v>0.33406842634584977</v>
       </c>
       <c r="F12" s="0">
-        <v>-186960.85022738617</v>
+        <v>0.42201347217616758</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>24.636845843702737</v>
+        <v>0.34318696714917313</v>
       </c>
       <c r="B13" s="0">
-        <v>126.11957009981451</v>
+        <v>0</v>
       </c>
       <c r="C13" s="0">
-        <v>0.49779954163703583</v>
+        <v>0</v>
       </c>
       <c r="D13" s="0">
-        <v>-80052.867546223977</v>
+        <v>0</v>
       </c>
       <c r="E13" s="0">
-        <v>2042.048148409262</v>
+        <v>0.34318696714917313</v>
       </c>
       <c r="F13" s="0">
-        <v>-198187.98372569526</v>
+        <v>0.4141783828253065</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>24.635112822572228</v>
+        <v>0.34040288906719829</v>
       </c>
       <c r="B14" s="0">
-        <v>126.11808920055184</v>
+        <v>0</v>
       </c>
       <c r="C14" s="0">
-        <v>0.49773604870144222</v>
+        <v>0</v>
       </c>
       <c r="D14" s="0">
-        <v>-80046.330913389393</v>
+        <v>0</v>
       </c>
       <c r="E14" s="0">
-        <v>2041.9887940358572</v>
+        <v>0.34040288906719829</v>
       </c>
       <c r="F14" s="0">
-        <v>-198168.9554369968</v>
+        <v>0.41655943827395903</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>25.207848894695875</v>
+        <v>0.34833005575021564</v>
       </c>
       <c r="B15" s="0">
-        <v>109.98278330432498</v>
+        <v>0</v>
       </c>
       <c r="C15" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D15" s="0">
-        <v>-71552.210688497405</v>
+        <v>0</v>
       </c>
       <c r="E15" s="0">
-        <v>1830.8574479749632</v>
+        <v>0.34833005575021564</v>
       </c>
       <c r="F15" s="0">
-        <v>-154274.03919795723</v>
+        <v>0.40980506970136077</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>25.221617513215858</v>
+        <v>0</v>
       </c>
       <c r="B16" s="0">
-        <v>109.98278315116404</v>
+        <v>0</v>
       </c>
       <c r="C16" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D16" s="0">
-        <v>-71591.11040733433</v>
+        <v>0</v>
       </c>
       <c r="E16" s="0">
-        <v>1831.1745371305415</v>
+        <v>0</v>
       </c>
       <c r="F16" s="0">
-        <v>-154360.83845494653</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>24.233471524036883</v>
+        <v>0.0043447236291691248</v>
       </c>
       <c r="B17" s="0">
-        <v>139.89728201152161</v>
+        <v>0.0043447236291691248</v>
       </c>
       <c r="C17" s="0">
-        <v>0.46277224429232955</v>
+        <v>0.0043447236291691248</v>
       </c>
       <c r="D17" s="0">
-        <v>-87241.114868897916</v>
+        <v>0.0043447236291691248</v>
       </c>
       <c r="E17" s="0">
-        <v>2224.8984242063439</v>
+        <v>0.0043447236291691248</v>
       </c>
       <c r="F17" s="0">
-        <v>-239784.43153802038</v>
+        <v>0.97191164096186722</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>24.243492047898204</v>
+        <v>0.002001831254436902</v>
       </c>
       <c r="B18" s="0">
-        <v>139.99963893364816</v>
+        <v>0.002001831254436902</v>
       </c>
       <c r="C18" s="0">
-        <v>0.48442148171524357</v>
+        <v>0.002001831254436902</v>
       </c>
       <c r="D18" s="0">
-        <v>-87340.475839731997</v>
+        <v>0.002001831254436902</v>
       </c>
       <c r="E18" s="0">
-        <v>2226.1627047995653</v>
+        <v>0.002001831254436902</v>
       </c>
       <c r="F18" s="0">
-        <v>-240238.08812697517</v>
+        <v>0.97287340640819575</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>24.233573832413228</v>
+        <v>0</v>
       </c>
       <c r="B19" s="0">
-        <v>139.99984964249674</v>
+        <v>0</v>
       </c>
       <c r="C19" s="0">
-        <v>0.48784636926144842</v>
+        <v>0</v>
       </c>
       <c r="D19" s="0">
-        <v>-87305.057198630675</v>
+        <v>0</v>
       </c>
       <c r="E19" s="0">
-        <v>2225.8756376718607</v>
+        <v>0</v>
       </c>
       <c r="F19" s="0">
-        <v>-240137.44540266096</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>24.233394436398182</v>
+        <v>0.0015281908463212982</v>
       </c>
       <c r="B20" s="0">
-        <v>139.84403067240376</v>
+        <v>0.0015281908463212982</v>
       </c>
       <c r="C20" s="0">
-        <v>0.46577160842373727</v>
+        <v>0.0015281908463212982</v>
       </c>
       <c r="D20" s="0">
-        <v>-87208.050032265906</v>
+        <v>0.0015281908463212982</v>
       </c>
       <c r="E20" s="0">
-        <v>2224.1025266972038</v>
+        <v>0.0015281908463212982</v>
       </c>
       <c r="F20" s="0">
-        <v>-239600.96924798458</v>
+        <v>0.97439372331193363</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>24.723485726408992</v>
+        <v>0</v>
       </c>
       <c r="B21" s="0">
-        <v>122.2444814546519</v>
+        <v>0</v>
       </c>
       <c r="C21" s="0">
-        <v>0.49891034410267648</v>
+        <v>0</v>
       </c>
       <c r="D21" s="0">
-        <v>-77895.932625725181</v>
+        <v>0</v>
       </c>
       <c r="E21" s="0">
-        <v>1990.1597605118943</v>
+        <v>0</v>
       </c>
       <c r="F21" s="0">
-        <v>-186859.81555496884</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>24.728931627359248</v>
+        <v>0.001561485075841629</v>
       </c>
       <c r="B22" s="0">
-        <v>122.24466899336817</v>
+        <v>0.001561485075841629</v>
       </c>
       <c r="C22" s="0">
-        <v>0.49999271605439022</v>
+        <v>0.001561485075841629</v>
       </c>
       <c r="D22" s="0">
-        <v>-77913.1502053312</v>
+        <v>0.001561485075841629</v>
       </c>
       <c r="E22" s="0">
-        <v>1990.2683253512432</v>
+        <v>0.001561485075841629</v>
       </c>
       <c r="F22" s="0">
-        <v>-186902.80906410687</v>
+        <v>0.97426103983172363</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>24.727852451260183</v>
+        <v>0</v>
       </c>
       <c r="B23" s="0">
-        <v>122.35026117672091</v>
+        <v>0</v>
       </c>
       <c r="C23" s="0">
-        <v>0.49993052751939276</v>
+        <v>0</v>
       </c>
       <c r="D23" s="0">
-        <v>-77976.189339403558</v>
+        <v>0</v>
       </c>
       <c r="E23" s="0">
-        <v>1991.712321424144</v>
+        <v>0</v>
       </c>
       <c r="F23" s="0">
-        <v>-187217.73215312045</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>24.72890615226035</v>
+        <v>0</v>
       </c>
       <c r="B24" s="0">
-        <v>122.24742065116168</v>
+        <v>0</v>
       </c>
       <c r="C24" s="0">
-        <v>0.49998368769329687</v>
+        <v>0</v>
       </c>
       <c r="D24" s="0">
-        <v>-77914.801238954897</v>
+        <v>0</v>
       </c>
       <c r="E24" s="0">
-        <v>1990.3061490329778</v>
+        <v>0</v>
       </c>
       <c r="F24" s="0">
-        <v>-186911.03320471465</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>24.728933381108028</v>
+        <v>0.69654416215177661</v>
       </c>
       <c r="B25" s="0">
-        <v>122.24448156685143</v>
+        <v>0</v>
       </c>
       <c r="C25" s="0">
-        <v>0.4999974537122418</v>
+        <v>0</v>
       </c>
       <c r="D25" s="0">
-        <v>-77913.037861067438</v>
+        <v>0</v>
       </c>
       <c r="E25" s="0">
-        <v>1990.2656753284068</v>
+        <v>0.69654416215177661</v>
       </c>
       <c r="F25" s="0">
-        <v>-186902.24902424208</v>
+        <v>0.16540778690921365</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>25.694940041256441</v>
+        <v>0.68575193911563925</v>
       </c>
       <c r="B26" s="0">
-        <v>100.01419825226098</v>
+        <v>0</v>
       </c>
       <c r="C26" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D26" s="0">
-        <v>-66412.108481921532</v>
+        <v>0</v>
       </c>
       <c r="E26" s="0">
-        <v>1703.5118248565636</v>
+        <v>0.68575193911563925</v>
       </c>
       <c r="F26" s="0">
-        <v>-130086.00254883181</v>
+        <v>0.17189859370024052</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>25.695059224837454</v>
+        <v>0.69401962525650907</v>
       </c>
       <c r="B27" s="0">
-        <v>100.12809135297761</v>
+        <v>0</v>
       </c>
       <c r="C27" s="0">
-        <v>0.33337349348275314</v>
+        <v>0</v>
       </c>
       <c r="D27" s="0">
-        <v>-66484.590433498481</v>
+        <v>0</v>
       </c>
       <c r="E27" s="0">
-        <v>1708.0936283415754</v>
+        <v>0.69401962525650907</v>
       </c>
       <c r="F27" s="0">
-        <v>-130383.89202622641</v>
+        <v>0.16692159717316579</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>25.695219533762163</v>
+        <v>0.69630329468485364</v>
       </c>
       <c r="B28" s="0">
-        <v>100.01394851723779</v>
+        <v>0</v>
       </c>
       <c r="C28" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D28" s="0">
-        <v>-66412.663990775749</v>
+        <v>0</v>
       </c>
       <c r="E28" s="0">
-        <v>1703.514790252148</v>
+        <v>0.69630329468485364</v>
       </c>
       <c r="F28" s="0">
-        <v>-130086.80884793536</v>
+        <v>0.16555210187522573</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>24.579306293403857</v>
+        <v>0.69799975288468197</v>
       </c>
       <c r="B29" s="0">
-        <v>136.40590491643599</v>
+        <v>0</v>
       </c>
       <c r="C29" s="0">
-        <v>0.49265709172725447</v>
+        <v>0</v>
       </c>
       <c r="D29" s="0">
-        <v>-86298.632474853948</v>
+        <v>0</v>
       </c>
       <c r="E29" s="0">
-        <v>2183.795527766295</v>
+        <v>0.69799975288468197</v>
       </c>
       <c r="F29" s="0">
-        <v>-231310.11383570003</v>
+        <v>0.16453620492286924</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>24.60850064663331</v>
+        <v>0.69602368563235983</v>
       </c>
       <c r="B30" s="0">
-        <v>136.23360153508216</v>
+        <v>0</v>
       </c>
       <c r="C30" s="0">
-        <v>0.41020893557474247</v>
+        <v>0</v>
       </c>
       <c r="D30" s="0">
-        <v>-86291.744176795051</v>
+        <v>0</v>
       </c>
       <c r="E30" s="0">
-        <v>2183.5552745679734</v>
+        <v>0.69602368563235983</v>
       </c>
       <c r="F30" s="0">
-        <v>-231008.3188969382</v>
+        <v>0.16571966004684024</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>24.582888934977557</v>
+        <v>0.34655927979443407</v>
       </c>
       <c r="B31" s="0">
-        <v>136.49798664469765</v>
+        <v>0</v>
       </c>
       <c r="C31" s="0">
-        <v>0.49749303235876968</v>
+        <v>0</v>
       </c>
       <c r="D31" s="0">
-        <v>-86368.815489328801</v>
+        <v>0</v>
       </c>
       <c r="E31" s="0">
-        <v>2185.0710218120198</v>
+        <v>0.34655927979443407</v>
       </c>
       <c r="F31" s="0">
-        <v>-231657.57931472606</v>
+        <v>0.41130714307507177</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>24.601212278254078</v>
+        <v>0.34378784919656452</v>
       </c>
       <c r="B32" s="0">
-        <v>136.41737271296327</v>
+        <v>0</v>
       </c>
       <c r="C32" s="0">
-        <v>0.49276475767192279</v>
+        <v>0</v>
       </c>
       <c r="D32" s="0">
-        <v>-86382.426343452113</v>
+        <v>0</v>
       </c>
       <c r="E32" s="0">
-        <v>2184.45748913544</v>
+        <v>0.34378784919656452</v>
       </c>
       <c r="F32" s="0">
-        <v>-231561.58763478536</v>
+        <v>0.41366575300724207</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>24.579481802690289</v>
+        <v>0.33855770850549949</v>
       </c>
       <c r="B33" s="0">
-        <v>136.49798658188055</v>
+        <v>0</v>
       </c>
       <c r="C33" s="0">
-        <v>0.49999592201205201</v>
+        <v>0</v>
       </c>
       <c r="D33" s="0">
-        <v>-86356.925337069813</v>
+        <v>0</v>
       </c>
       <c r="E33" s="0">
-        <v>2184.9475527263203</v>
+        <v>0.33855770850549949</v>
       </c>
       <c r="F33" s="0">
-        <v>-231624.47522783405</v>
+        <v>0.41814287964698804</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>25.994530605726482</v>
+        <v>0.34663656299847695</v>
       </c>
       <c r="B34" s="0">
-        <v>100.30469889742342</v>
+        <v>0</v>
       </c>
       <c r="C34" s="0">
-        <v>0.49910169128620496</v>
+        <v>0</v>
       </c>
       <c r="D34" s="0">
-        <v>-67374.646981768034</v>
+        <v>0</v>
       </c>
       <c r="E34" s="0">
-        <v>1714.4655061147407</v>
+        <v>0.34663656299847695</v>
       </c>
       <c r="F34" s="0">
-        <v>-132414.3108492014</v>
+        <v>0.41124150706891971</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>25.978064501392584</v>
+        <v>0.34936247946518817</v>
       </c>
       <c r="B35" s="0">
-        <v>100.14705562844978</v>
+        <v>0</v>
       </c>
       <c r="C35" s="0">
-        <v>0.49916226409750736</v>
+        <v>0</v>
       </c>
       <c r="D35" s="0">
-        <v>-67227.997448784212</v>
+        <v>0</v>
       </c>
       <c r="E35" s="0">
-        <v>1711.8939611940498</v>
+        <v>0.34936247946518817</v>
       </c>
       <c r="F35" s="0">
-        <v>-131911.86628422557</v>
+        <v>0.40893107046200761</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>25.993578391266716</v>
+        <v>0.3415260661866808</v>
       </c>
       <c r="B36" s="0">
-        <v>100.4030211607184</v>
+        <v>0</v>
       </c>
       <c r="C36" s="0">
-        <v>0.49980059204840921</v>
+        <v>0</v>
       </c>
       <c r="D36" s="0">
-        <v>-67437.218936462639</v>
+        <v>0</v>
       </c>
       <c r="E36" s="0">
-        <v>1715.7976898398279</v>
+        <v>0.3415260661866808</v>
       </c>
       <c r="F36" s="0">
-        <v>-132669.34379900459</v>
+        <v>0.41559768464979474</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>25.992807881840015</v>
+        <v>0.34598725948272285</v>
       </c>
       <c r="B37" s="0">
-        <v>100.40176846565717</v>
+        <v>0</v>
       </c>
       <c r="C37" s="0">
-        <v>0.49969115575311296</v>
+        <v>0</v>
       </c>
       <c r="D37" s="0">
-        <v>-67434.399986130622</v>
+        <v>0</v>
       </c>
       <c r="E37" s="0">
-        <v>1715.7645002109693</v>
+        <v>0.34598725948272285</v>
       </c>
       <c r="F37" s="0">
-        <v>-132661.98238107836</v>
+        <v>0.41179318307016977</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>25.99358137210012</v>
+        <v>0.35205596799481542</v>
       </c>
       <c r="B38" s="0">
-        <v>100.40317827258617</v>
+        <v>0</v>
       </c>
       <c r="C38" s="0">
-        <v>0.49983723794568502</v>
+        <v>0</v>
       </c>
       <c r="D38" s="0">
-        <v>-67437.331026247382</v>
+        <v>0</v>
       </c>
       <c r="E38" s="0">
-        <v>1715.7992834501501</v>
+        <v>0.35205596799481542</v>
       </c>
       <c r="F38" s="0">
-        <v>-132669.77506136795</v>
+        <v>0.40665695588907813</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>25.993594674229438</v>
+        <v>0.34466031261491942</v>
       </c>
       <c r="B39" s="0">
-        <v>100.40273182872063</v>
+        <v>0</v>
       </c>
       <c r="C39" s="0">
-        <v>0.49982296508894447</v>
+        <v>0</v>
       </c>
       <c r="D39" s="0">
-        <v>-67437.06994841127</v>
+        <v>0</v>
       </c>
       <c r="E39" s="0">
-        <v>1715.7936408544217</v>
+        <v>0.34466031261491942</v>
       </c>
       <c r="F39" s="0">
-        <v>-132668.66371294187</v>
+        <v>0.41292222609357843</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>25.993603664937506</v>
+        <v>0.35083979080507582</v>
       </c>
       <c r="B40" s="0">
-        <v>100.40354684767328</v>
+        <v>0</v>
       </c>
       <c r="C40" s="0">
-        <v>0.49983723794568502</v>
+        <v>0</v>
       </c>
       <c r="D40" s="0">
-        <v>-67437.632306581683</v>
+        <v>0</v>
       </c>
       <c r="E40" s="0">
-        <v>1715.8049200479063</v>
+        <v>0.35083979080507582</v>
       </c>
       <c r="F40" s="0">
-        <v>-132670.86739090137</v>
+        <v>0.40768269415365233</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>25.993601850003284</v>
+        <v>0.34999932587935478</v>
       </c>
       <c r="B41" s="0">
-        <v>100.40330838710769</v>
+        <v>0</v>
       </c>
       <c r="C41" s="0">
-        <v>0.49983638928189927</v>
+        <v>0</v>
       </c>
       <c r="D41" s="0">
-        <v>-67437.469921100143</v>
+        <v>0</v>
       </c>
       <c r="E41" s="0">
-        <v>1715.8015789070839</v>
+        <v>0.34999932587935478</v>
       </c>
       <c r="F41" s="0">
-        <v>-132670.22690529202</v>
+        <v>0.40839259142624429</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>25.993616767257596</v>
+        <v>0.3457932131387435</v>
       </c>
       <c r="B42" s="0">
-        <v>100.40354684767119</v>
+        <v>0</v>
       </c>
       <c r="C42" s="0">
-        <v>0.49969097691714992</v>
+        <v>0</v>
       </c>
       <c r="D42" s="0">
-        <v>-67437.664134493345</v>
+        <v>0</v>
       </c>
       <c r="E42" s="0">
-        <v>1715.8078515676018</v>
+        <v>0.3457932131387435</v>
       </c>
       <c r="F42" s="0">
-        <v>-132670.93662809281</v>
+        <v>0.41195815358195509</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>24.490026832697335</v>
+        <v>0.35276063938407665</v>
       </c>
       <c r="B43" s="0">
-        <v>126.05239196412442</v>
+        <v>0</v>
       </c>
       <c r="C43" s="0">
-        <v>0.49995746219383258</v>
+        <v>0</v>
       </c>
       <c r="D43" s="0">
-        <v>-79535.970432872418</v>
+        <v>0</v>
       </c>
       <c r="E43" s="0">
-        <v>2037.694331088104</v>
+        <v>0.35276063938407665</v>
       </c>
       <c r="F43" s="0">
-        <v>-196760.58384421104</v>
+        <v>0.40606343824944013</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>24.487798915820502</v>
+        <v>0.34539046257451989</v>
       </c>
       <c r="B44" s="0">
-        <v>126.03568657269392</v>
+        <v>0</v>
       </c>
       <c r="C44" s="0">
-        <v>0.49995399467527657</v>
+        <v>0</v>
       </c>
       <c r="D44" s="0">
-        <v>-79518.358211241924</v>
+        <v>0</v>
       </c>
       <c r="E44" s="0">
-        <v>2037.4108795675302</v>
+        <v>0.34539046257451989</v>
       </c>
       <c r="F44" s="0">
-        <v>-196689.93580606443</v>
+        <v>0.41230070395267626</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>24.635110122309499</v>
+        <v>0.35560455712434796</v>
       </c>
       <c r="B45" s="0">
-        <v>126.11810200013151</v>
+        <v>0</v>
       </c>
       <c r="C45" s="0">
-        <v>0.49774967733705539</v>
+        <v>0</v>
       </c>
       <c r="D45" s="0">
-        <v>-80046.330383804569</v>
+        <v>0</v>
       </c>
       <c r="E45" s="0">
-        <v>2041.9886647200956</v>
+        <v>0.35560455712434796</v>
       </c>
       <c r="F45" s="0">
-        <v>-198168.97327293019</v>
+        <v>0.40367411835109157</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>24.629977178534578</v>
+        <v>0.35389116415478028</v>
       </c>
       <c r="B46" s="0">
-        <v>126.11811895020004</v>
+        <v>0</v>
       </c>
       <c r="C46" s="0">
-        <v>0.497736126386634</v>
+        <v>0</v>
       </c>
       <c r="D46" s="0">
-        <v>-80029.731976184761</v>
+        <v>0</v>
       </c>
       <c r="E46" s="0">
-        <v>2041.8709322770003</v>
+        <v>0.35389116415478028</v>
       </c>
       <c r="F46" s="0">
-        <v>-198126.4655429429</v>
+        <v>0.40511247772811687</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>24.635112822411642</v>
+        <v>0.35085091672272645</v>
       </c>
       <c r="B47" s="0">
-        <v>126.11808920061023</v>
+        <v>0</v>
       </c>
       <c r="C47" s="0">
-        <v>0.49777184502965388</v>
+        <v>0</v>
       </c>
       <c r="D47" s="0">
-        <v>-80046.331401526244</v>
+        <v>0</v>
       </c>
       <c r="E47" s="0">
-        <v>2041.9881504149891</v>
+        <v>0.35085091672272645</v>
       </c>
       <c r="F47" s="0">
-        <v>-198168.9553397464</v>
+        <v>0.40767330237213983</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>25.987852089076881</v>
+        <v>0.34705661811303751</v>
       </c>
       <c r="B48" s="0">
-        <v>100.1430373766635</v>
+        <v>0</v>
       </c>
       <c r="C48" s="0">
-        <v>0.49941987503950597</v>
+        <v>0</v>
       </c>
       <c r="D48" s="0">
-        <v>-67250.547717157999</v>
+        <v>0</v>
       </c>
       <c r="E48" s="0">
-        <v>1712.0588837938531</v>
+        <v>0.34705661811303751</v>
       </c>
       <c r="F48" s="0">
-        <v>-131952.41298954652</v>
+        <v>0.41088488551638946</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>25.983250366214705</v>
+        <v>0.34751466731022956</v>
       </c>
       <c r="B49" s="0">
-        <v>100.17980272200197</v>
+        <v>0</v>
       </c>
       <c r="C49" s="0">
-        <v>0.49890889240302139</v>
+        <v>0</v>
       </c>
       <c r="D49" s="0">
-        <v>-67262.994037105731</v>
+        <v>0</v>
       </c>
       <c r="E49" s="0">
-        <v>1712.4731318843458</v>
+        <v>0.34751466731022956</v>
       </c>
       <c r="F49" s="0">
-        <v>-132025.37257573107</v>
+        <v>0.41049625335352657</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>25.984691860246738</v>
+        <v>0.64236967302922965</v>
       </c>
       <c r="B50" s="0">
-        <v>100.19287466913889</v>
+        <v>0</v>
       </c>
       <c r="C50" s="0">
-        <v>0.49881114885696226</v>
+        <v>0</v>
       </c>
       <c r="D50" s="0">
-        <v>-67275.347013738152</v>
+        <v>0</v>
       </c>
       <c r="E50" s="0">
-        <v>1712.6897869860647</v>
+        <v>0.64236967302922965</v>
       </c>
       <c r="F50" s="0">
-        <v>-132067.41166166583</v>
+        <v>0.19852032275969111</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>25.989193062023944</v>
+        <v>0.63895266568810838</v>
       </c>
       <c r="B51" s="0">
-        <v>100.17542320355184</v>
+        <v>0</v>
       </c>
       <c r="C51" s="0">
-        <v>0.49845312408693959</v>
+        <v>0</v>
       </c>
       <c r="D51" s="0">
-        <v>-67275.399808514077</v>
+        <v>0</v>
       </c>
       <c r="E51" s="0">
-        <v>1712.557311576699</v>
+        <v>0.63895266568810838</v>
       </c>
       <c r="F51" s="0">
-        <v>-132044.89072354804</v>
+        <v>0.20065485196436683</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>25.989611710353799</v>
+        <v>0.63512983459516847</v>
       </c>
       <c r="B52" s="0">
-        <v>100.14281092340165</v>
+        <v>0</v>
       </c>
       <c r="C52" s="0">
-        <v>0.49892940710700751</v>
+        <v>0</v>
       </c>
       <c r="D52" s="0">
-        <v>-67254.922196499567</v>
+        <v>0</v>
       </c>
       <c r="E52" s="0">
-        <v>1712.105078784947</v>
+        <v>0.63512983459516847</v>
       </c>
       <c r="F52" s="0">
-        <v>-131961.01184476897</v>
+        <v>0.20304966616785425</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>25.970687880467295</v>
+        <v>0.63188097537896781</v>
       </c>
       <c r="B53" s="0">
-        <v>100.14281109888539</v>
+        <v>0</v>
       </c>
       <c r="C53" s="0">
-        <v>0.49893693687600649</v>
+        <v>0</v>
       </c>
       <c r="D53" s="0">
-        <v>-67206.195008319584</v>
+        <v>0</v>
       </c>
       <c r="E53" s="0">
-        <v>1711.6691300366383</v>
+        <v>0.63188097537896781</v>
       </c>
       <c r="F53" s="0">
-        <v>-131862.12516359915</v>
+        <v>0.20509058668363489</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>25.989698744394708</v>
+        <v>0.64020508839411316</v>
       </c>
       <c r="B54" s="0">
-        <v>100.2214533361803</v>
+        <v>0</v>
       </c>
       <c r="C54" s="0">
-        <v>0.49873748750026348</v>
+        <v>0</v>
       </c>
       <c r="D54" s="0">
-        <v>-67307.140310927774</v>
+        <v>0</v>
       </c>
       <c r="E54" s="0">
-        <v>1713.2036634310618</v>
+        <v>0.64020508839411316</v>
       </c>
       <c r="F54" s="0">
-        <v>-132169.059760879</v>
+        <v>0.19987183002089404</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>25.98969913278172</v>
+        <v>0.64156508130842338</v>
       </c>
       <c r="B55" s="0">
-        <v>100.24398619192473</v>
+        <v>0</v>
       </c>
       <c r="C55" s="0">
-        <v>0.49902115360546762</v>
+        <v>0</v>
       </c>
       <c r="D55" s="0">
-        <v>-67322.043411091043</v>
+        <v>0</v>
       </c>
       <c r="E55" s="0">
-        <v>1713.5117787538904</v>
+        <v>0.64156508130842338</v>
       </c>
       <c r="F55" s="0">
-        <v>-132228.57109881076</v>
+        <v>0.19902242146959981</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>25.989419212691942</v>
+        <v>0.63938369959049235</v>
       </c>
       <c r="B56" s="0">
-        <v>100.14294607680752</v>
+        <v>0</v>
       </c>
       <c r="C56" s="0">
-        <v>0.49902025129928684</v>
+        <v>0</v>
       </c>
       <c r="D56" s="0">
-        <v>-67254.517129333501</v>
+        <v>0</v>
       </c>
       <c r="E56" s="0">
-        <v>1712.100890817559</v>
+        <v>0.63938369959049235</v>
       </c>
       <c r="F56" s="0">
-        <v>-131960.36230594668</v>
+        <v>0.2003852805316223</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>25.989699135486454</v>
+        <v>0.63570054466953918</v>
       </c>
       <c r="B57" s="0">
-        <v>100.14350609028087</v>
+        <v>0</v>
       </c>
       <c r="C57" s="0">
-        <v>0.49893197429535413</v>
+        <v>0</v>
       </c>
       <c r="D57" s="0">
-        <v>-67255.606973545466</v>
+        <v>0</v>
       </c>
       <c r="E57" s="0">
-        <v>1712.1167088473267</v>
+        <v>0.63570054466953918</v>
       </c>
       <c r="F57" s="0">
-        <v>-131963.30299963412</v>
+        <v>0.20269168782111702</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>25.9889988526952</v>
+        <v>0.63286111652473742</v>
       </c>
       <c r="B58" s="0">
-        <v>100.14281081184765</v>
+        <v>0</v>
       </c>
       <c r="C58" s="0">
-        <v>0.49892993414461151</v>
+        <v>0</v>
       </c>
       <c r="D58" s="0">
-        <v>-67253.344068590362</v>
+        <v>0</v>
       </c>
       <c r="E58" s="0">
-        <v>1712.0909536463328</v>
+        <v>0.63286111652473742</v>
       </c>
       <c r="F58" s="0">
-        <v>-131957.8090402043</v>
+        <v>0.20447431435261787</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>22.13770774449247</v>
+        <v>0.63540990228020222</v>
       </c>
       <c r="B59" s="0">
-        <v>100.00000130980764</v>
+        <v>0</v>
       </c>
       <c r="C59" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D59" s="0">
-        <v>-57256.152283997813</v>
+        <v>0</v>
       </c>
       <c r="E59" s="0">
-        <v>1621.3914275619879</v>
+        <v>0.63540990228020222</v>
       </c>
       <c r="F59" s="0">
-        <v>-111513.62819203545</v>
+        <v>0.20287397340182012</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>22.105789939758711</v>
+        <v>0.63877470663518565</v>
       </c>
       <c r="B60" s="0">
-        <v>100.00034022492359</v>
+        <v>0</v>
       </c>
       <c r="C60" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D60" s="0">
-        <v>-57174.272946933415</v>
+        <v>0</v>
       </c>
       <c r="E60" s="0">
-        <v>1620.6610714390811</v>
+        <v>0.63877470663518565</v>
       </c>
       <c r="F60" s="0">
-        <v>-111348.07218196601</v>
+        <v>0.20076617524332363</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>22.117836587050856</v>
+        <v>0.90362352699887749</v>
       </c>
       <c r="B61" s="0">
-        <v>100.00091211861616</v>
+        <v>0</v>
       </c>
       <c r="C61" s="0">
-        <v>0.4811458876712813</v>
+        <v>0</v>
       </c>
       <c r="D61" s="0">
-        <v>-57205.31290814704</v>
+        <v>0</v>
       </c>
       <c r="E61" s="0">
-        <v>1621.285451988216</v>
+        <v>0.90362352699887749</v>
       </c>
       <c r="F61" s="0">
-        <v>-111412.16472985045</v>
+        <v>0.049408853923582186</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>22.038705244659095</v>
+        <v>0.89985859240326926</v>
       </c>
       <c r="B62" s="0">
-        <v>100.00002206542131</v>
+        <v>0</v>
       </c>
       <c r="C62" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D62" s="0">
-        <v>-57001.599779841454</v>
+        <v>0</v>
       </c>
       <c r="E62" s="0">
-        <v>1619.1116884938551</v>
+        <v>0.89985859240326926</v>
       </c>
       <c r="F62" s="0">
-        <v>-110997.80950023182</v>
+        <v>0.051391233224534649</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>22.000022956889616</v>
+        <v>0.90605782414445668</v>
       </c>
       <c r="B63" s="0">
-        <v>100.00107563041888</v>
+        <v>0</v>
       </c>
       <c r="C63" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D63" s="0">
-        <v>-56902.72603828174</v>
+        <v>0</v>
       </c>
       <c r="E63" s="0">
-        <v>1618.2354799599905</v>
+        <v>0.90605782414445668</v>
       </c>
       <c r="F63" s="0">
-        <v>-110798.58806048136</v>
+        <v>0.04812930282287986</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>22.018575875402306</v>
+        <v>0.89806559520079365</v>
       </c>
       <c r="B64" s="0">
-        <v>100.00000009345632</v>
+        <v>0</v>
       </c>
       <c r="C64" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D64" s="0">
-        <v>-56949.829015013005</v>
+        <v>0</v>
       </c>
       <c r="E64" s="0">
-        <v>1618.647803709558</v>
+        <v>0.89806559520079365</v>
       </c>
       <c r="F64" s="0">
-        <v>-110892.87408657809</v>
+        <v>0.052336771209944177</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0">
-        <v>22.000239272706747</v>
+        <v>0.90825261914583688</v>
       </c>
       <c r="B65" s="0">
-        <v>100.00038773544443</v>
+        <v>0</v>
       </c>
       <c r="C65" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D65" s="0">
-        <v>-56902.897249651855</v>
+        <v>0</v>
       </c>
       <c r="E65" s="0">
-        <v>1618.230899973114</v>
+        <v>0.90825261914583688</v>
       </c>
       <c r="F65" s="0">
-        <v>-110798.18899677182</v>
+        <v>0.046977115098573941</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>22.01016505878248</v>
+        <v>0.89757528596825875</v>
       </c>
       <c r="B66" s="0">
-        <v>100.00000000000254</v>
+        <v>0</v>
       </c>
       <c r="C66" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D66" s="0">
-        <v>-56928.202313998227</v>
+        <v>0</v>
       </c>
       <c r="E66" s="0">
-        <v>1618.4541013037961</v>
+        <v>0.89757528596825875</v>
       </c>
       <c r="F66" s="0">
-        <v>-110849.04827527556</v>
+        <v>0.052595500344093438</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>24.490530511472393</v>
+        <v>0.90292774296534284</v>
       </c>
       <c r="B67" s="0">
-        <v>125.94134567473044</v>
+        <v>0</v>
       </c>
       <c r="C67" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D67" s="0">
-        <v>-79468.413762547294</v>
+        <v>0</v>
       </c>
       <c r="E67" s="0">
-        <v>2036.1616225579623</v>
+        <v>0.90292774296534284</v>
       </c>
       <c r="F67" s="0">
-        <v>-196417.89505988927</v>
+        <v>0.049774898792216304</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0">
-        <v>24.476335251120368</v>
+        <v>0.90655539049198064</v>
       </c>
       <c r="B68" s="0">
-        <v>125.9291672534882</v>
+        <v>0</v>
       </c>
       <c r="C68" s="0">
-        <v>0.47887972647746396</v>
+        <v>0</v>
       </c>
       <c r="D68" s="0">
-        <v>-79414.673973899087</v>
+        <v>0</v>
       </c>
       <c r="E68" s="0">
-        <v>2036.0451681747234</v>
+        <v>0.90655539049198064</v>
       </c>
       <c r="F68" s="0">
-        <v>-196262.57904355676</v>
+        <v>0.047867976333123896</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>24.492293086119183</v>
+        <v>0.90907417447044669</v>
       </c>
       <c r="B69" s="0">
-        <v>125.99973538556603</v>
+        <v>0</v>
       </c>
       <c r="C69" s="0">
-        <v>0.49095234451052144</v>
+        <v>0</v>
       </c>
       <c r="D69" s="0">
-        <v>-79510.367250789568</v>
+        <v>0</v>
       </c>
       <c r="E69" s="0">
-        <v>2037.1765084783935</v>
+        <v>0.90907417447044669</v>
       </c>
       <c r="F69" s="0">
-        <v>-196614.85270604884</v>
+        <v>0.046546186503799936</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>24.522505081753227</v>
+        <v>0.90616703690410505</v>
       </c>
       <c r="B70" s="0">
-        <v>126.04304056761703</v>
+        <v>0</v>
       </c>
       <c r="C70" s="0">
-        <v>0.49943343039304211</v>
+        <v>0</v>
       </c>
       <c r="D70" s="0">
-        <v>-79635.166086230514</v>
+        <v>0</v>
       </c>
       <c r="E70" s="0">
-        <v>2038.3217428441867</v>
+        <v>0.90616703690410505</v>
       </c>
       <c r="F70" s="0">
-        <v>-197000.34502150188</v>
+        <v>0.048071937117039831</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0">
-        <v>24.534974982673003</v>
+        <v>0.90714770441206061</v>
       </c>
       <c r="B71" s="0">
-        <v>126.04307989342185</v>
+        <v>0</v>
       </c>
       <c r="C71" s="0">
-        <v>0.499943461255208</v>
+        <v>0</v>
       </c>
       <c r="D71" s="0">
-        <v>-79675.523070873911</v>
+        <v>0</v>
       </c>
       <c r="E71" s="0">
-        <v>2038.6003009361543</v>
+        <v>0.90714770441206061</v>
       </c>
       <c r="F71" s="0">
-        <v>-197103.74088587437</v>
+        <v>0.047556981015630218</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>24.527352359731506</v>
+        <v>0.90506657626968401</v>
       </c>
       <c r="B72" s="0">
-        <v>126.04308862311977</v>
+        <v>0</v>
       </c>
       <c r="C72" s="0">
-        <v>0.49533024250316371</v>
+        <v>0</v>
       </c>
       <c r="D72" s="0">
-        <v>-79650.815311664323</v>
+        <v>0</v>
       </c>
       <c r="E72" s="0">
-        <v>2038.5078189457745</v>
+        <v>0.90506657626968401</v>
       </c>
       <c r="F72" s="0">
-        <v>-197040.65091718835</v>
+        <v>0.0486501294110121</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>24.535379716770226</v>
+        <v>0.8995731432781483</v>
       </c>
       <c r="B73" s="0">
-        <v>125.9829438607413</v>
+        <v>0</v>
       </c>
       <c r="C73" s="0">
-        <v>0.49936983007510977</v>
+        <v>0</v>
       </c>
       <c r="D73" s="0">
-        <v>-79639.288367949368</v>
+        <v>0</v>
       </c>
       <c r="E73" s="0">
-        <v>2037.7840449967719</v>
+        <v>0.8995731432781483</v>
       </c>
       <c r="F73" s="0">
-        <v>-196918.87661426121</v>
+        <v>0.051541701877120816</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0">
-        <v>25.962282175168347</v>
+        <v>0.9019267606200787</v>
       </c>
       <c r="B74" s="0">
-        <v>139.92724356070332</v>
+        <v>0</v>
       </c>
       <c r="C74" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D74" s="0">
-        <v>-93461.405669251792</v>
+        <v>0</v>
       </c>
       <c r="E74" s="0">
-        <v>2264.4600439879032</v>
+        <v>0.9019267606200787</v>
       </c>
       <c r="F74" s="0">
-        <v>-257536.07936744922</v>
+        <v>0.05030175286037375</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>25.99997430970501</v>
+        <v>0.90121398436135991</v>
       </c>
       <c r="B75" s="0">
-        <v>139.99572210238904</v>
+        <v>0</v>
       </c>
       <c r="C75" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D75" s="0">
-        <v>-93641.903230557306</v>
+        <v>0</v>
       </c>
       <c r="E75" s="0">
-        <v>2266.2799455757145</v>
+        <v>0.90121398436135991</v>
       </c>
       <c r="F75" s="0">
-        <v>-258173.59189031084</v>
+        <v>0.050677091627216675</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>25.999999762613285</v>
+        <v>0.9057603489978191</v>
       </c>
       <c r="B76" s="0">
-        <v>139.99999902456028</v>
+        <v>0</v>
       </c>
       <c r="C76" s="0">
-        <v>0.42623823501991642</v>
+        <v>0</v>
       </c>
       <c r="D76" s="0">
-        <v>-93643.816654758382</v>
+        <v>0</v>
       </c>
       <c r="E76" s="0">
-        <v>2267.666217508714</v>
+        <v>0.9057603489978191</v>
       </c>
       <c r="F76" s="0">
-        <v>-258189.84794486852</v>
+        <v>0.048285573820686989</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0">
-        <v>25.999999999298375</v>
+        <v>0.89815077478547178</v>
       </c>
       <c r="B77" s="0">
-        <v>139.9999999634727</v>
+        <v>0</v>
       </c>
       <c r="C77" s="0">
-        <v>0.31724978858842579</v>
+        <v>0</v>
       </c>
       <c r="D77" s="0">
-        <v>-93642.33043293556</v>
+        <v>0</v>
       </c>
       <c r="E77" s="0">
-        <v>2269.6258482772923</v>
+        <v>0.89815077478547178</v>
       </c>
       <c r="F77" s="0">
-        <v>-258190.15752375964</v>
+        <v>0.052291830368930592</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>25.999996791855111</v>
+        <v>0.89713736792667031</v>
       </c>
       <c r="B78" s="0">
-        <v>139.99999999174244</v>
+        <v>0</v>
       </c>
       <c r="C78" s="0">
-        <v>0.30503473334623221</v>
+        <v>0</v>
       </c>
       <c r="D78" s="0">
-        <v>-93642.152204969199</v>
+        <v>0</v>
       </c>
       <c r="E78" s="0">
-        <v>2269.845401496078</v>
+        <v>0.89713736792667031</v>
       </c>
       <c r="F78" s="0">
-        <v>-258190.15866071821</v>
+        <v>0.052826643149908703</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>25.999999371342099</v>
+        <v>0.34936952724326742</v>
       </c>
       <c r="B79" s="0">
-        <v>139.98156127054992</v>
+        <v>0</v>
       </c>
       <c r="C79" s="0">
-        <v>0.4966271822521755</v>
+        <v>0</v>
       </c>
       <c r="D79" s="0">
-        <v>-93632.580591941121</v>
+        <v>0</v>
       </c>
       <c r="E79" s="0">
-        <v>2266.1443304457584</v>
+        <v>0.34936952724326742</v>
       </c>
       <c r="F79" s="0">
-        <v>-258121.58590944222</v>
+        <v>0.40892510860021514</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>25.999999890109095</v>
+        <v>0.33774239495684649</v>
       </c>
       <c r="B80" s="0">
-        <v>139.99994823542772</v>
+        <v>0</v>
       </c>
       <c r="C80" s="0">
-        <v>0.43894729928865589</v>
+        <v>0</v>
       </c>
       <c r="D80" s="0">
-        <v>-93643.956997090398</v>
+        <v>0</v>
       </c>
       <c r="E80" s="0">
-        <v>2267.4370055004479</v>
+        <v>0.33774239495684649</v>
       </c>
       <c r="F80" s="0">
-        <v>-258189.62610561858</v>
+        <v>0.41884391515114761</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>25.999997130356387</v>
+        <v>0.34207520414097636</v>
       </c>
       <c r="B81" s="0">
-        <v>139.99998507282064</v>
+        <v>0</v>
       </c>
       <c r="C81" s="0">
-        <v>0.38399714555848585</v>
+        <v>0</v>
       </c>
       <c r="D81" s="0">
-        <v>-93643.221388769191</v>
+        <v>0</v>
       </c>
       <c r="E81" s="0">
-        <v>2268.4254577471725</v>
+        <v>0.34207520414097636</v>
       </c>
       <c r="F81" s="0">
-        <v>-258189.88767595438</v>
+        <v>0.41512804466193087</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>24.561824864841739</v>
+        <v>0.34942659848425695</v>
       </c>
       <c r="B82" s="0">
-        <v>126.14813795049663</v>
+        <v>0</v>
       </c>
       <c r="C82" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D82" s="0">
-        <v>-79827.99751211243</v>
+        <v>0</v>
       </c>
       <c r="E82" s="0">
-        <v>2040.6779441492088</v>
+        <v>0.34942659848425695</v>
       </c>
       <c r="F82" s="0">
-        <v>-197655.50716051663</v>
+        <v>0.40887683306754341</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0">
-        <v>24.539819572276201</v>
+        <v>0.34255351067013445</v>
       </c>
       <c r="B83" s="0">
-        <v>126.04308948967214</v>
+        <v>0</v>
       </c>
       <c r="C83" s="0">
-        <v>0.4930951915640841</v>
+        <v>0</v>
       </c>
       <c r="D83" s="0">
-        <v>-79691.102142452597</v>
+        <v>0</v>
       </c>
       <c r="E83" s="0">
-        <v>2038.8351371116416</v>
+        <v>0.34255351067013445</v>
       </c>
       <c r="F83" s="0">
-        <v>-197143.91154284729</v>
+        <v>0.41471928899874511</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>24.536564521677761</v>
+        <v>0.33808457145448734</v>
       </c>
       <c r="B84" s="0">
-        <v>126.05375092934713</v>
+        <v>0</v>
       </c>
       <c r="C84" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D84" s="0">
-        <v>-79687.325104598247</v>
+        <v>0</v>
       </c>
       <c r="E84" s="0">
-        <v>2038.784218852164</v>
+        <v>0.33808457145448734</v>
       </c>
       <c r="F84" s="0">
-        <v>-197150.31507526236</v>
+        <v>0.4185495967371875</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>24.550846963956413</v>
+        <v>0.34994614211385883</v>
       </c>
       <c r="B85" s="0">
-        <v>126.08290455993628</v>
+        <v>0</v>
       </c>
       <c r="C85" s="0">
-        <v>0.48183560717118606</v>
+        <v>0</v>
       </c>
       <c r="D85" s="0">
-        <v>-79751.476556870941</v>
+        <v>0</v>
       </c>
       <c r="E85" s="0">
-        <v>2039.8449747460927</v>
+        <v>0.34994614211385883</v>
       </c>
       <c r="F85" s="0">
-        <v>-197360.0155075551</v>
+        <v>0.40843754166287827</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0">
-        <v>24.560154658423048</v>
+        <v>0.34673338488791777</v>
       </c>
       <c r="B86" s="0">
-        <v>126.04313508982501</v>
+        <v>0</v>
       </c>
       <c r="C86" s="0">
-        <v>0.49656591979165199</v>
+        <v>0</v>
       </c>
       <c r="D86" s="0">
-        <v>-79756.938143631793</v>
+        <v>0</v>
       </c>
       <c r="E86" s="0">
-        <v>2039.2416842941968</v>
+        <v>0.34673338488791777</v>
       </c>
       <c r="F86" s="0">
-        <v>-197312.4578742185</v>
+        <v>0.41115928733831786</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>24.552687291661318</v>
+        <v>0.34424688826368899</v>
       </c>
       <c r="B87" s="0">
-        <v>126.06559616093703</v>
+        <v>0</v>
       </c>
       <c r="C87" s="0">
-        <v>0.49955303990324595</v>
+        <v>0</v>
       </c>
       <c r="D87" s="0">
-        <v>-79746.860385334381</v>
+        <v>0</v>
       </c>
       <c r="E87" s="0">
-        <v>2039.3282113065247</v>
+        <v>0.34424688826368899</v>
       </c>
       <c r="F87" s="0">
-        <v>-197320.98039840092</v>
+        <v>0.41327443530753749</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>24.540138180366295</v>
+        <v>0.34020569271994738</v>
       </c>
       <c r="B88" s="0">
-        <v>126.0430886299015</v>
+        <v>0</v>
       </c>
       <c r="C88" s="0">
-        <v>0.49163442469247437</v>
+        <v>0</v>
       </c>
       <c r="D88" s="0">
-        <v>-79692.111989417215</v>
+        <v>0</v>
       </c>
       <c r="E88" s="0">
-        <v>2038.8687272934962</v>
+        <v>0.34020569271994738</v>
       </c>
       <c r="F88" s="0">
-        <v>-197146.55142926952</v>
+        <v>0.41672845713171691</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0">
-        <v>24.53655541949168</v>
+        <v>0.34971623603671453</v>
       </c>
       <c r="B89" s="0">
-        <v>126.0430950079688</v>
+        <v>0</v>
       </c>
       <c r="C89" s="0">
-        <v>0.49994210837661363</v>
+        <v>0</v>
       </c>
       <c r="D89" s="0">
-        <v>-79680.643344658514</v>
+        <v>0</v>
       </c>
       <c r="E89" s="0">
-        <v>2038.6369328130484</v>
+        <v>0.34971623603671453</v>
       </c>
       <c r="F89" s="0">
-        <v>-197116.87719236908</v>
+        <v>0.40863189464030569</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>24.536621913989901</v>
+        <v>0.34356680240715459</v>
       </c>
       <c r="B90" s="0">
-        <v>126.07201333717923</v>
+        <v>0</v>
       </c>
       <c r="C90" s="0">
-        <v>0.49992586340198203</v>
+        <v>0</v>
       </c>
       <c r="D90" s="0">
-        <v>-79698.909312898235</v>
+        <v>0</v>
       </c>
       <c r="E90" s="0">
-        <v>2039.0407210420112</v>
+        <v>0.34356680240715459</v>
       </c>
       <c r="F90" s="0">
-        <v>-197207.97519771592</v>
+        <v>0.41385428227517129</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>24.536593258949367</v>
+        <v>0.33703162558921312</v>
       </c>
       <c r="B91" s="0">
-        <v>126.04308862565426</v>
+        <v>0</v>
       </c>
       <c r="C91" s="0">
-        <v>0.49818994837969771</v>
+        <v>0</v>
       </c>
       <c r="D91" s="0">
-        <v>-79680.737809998885</v>
+        <v>0</v>
       </c>
       <c r="E91" s="0">
-        <v>2038.6692193783313</v>
+        <v>0.33703162558921312</v>
       </c>
       <c r="F91" s="0">
-        <v>-197117.17527956513</v>
+        <v>0.41945575053299067</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0">
-        <v>24.536953659401004</v>
+        <v>0.33763632019122658</v>
       </c>
       <c r="B92" s="0">
-        <v>126.04925613106292</v>
+        <v>0</v>
       </c>
       <c r="C92" s="0">
-        <v>0.49986083612657128</v>
+        <v>0</v>
       </c>
       <c r="D92" s="0">
-        <v>-79685.77597088019</v>
+        <v>0</v>
       </c>
       <c r="E92" s="0">
-        <v>2038.7332051642238</v>
+        <v>0.33763632019122658</v>
       </c>
       <c r="F92" s="0">
-        <v>-197139.46543330821</v>
+        <v>0.41893518417372178</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0">
-        <v>24.536557138800749</v>
+        <v>0.3492378164057845</v>
       </c>
       <c r="B93" s="0">
-        <v>126.12237158753652</v>
+        <v>0</v>
       </c>
       <c r="C93" s="0">
-        <v>0.49996822604137581</v>
+        <v>0</v>
       </c>
       <c r="D93" s="0">
-        <v>-79730.134495922597</v>
+        <v>0</v>
       </c>
       <c r="E93" s="0">
-        <v>2039.7384472691151</v>
+        <v>0.3492378164057845</v>
       </c>
       <c r="F93" s="0">
-        <v>-197365.16617737271</v>
+        <v>0.40903653547297492</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0">
-        <v>24.536555624889754</v>
+        <v>0.34703907182940158</v>
       </c>
       <c r="B94" s="0">
-        <v>126.04308862652863</v>
+        <v>0</v>
       </c>
       <c r="C94" s="0">
-        <v>0.4999532461321064</v>
+        <v>0</v>
       </c>
       <c r="D94" s="0">
-        <v>-79680.640177551977</v>
+        <v>0</v>
       </c>
       <c r="E94" s="0">
-        <v>2038.636648584504</v>
+        <v>0.34703907182940158</v>
       </c>
       <c r="F94" s="0">
-        <v>-197116.85888483888</v>
+        <v>0.41089977777172615</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0">
-        <v>25.999996457078737</v>
+        <v>0.33723250723716575</v>
       </c>
       <c r="B95" s="0">
-        <v>139.96387174519316</v>
+        <v>0</v>
       </c>
       <c r="C95" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D95" s="0">
-        <v>-93620.915615242178</v>
+        <v>0</v>
       </c>
       <c r="E95" s="0">
-        <v>2265.8377356647088</v>
+        <v>0.33723250723716575</v>
       </c>
       <c r="F95" s="0">
-        <v>-258056.25704211273</v>
+        <v>0.41928276481822435</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0">
-        <v>25.999996781176378</v>
+        <v>0.34060726467062902</v>
       </c>
       <c r="B96" s="0">
-        <v>139.99998700339299</v>
+        <v>0</v>
       </c>
       <c r="C96" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D96" s="0">
-        <v>-93644.804851521418</v>
+        <v>0</v>
       </c>
       <c r="E96" s="0">
-        <v>2266.339745217655</v>
+        <v>0.34060726467062902</v>
       </c>
       <c r="F96" s="0">
-        <v>-258189.56550271856</v>
+        <v>0.41638431766218875</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0">
-        <v>25.999988812838286</v>
+        <v>0.34860398777353796</v>
       </c>
       <c r="B97" s="0">
-        <v>139.99465315847988</v>
+        <v>0</v>
       </c>
       <c r="C97" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D97" s="0">
-        <v>-93641.248237173844</v>
+        <v>0</v>
       </c>
       <c r="E97" s="0">
-        <v>2266.2654212625366</v>
+        <v>0.34860398777353796</v>
       </c>
       <c r="F97" s="0">
-        <v>-258169.79413855355</v>
+        <v>0.4095730462000079</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0">
-        <v>25.999994854670891</v>
+        <v>0.34810540559322145</v>
       </c>
       <c r="B98" s="0">
-        <v>139.99999303642508</v>
+        <v>0</v>
       </c>
       <c r="C98" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D98" s="0">
-        <v>-93644.801927993729</v>
+        <v>0</v>
       </c>
       <c r="E98" s="0">
-        <v>2266.3397847093797</v>
+        <v>0.34810540559322145</v>
       </c>
       <c r="F98" s="0">
-        <v>-258189.56808651844</v>
+        <v>0.40999541900657965</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0">
-        <v>25.999711047051836</v>
+        <v>0.34827908459968132</v>
       </c>
       <c r="B99" s="0">
-        <v>139.99999998621846</v>
+        <v>0</v>
       </c>
       <c r="C99" s="0">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D99" s="0">
-        <v>-93643.787970538309</v>
+        <v>0</v>
       </c>
       <c r="E99" s="0">
-        <v>2266.3333452220404</v>
+        <v>0.34827908459968132</v>
       </c>
       <c r="F99" s="0">
-        <v>-258186.69341451887</v>
+        <v>0.40984825290466065</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0">
-        <v>25.999996777236678</v>
+        <v>0.34182108347837892</v>
       </c>
       <c r="B100" s="0">
-        <v>139.99999999173951</v>
+        <v>0</v>
       </c>
       <c r="C100" s="0">
-        <v>0.34952280276741265</v>
+        <v>0</v>
       </c>
       <c r="D100" s="0">
-        <v>-93642.759414650907</v>
+        <v>0</v>
       </c>
       <c r="E100" s="0">
-        <v>2269.0455056711817</v>
+        <v>0.34182108347837892</v>
       </c>
       <c r="F100" s="0">
-        <v>-258190.03515117092</v>
+        <v>0.41534532972157068</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0">
-        <v>25.999996791630114</v>
+        <v>0.34950393408721481</v>
       </c>
       <c r="B101" s="0">
-        <v>139.99997325117667</v>
+        <v>0</v>
       </c>
       <c r="C101" s="0">
-        <v>0.36169876463469786</v>
+        <v>0</v>
       </c>
       <c r="D101" s="0">
-        <v>-93642.907980911143</v>
+        <v>0</v>
       </c>
       <c r="E101" s="0">
-        <v>2268.8262105144654</v>
+        <v>0.34950393408721481</v>
       </c>
       <c r="F101" s="0">
-        <v>-258189.90271534762</v>
+        <v>0.4088114225670334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add save functionality to multi-objective optimization runners
Added `save` command to all MO* algorithm runner files (MOABC, MOACO, etc.) to persist workspace data after execution. Updated Optimal.xlsx with new results. The changes ensure optimization results are automatically saved for future reference.
</commit_message>
<xml_diff>
--- a/Optimal.xlsx
+++ b/Optimal.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="78" uniqueCount="7">
   <si>
     <t>X1</t>
   </si>
@@ -85,12 +85,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="true"/>
-    <col min="2" max="2" width="14.5546875" customWidth="true"/>
-    <col min="3" max="3" width="14.5546875" customWidth="true"/>
-    <col min="4" max="4" width="14.5546875" customWidth="true"/>
-    <col min="5" max="5" width="14.5546875" customWidth="true"/>
-    <col min="6" max="6" width="13.5546875" customWidth="true"/>
+    <col min="1" max="1" width="11.5546875" customWidth="true"/>
+    <col min="2" max="2" width="11.5546875" customWidth="true"/>
+    <col min="3" max="3" width="12.5546875" customWidth="true"/>
+    <col min="4" max="4" width="12.21875" customWidth="true"/>
+    <col min="5" max="5" width="11.5546875" customWidth="true"/>
+    <col min="6" max="6" width="12.21875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -104,1013 +104,1013 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.35111972542188447</v>
+        <v>26</v>
       </c>
       <c r="B2" s="0">
-        <v>0</v>
+        <v>111.50537985829369</v>
       </c>
       <c r="C2" s="0">
-        <v>0</v>
+        <v>0.32690292778664165</v>
       </c>
       <c r="D2" s="0">
-        <v>0</v>
+        <v>-74794.980678434076</v>
       </c>
       <c r="E2" s="0">
-        <v>0.35111972542188447</v>
+        <v>1873.3770653886784</v>
       </c>
       <c r="F2" s="0">
-        <v>0.40744643666425862</v>
+        <v>-163713.61519928009</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.65589331251858773</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0">
-        <v>0</v>
+        <v>113.32142911143836</v>
       </c>
       <c r="C3" s="0">
-        <v>0</v>
+        <v>0.33826928731642791</v>
       </c>
       <c r="D3" s="0">
-        <v>0</v>
+        <v>-75996.34344724167</v>
       </c>
       <c r="E3" s="0">
-        <v>0.65589331251858773</v>
+        <v>1898.4157828630439</v>
       </c>
       <c r="F3" s="0">
-        <v>0.19012759491473741</v>
+        <v>-169095.56353565105</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.65597693366699372</v>
+        <v>25.987028270180641</v>
       </c>
       <c r="B4" s="0">
-        <v>0</v>
+        <v>131.8414700683559</v>
       </c>
       <c r="C4" s="0">
-        <v>0</v>
+        <v>0.39197518163517098</v>
       </c>
       <c r="D4" s="0">
-        <v>0</v>
+        <v>-88203.110633269403</v>
       </c>
       <c r="E4" s="0">
-        <v>0.65597693366699372</v>
+        <v>2154.5799812466066</v>
       </c>
       <c r="F4" s="0">
-        <v>0.19007597043488478</v>
+        <v>-228832.81415083623</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.34880903083467485</v>
+        <v>25.960741923814112</v>
       </c>
       <c r="B5" s="0">
-        <v>0</v>
+        <v>112.47659188403132</v>
       </c>
       <c r="C5" s="0">
-        <v>0</v>
+        <v>0.34084085776009038</v>
       </c>
       <c r="D5" s="0">
-        <v>0</v>
+        <v>-75324.164824820327</v>
       </c>
       <c r="E5" s="0">
-        <v>0.34880903083467485</v>
+        <v>1885.7221950709479</v>
       </c>
       <c r="F5" s="0">
-        <v>0.40939943207386364</v>
+        <v>-166322.14711560388</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.69989618528878328</v>
+        <v>25.566435838742741</v>
       </c>
       <c r="B6" s="0">
-        <v>0</v>
+        <v>107.85170971149407</v>
       </c>
       <c r="C6" s="0">
-        <v>0</v>
+        <v>0.33121191859707666</v>
       </c>
       <c r="D6" s="0">
-        <v>0</v>
+        <v>-71176.933366901212</v>
       </c>
       <c r="E6" s="0">
-        <v>0.69989618528878328</v>
+        <v>1812.5285920596377</v>
       </c>
       <c r="F6" s="0">
-        <v>0.16340201692283329</v>
+        <v>-150521.14517632904</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.90919823802307265</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C7" s="0">
-        <v>0</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="D7" s="0">
-        <v>0</v>
+        <v>-56899.335000000006</v>
       </c>
       <c r="E7" s="0">
-        <v>0.90919823802307265</v>
+        <v>1621.816</v>
       </c>
       <c r="F7" s="0">
-        <v>0.046481128648691805</v>
+        <v>-110796.55875900001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.65161580057967938</v>
+        <v>24.500376774307068</v>
       </c>
       <c r="B8" s="0">
-        <v>0</v>
+        <v>100.82513908020285</v>
       </c>
       <c r="C8" s="0">
-        <v>0</v>
+        <v>0.30259883355898065</v>
       </c>
       <c r="D8" s="0">
-        <v>0</v>
+        <v>-63842.864865067197</v>
       </c>
       <c r="E8" s="0">
-        <v>0.65161580057967938</v>
+        <v>1690.822383299721</v>
       </c>
       <c r="F8" s="0">
-        <v>0.19277277016958883</v>
+        <v>-125879.52400896262</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0.64190087281693864</v>
+        <v>24.177483839159212</v>
       </c>
       <c r="B9" s="0">
-        <v>0</v>
+        <v>100.49090689764989</v>
       </c>
       <c r="C9" s="0">
-        <v>0</v>
+        <v>0.30137259089471941</v>
       </c>
       <c r="D9" s="0">
-        <v>0</v>
+        <v>-62800.240809446121</v>
       </c>
       <c r="E9" s="0">
-        <v>0.64190087281693864</v>
+        <v>1678.7623795088832</v>
       </c>
       <c r="F9" s="0">
-        <v>0.19881283533937055</v>
+        <v>-123346.2749032557</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.89526633762802676</v>
+        <v>23.803950205544464</v>
       </c>
       <c r="B10" s="0">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C10" s="0">
-        <v>0</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="D10" s="0">
-        <v>0</v>
+        <v>-61537.814124014418</v>
       </c>
       <c r="E10" s="0">
-        <v>0.89526633762802676</v>
+        <v>1663.360973233689</v>
       </c>
       <c r="F10" s="0">
-        <v>0.053814850239115808</v>
+        <v>-120196.30226442617</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.33306554321145693</v>
+        <v>25.563697421476657</v>
       </c>
       <c r="B11" s="0">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C11" s="0">
-        <v>0</v>
+        <v>0.31158422445065737</v>
       </c>
       <c r="D11" s="0">
-        <v>0</v>
+        <v>-66062.792667532471</v>
       </c>
       <c r="E11" s="0">
-        <v>0.33306554321145693</v>
+        <v>1703.6796672609848</v>
       </c>
       <c r="F11" s="0">
-        <v>0.42288169045553847</v>
+        <v>-129365.68817207748</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.33406842634584977</v>
+        <v>23.826708577564752</v>
       </c>
       <c r="B12" s="0">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C12" s="0">
-        <v>0</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="D12" s="0">
-        <v>0</v>
+        <v>-61596.332498406475</v>
       </c>
       <c r="E12" s="0">
-        <v>0.33406842634584977</v>
+        <v>1663.8850985413162</v>
       </c>
       <c r="F12" s="0">
-        <v>0.42201347217616758</v>
+        <v>-120314.88805406397</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.34318696714917313</v>
+        <v>25.815623266204064</v>
       </c>
       <c r="B13" s="0">
-        <v>0</v>
+        <v>103.64328095698325</v>
       </c>
       <c r="C13" s="0">
-        <v>0</v>
+        <v>0.32145033188879929</v>
       </c>
       <c r="D13" s="0">
-        <v>0</v>
+        <v>-69103.424531349403</v>
       </c>
       <c r="E13" s="0">
-        <v>0.34318696714917313</v>
+        <v>1759.9457321553862</v>
       </c>
       <c r="F13" s="0">
-        <v>0.4141783828253065</v>
+        <v>-140385.7308066074</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.34040288906719829</v>
+        <v>25.582334289548761</v>
       </c>
       <c r="B14" s="0">
-        <v>0</v>
+        <v>107.28065463927706</v>
       </c>
       <c r="C14" s="0">
-        <v>0</v>
+        <v>0.32953095870710175</v>
       </c>
       <c r="D14" s="0">
-        <v>0</v>
+        <v>-70849.314655643335</v>
       </c>
       <c r="E14" s="0">
-        <v>0.34040288906719829</v>
+        <v>1804.9872915367052</v>
       </c>
       <c r="F14" s="0">
-        <v>0.41655943827395903</v>
+        <v>-149024.98483518843</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.34833005575021564</v>
+        <v>24.798152696818768</v>
       </c>
       <c r="B15" s="0">
-        <v>0</v>
+        <v>111.57595562103141</v>
       </c>
       <c r="C15" s="0">
-        <v>0</v>
+        <v>0.33324711547581093</v>
       </c>
       <c r="D15" s="0">
-        <v>0</v>
+        <v>-71397.516167122594</v>
       </c>
       <c r="E15" s="0">
-        <v>0.34833005575021564</v>
+        <v>1846.5654566038179</v>
       </c>
       <c r="F15" s="0">
-        <v>0.40980506970136077</v>
+        <v>-156123.13773936126</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B16" s="0">
-        <v>0</v>
+        <v>123.30949284918394</v>
       </c>
       <c r="C16" s="0">
-        <v>0</v>
+        <v>0.37567513747291126</v>
       </c>
       <c r="D16" s="0">
-        <v>0</v>
+        <v>-82603.358915790741</v>
       </c>
       <c r="E16" s="0">
-        <v>0</v>
+        <v>2036.5773116318937</v>
       </c>
       <c r="F16" s="0">
-        <v>1</v>
+        <v>-200251.44021959158</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.0043447236291691248</v>
+        <v>24.864937625439577</v>
       </c>
       <c r="B17" s="0">
-        <v>0.0043447236291691248</v>
+        <v>102.51610621758296</v>
       </c>
       <c r="C17" s="0">
-        <v>0.0043447236291691248</v>
+        <v>0.30781439044035375</v>
       </c>
       <c r="D17" s="0">
-        <v>0.0043447236291691248</v>
+        <v>-65857.6253799556</v>
       </c>
       <c r="E17" s="0">
-        <v>0.0043447236291691248</v>
+        <v>1722.628887198159</v>
       </c>
       <c r="F17" s="0">
-        <v>0.97191164096186722</v>
+        <v>-132138.92030516063</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.002001831254436902</v>
+        <v>24.79445506498999</v>
       </c>
       <c r="B18" s="0">
-        <v>0.002001831254436902</v>
+        <v>102.11552161774422</v>
       </c>
       <c r="C18" s="0">
-        <v>0.002001831254436902</v>
+        <v>0.30628033121591353</v>
       </c>
       <c r="D18" s="0">
-        <v>0.002001831254436902</v>
+        <v>-65419.184643337234</v>
       </c>
       <c r="E18" s="0">
-        <v>0.002001831254436902</v>
+        <v>1715.4651302781022</v>
       </c>
       <c r="F18" s="0">
-        <v>0.97287340640819575</v>
+        <v>-130724.0694070836</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B19" s="0">
-        <v>0</v>
+        <v>130.24419903431152</v>
       </c>
       <c r="C19" s="0">
-        <v>0</v>
+        <v>0.33797064344440736</v>
       </c>
       <c r="D19" s="0">
-        <v>0</v>
+        <v>-87189.736308538035</v>
       </c>
       <c r="E19" s="0">
-        <v>0</v>
+        <v>2133.6476544077996</v>
       </c>
       <c r="F19" s="0">
-        <v>1</v>
+        <v>-223431.62590128073</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.0015281908463212982</v>
+        <v>26</v>
       </c>
       <c r="B20" s="0">
-        <v>0.0015281908463212982</v>
+        <v>138.77414272964197</v>
       </c>
       <c r="C20" s="0">
-        <v>0.0015281908463212982</v>
+        <v>0.41122209000322812</v>
       </c>
       <c r="D20" s="0">
-        <v>0.0015281908463212982</v>
+        <v>-92832.782148622937</v>
       </c>
       <c r="E20" s="0">
-        <v>0.0015281908463212982</v>
+        <v>2250.8968107637652</v>
       </c>
       <c r="F20" s="0">
-        <v>0.97439372331193363</v>
+        <v>-253684.37360991447</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0</v>
+        <v>25.915869961183937</v>
       </c>
       <c r="B21" s="0">
-        <v>0</v>
+        <v>132.93190402715649</v>
       </c>
       <c r="C21" s="0">
-        <v>0</v>
+        <v>0.39441913127316269</v>
       </c>
       <c r="D21" s="0">
-        <v>0</v>
+        <v>-88681.456586814427</v>
       </c>
       <c r="E21" s="0">
-        <v>0</v>
+        <v>2168.0542952032501</v>
       </c>
       <c r="F21" s="0">
-        <v>1</v>
+        <v>-231981.62771728719</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.001561485075841629</v>
+        <v>26</v>
       </c>
       <c r="B22" s="0">
-        <v>0.001561485075841629</v>
+        <v>132.1863735709251</v>
       </c>
       <c r="C22" s="0">
-        <v>0.001561485075841629</v>
+        <v>0.38014593733343877</v>
       </c>
       <c r="D22" s="0">
-        <v>0.001561485075841629</v>
+        <v>-88474.943926797307</v>
       </c>
       <c r="E22" s="0">
-        <v>0.001561485075841629</v>
+        <v>2159.8855686826037</v>
       </c>
       <c r="F22" s="0">
-        <v>0.97426103983172363</v>
+        <v>-230150.94757436542</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0</v>
+        <v>25.845855019266924</v>
       </c>
       <c r="B23" s="0">
-        <v>0</v>
+        <v>111.98366213217814</v>
       </c>
       <c r="C23" s="0">
-        <v>0</v>
+        <v>0.33936570652243503</v>
       </c>
       <c r="D23" s="0">
-        <v>0</v>
+        <v>-74668.161063478765</v>
       </c>
       <c r="E23" s="0">
-        <v>0</v>
+        <v>1876.25114932772</v>
       </c>
       <c r="F23" s="0">
-        <v>1</v>
+        <v>-164115.08419688541</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0</v>
+        <v>24.765857513254485</v>
       </c>
       <c r="B24" s="0">
-        <v>0</v>
+        <v>101.7271477868814</v>
       </c>
       <c r="C24" s="0">
-        <v>0</v>
+        <v>0.30499133694368913</v>
       </c>
       <c r="D24" s="0">
-        <v>0</v>
+        <v>-65099.402987098809</v>
       </c>
       <c r="E24" s="0">
-        <v>0</v>
+        <v>1709.4313085296549</v>
       </c>
       <c r="F24" s="0">
-        <v>1</v>
+        <v>-129576.21547100264</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.69654416215177661</v>
+        <v>25.012791437279049</v>
       </c>
       <c r="B25" s="0">
-        <v>0</v>
+        <v>102.97922589063948</v>
       </c>
       <c r="C25" s="0">
-        <v>0</v>
+        <v>0.30887245424145116</v>
       </c>
       <c r="D25" s="0">
-        <v>0</v>
+        <v>-66541.973752512058</v>
       </c>
       <c r="E25" s="0">
-        <v>0.69654416215177661</v>
+        <v>1732.4522999531641</v>
       </c>
       <c r="F25" s="0">
-        <v>0.16540778690921365</v>
+        <v>-134153.97332683054</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0.68575193911563925</v>
+        <v>26</v>
       </c>
       <c r="B26" s="0">
-        <v>0</v>
+        <v>133.57373607811664</v>
       </c>
       <c r="C26" s="0">
-        <v>0</v>
+        <v>0.39629949482921134</v>
       </c>
       <c r="D26" s="0">
-        <v>0</v>
+        <v>-89392.821479613907</v>
       </c>
       <c r="E26" s="0">
-        <v>0.68575193911563925</v>
+        <v>2178.8794665687924</v>
       </c>
       <c r="F26" s="0">
-        <v>0.17189859370024052</v>
+        <v>-235011.78219299499</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>0.69401962525650907</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0">
-        <v>0</v>
+        <v>123.30949284918394</v>
       </c>
       <c r="C27" s="0">
-        <v>0</v>
+        <v>0.37567513747291126</v>
       </c>
       <c r="D27" s="0">
-        <v>0</v>
+        <v>-82603.358915790741</v>
       </c>
       <c r="E27" s="0">
-        <v>0.69401962525650907</v>
+        <v>2036.5773116318937</v>
       </c>
       <c r="F27" s="0">
-        <v>0.16692159717316579</v>
+        <v>-200251.44021959158</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.69630329468485364</v>
+        <v>25.776098036283138</v>
       </c>
       <c r="B28" s="0">
-        <v>0</v>
+        <v>121.82984473593753</v>
       </c>
       <c r="C28" s="0">
-        <v>0</v>
+        <v>0.3712746464380256</v>
       </c>
       <c r="D28" s="0">
-        <v>0</v>
+        <v>-80924.539285330844</v>
       </c>
       <c r="E28" s="0">
-        <v>0.69630329468485364</v>
+        <v>2010.9328614621766</v>
       </c>
       <c r="F28" s="0">
-        <v>0.16555210187522573</v>
+        <v>-193737.50684555239</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>0.69799975288468197</v>
+        <v>24.79445506498999</v>
       </c>
       <c r="B29" s="0">
-        <v>0</v>
+        <v>102.11552161774422</v>
       </c>
       <c r="C29" s="0">
-        <v>0</v>
+        <v>0.30628033121591353</v>
       </c>
       <c r="D29" s="0">
-        <v>0</v>
+        <v>-65419.184643337234</v>
       </c>
       <c r="E29" s="0">
-        <v>0.69799975288468197</v>
+        <v>1715.4651302781022</v>
       </c>
       <c r="F29" s="0">
-        <v>0.16453620492286924</v>
+        <v>-130724.0694070836</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0.69602368563235983</v>
+        <v>25.767914613404095</v>
       </c>
       <c r="B30" s="0">
-        <v>0</v>
+        <v>127.41696352722077</v>
       </c>
       <c r="C30" s="0">
-        <v>0</v>
+        <v>0.37868427977654806</v>
       </c>
       <c r="D30" s="0">
-        <v>0</v>
+        <v>-84561.609893981178</v>
       </c>
       <c r="E30" s="0">
-        <v>0.69602368563235983</v>
+        <v>2088.2721232246827</v>
       </c>
       <c r="F30" s="0">
-        <v>0.16571966004684024</v>
+        <v>-211863.63612588128</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.34655927979443407</v>
+        <v>24.817629338758014</v>
       </c>
       <c r="B31" s="0">
-        <v>0</v>
+        <v>102.2077490209733</v>
       </c>
       <c r="C31" s="0">
-        <v>0</v>
+        <v>0.30655789681123063</v>
       </c>
       <c r="D31" s="0">
-        <v>0</v>
+        <v>-65538.252162259829</v>
       </c>
       <c r="E31" s="0">
-        <v>0.34655927979443407</v>
+        <v>1717.2758040784599</v>
       </c>
       <c r="F31" s="0">
-        <v>0.41130714307507177</v>
+        <v>-131086.73763638426</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.34378784919656452</v>
+        <v>24.091446215109514</v>
       </c>
       <c r="B32" s="0">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C32" s="0">
-        <v>0</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="D32" s="0">
-        <v>0</v>
+        <v>-62277.049738448943</v>
       </c>
       <c r="E32" s="0">
-        <v>0.34378784919656452</v>
+        <v>1669.9820063339721</v>
       </c>
       <c r="F32" s="0">
-        <v>0.41366575300724207</v>
+        <v>-121694.3418114376</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.33855770850549949</v>
+        <v>25.960741923814112</v>
       </c>
       <c r="B33" s="0">
-        <v>0</v>
+        <v>112.47659188403132</v>
       </c>
       <c r="C33" s="0">
-        <v>0</v>
+        <v>0.34084085776009038</v>
       </c>
       <c r="D33" s="0">
-        <v>0</v>
+        <v>-75324.164824820327</v>
       </c>
       <c r="E33" s="0">
-        <v>0.33855770850549949</v>
+        <v>1885.7221950709479</v>
       </c>
       <c r="F33" s="0">
-        <v>0.41814287964698804</v>
+        <v>-166322.14711560388</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.34663656299847695</v>
+        <v>26</v>
       </c>
       <c r="B34" s="0">
-        <v>0</v>
+        <v>133.57373607811664</v>
       </c>
       <c r="C34" s="0">
-        <v>0</v>
+        <v>0.39629949482921134</v>
       </c>
       <c r="D34" s="0">
-        <v>0</v>
+        <v>-89392.821479613907</v>
       </c>
       <c r="E34" s="0">
-        <v>0.34663656299847695</v>
+        <v>2178.8794665687924</v>
       </c>
       <c r="F34" s="0">
-        <v>0.41124150706891971</v>
+        <v>-235011.78219299499</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>0.34936247946518817</v>
+        <v>24.79445506498999</v>
       </c>
       <c r="B35" s="0">
-        <v>0</v>
+        <v>102.11552161774422</v>
       </c>
       <c r="C35" s="0">
-        <v>0</v>
+        <v>0.30628033121591353</v>
       </c>
       <c r="D35" s="0">
-        <v>0</v>
+        <v>-65419.184643337234</v>
       </c>
       <c r="E35" s="0">
-        <v>0.34936247946518817</v>
+        <v>1715.4651302781022</v>
       </c>
       <c r="F35" s="0">
-        <v>0.40893107046200761</v>
+        <v>-130724.0694070836</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.3415260661866808</v>
+        <v>26</v>
       </c>
       <c r="B36" s="0">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="C36" s="0">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D36" s="0">
-        <v>0</v>
+        <v>-93644.825000000012</v>
       </c>
       <c r="E36" s="0">
-        <v>0.3415260661866808</v>
+        <v>2266.3400000000001</v>
       </c>
       <c r="F36" s="0">
-        <v>0.41559768464979474</v>
+        <v>-258189.64637499998</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.34598725948272285</v>
+        <v>25.960741923814112</v>
       </c>
       <c r="B37" s="0">
-        <v>0</v>
+        <v>112.47659188403132</v>
       </c>
       <c r="C37" s="0">
-        <v>0</v>
+        <v>0.34084085776009038</v>
       </c>
       <c r="D37" s="0">
-        <v>0</v>
+        <v>-75324.164824820327</v>
       </c>
       <c r="E37" s="0">
-        <v>0.34598725948272285</v>
+        <v>1885.7221950709479</v>
       </c>
       <c r="F37" s="0">
-        <v>0.41179318307016977</v>
+        <v>-166322.14711560388</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>0.35205596799481542</v>
+        <v>26</v>
       </c>
       <c r="B38" s="0">
-        <v>0</v>
+        <v>123.11652984719713</v>
       </c>
       <c r="C38" s="0">
-        <v>0</v>
+        <v>0.37515673832248242</v>
       </c>
       <c r="D38" s="0">
-        <v>0</v>
+        <v>-82475.71839160817</v>
       </c>
       <c r="E38" s="0">
-        <v>0.35205596799481542</v>
+        <v>2033.9044467210019</v>
       </c>
       <c r="F38" s="0">
-        <v>0.40665695588907813</v>
+        <v>-199624.5880938386</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0.34466031261491942</v>
+        <v>25.181779988745912</v>
       </c>
       <c r="B39" s="0">
-        <v>0</v>
+        <v>105.66993167323744</v>
       </c>
       <c r="C39" s="0">
-        <v>0</v>
+        <v>0.31817692700808514</v>
       </c>
       <c r="D39" s="0">
-        <v>0</v>
+        <v>-68713.159228639866</v>
       </c>
       <c r="E39" s="0">
-        <v>0.34466031261491942</v>
+        <v>1773.5776222512134</v>
       </c>
       <c r="F39" s="0">
-        <v>0.41292222609357843</v>
+        <v>-142247.86853350193</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>0.35083979080507582</v>
+        <v>25.957240843969895</v>
       </c>
       <c r="B40" s="0">
-        <v>0</v>
+        <v>111.35903950289826</v>
       </c>
       <c r="C40" s="0">
-        <v>0</v>
+        <v>0.33888943031255864</v>
       </c>
       <c r="D40" s="0">
-        <v>0</v>
+        <v>-74576.046456356053</v>
       </c>
       <c r="E40" s="0">
-        <v>0.35083979080507582</v>
+        <v>1870.1426737698928</v>
       </c>
       <c r="F40" s="0">
-        <v>0.40768269415365233</v>
+        <v>-163007.32509880053</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>0.34999932587935478</v>
+        <v>24.817629338758014</v>
       </c>
       <c r="B41" s="0">
-        <v>0</v>
+        <v>102.2077490209733</v>
       </c>
       <c r="C41" s="0">
-        <v>0</v>
+        <v>0.30655789681123063</v>
       </c>
       <c r="D41" s="0">
-        <v>0</v>
+        <v>-65538.252162259829</v>
       </c>
       <c r="E41" s="0">
-        <v>0.34999932587935478</v>
+        <v>1717.2758040784599</v>
       </c>
       <c r="F41" s="0">
-        <v>0.40839259142624429</v>
+        <v>-131086.73763638426</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0.3457932131387435</v>
+        <v>26</v>
       </c>
       <c r="B42" s="0">
-        <v>0</v>
+        <v>114.5167257643447</v>
       </c>
       <c r="C42" s="0">
-        <v>0</v>
+        <v>0.34266584072727874</v>
       </c>
       <c r="D42" s="0">
-        <v>0</v>
+        <v>-76787.020478294085</v>
       </c>
       <c r="E42" s="0">
-        <v>0.3457932131387435</v>
+        <v>1914.9513563081148</v>
       </c>
       <c r="F42" s="0">
-        <v>0.41195815358195509</v>
+        <v>-172685.38568964577</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>0.35276063938407665</v>
+        <v>26</v>
       </c>
       <c r="B43" s="0">
-        <v>0</v>
+        <v>133.57373607811664</v>
       </c>
       <c r="C43" s="0">
-        <v>0</v>
+        <v>0.39629949482921134</v>
       </c>
       <c r="D43" s="0">
-        <v>0</v>
+        <v>-89392.821479613907</v>
       </c>
       <c r="E43" s="0">
-        <v>0.35276063938407665</v>
+        <v>2178.8794665687924</v>
       </c>
       <c r="F43" s="0">
-        <v>0.40606343824944013</v>
+        <v>-235011.78219299499</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>0.34539046257451989</v>
+        <v>25.859367647961051</v>
       </c>
       <c r="B44" s="0">
-        <v>0</v>
+        <v>121.11310880263503</v>
       </c>
       <c r="C44" s="0">
-        <v>0</v>
+        <v>0.36496630110841599</v>
       </c>
       <c r="D44" s="0">
-        <v>0</v>
+        <v>-80713.293820300692</v>
       </c>
       <c r="E44" s="0">
-        <v>0.34539046257451989</v>
+        <v>2003.0013551952406</v>
       </c>
       <c r="F44" s="0">
-        <v>0.41230070395267626</v>
+        <v>-192099.13219150651</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>0.35560455712434796</v>
+        <v>26</v>
       </c>
       <c r="B45" s="0">
-        <v>0</v>
+        <v>113.32142911143836</v>
       </c>
       <c r="C45" s="0">
-        <v>0</v>
+        <v>0.33826928731642791</v>
       </c>
       <c r="D45" s="0">
-        <v>0</v>
+        <v>-75996.34344724167</v>
       </c>
       <c r="E45" s="0">
-        <v>0.35560455712434796</v>
+        <v>1898.4157828630439</v>
       </c>
       <c r="F45" s="0">
-        <v>0.40367411835109157</v>
+        <v>-169095.56353565105</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>0.35389116415478028</v>
+        <v>25.691832909059549</v>
       </c>
       <c r="B46" s="0">
-        <v>0</v>
+        <v>110.13068715013875</v>
       </c>
       <c r="C46" s="0">
-        <v>0</v>
+        <v>0.33283338490613107</v>
       </c>
       <c r="D46" s="0">
-        <v>0</v>
+        <v>-73013.975659789488</v>
       </c>
       <c r="E46" s="0">
-        <v>0.35389116415478028</v>
+        <v>1847.065119021958</v>
       </c>
       <c r="F46" s="0">
-        <v>0.40511247772811687</v>
+        <v>-157749.50871127206</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>0.35085091672272645</v>
+        <v>26</v>
       </c>
       <c r="B47" s="0">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="C47" s="0">
-        <v>0</v>
+        <v>0.44745101610300025</v>
       </c>
       <c r="D47" s="0">
-        <v>0</v>
+        <v>-93644.107706369818</v>
       </c>
       <c r="E47" s="0">
-        <v>0.35085091672272645</v>
+        <v>2267.284830730468</v>
       </c>
       <c r="F47" s="0">
-        <v>0.40767330237213983</v>
+        <v>-258189.79444044639</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0.34705661811303751</v>
+        <v>26</v>
       </c>
       <c r="B48" s="0">
-        <v>0</v>
+        <v>123.31084830966549</v>
       </c>
       <c r="C48" s="0">
-        <v>0</v>
+        <v>0.37553192511996231</v>
       </c>
       <c r="D48" s="0">
-        <v>0</v>
+        <v>-82604.253516723038</v>
       </c>
       <c r="E48" s="0">
-        <v>0.34705661811303751</v>
+        <v>2036.5987274906934</v>
       </c>
       <c r="F48" s="0">
-        <v>0.41088488551638946</v>
+        <v>-200255.84740080024</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0.34751466731022956</v>
+        <v>26</v>
       </c>
       <c r="B49" s="0">
-        <v>0</v>
+        <v>118.77298393747444</v>
       </c>
       <c r="C49" s="0">
-        <v>0</v>
+        <v>0.36598003414542912</v>
       </c>
       <c r="D49" s="0">
-        <v>0</v>
+        <v>-79602.598123069183</v>
       </c>
       <c r="E49" s="0">
-        <v>0.34751466731022956</v>
+        <v>1973.6941557169598</v>
       </c>
       <c r="F49" s="0">
-        <v>0.41049625335352657</v>
+        <v>-185774.30962561115</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>0.64236967302922965</v>
+        <v>24.723423560383161</v>
       </c>
       <c r="B50" s="0">
-        <v>0</v>
+        <v>101.84793273510381</v>
       </c>
       <c r="C50" s="0">
-        <v>0</v>
+        <v>0.3054784271146076</v>
       </c>
       <c r="D50" s="0">
-        <v>0</v>
+        <v>-65064.404518571726</v>
       </c>
       <c r="E50" s="0">
-        <v>0.64236967302922965</v>
+        <v>1710.1242074940467</v>
       </c>
       <c r="F50" s="0">
-        <v>0.19852032275969111</v>
+        <v>-129655.10259269616</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>0.63895266568810838</v>
+        <v>24.703260632614182</v>
       </c>
       <c r="B51" s="0">
-        <v>0</v>
+        <v>101.80556777788125</v>
       </c>
       <c r="C51" s="0">
-        <v>0</v>
+        <v>0.30534196982274092</v>
       </c>
       <c r="D51" s="0">
-        <v>0</v>
+        <v>-64984.985736112882</v>
       </c>
       <c r="E51" s="0">
-        <v>0.63895266568810838</v>
+        <v>1709.0734358642412</v>
       </c>
       <c r="F51" s="0">
-        <v>0.20065485196436683</v>
+        <v>-129438.2389502852</v>
       </c>
     </row>
     <row r="52">

</xml_diff>

<commit_message>
Refactor MOTLB algorithm and simplify plotting functions
- Rename MOTlb to MOTLB for consistency across all files
- Fix callback_outputs reference in myFitness.m
- Simplify plotChart.m by removing redundant figures and consolidating plotting logic
- Remove old plotChart_old and add plotChart_new
- Update Optimal.xlsx with latest results

The changes improve code consistency and maintainability while reducing redundant plotting functionality.
</commit_message>
<xml_diff>
--- a/Optimal.xlsx
+++ b/Optimal.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="78" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="84" uniqueCount="7">
   <si>
     <t>X1</t>
   </si>
@@ -115,1002 +115,1002 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>26</v>
+        <v>24.470486141913241</v>
       </c>
       <c r="B2" s="0">
-        <v>111.50537985829369</v>
+        <v>108.85339849603808</v>
       </c>
       <c r="C2" s="0">
-        <v>0.32690292778664165</v>
+        <v>0.4709111763710514</v>
       </c>
       <c r="D2" s="0">
-        <v>-74794.980678434076</v>
+        <v>-68765.503044241661</v>
       </c>
       <c r="E2" s="0">
-        <v>1873.3770653886784</v>
+        <v>1798.7005519920397</v>
       </c>
       <c r="F2" s="0">
-        <v>-163713.61519928009</v>
+        <v>-146565.13893950562</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>26</v>
+        <v>25.919392196733387</v>
       </c>
       <c r="B3" s="0">
-        <v>113.32142911143836</v>
+        <v>127.72560980531588</v>
       </c>
       <c r="C3" s="0">
-        <v>0.33826928731642791</v>
+        <v>0.41509101354197586</v>
       </c>
       <c r="D3" s="0">
-        <v>-75996.34344724167</v>
+        <v>-85260.771434765455</v>
       </c>
       <c r="E3" s="0">
-        <v>1898.4157828630439</v>
+        <v>2095.3962421611759</v>
       </c>
       <c r="F3" s="0">
-        <v>-169095.56353565105</v>
+        <v>-214180.42323207686</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>25.987028270180641</v>
+        <v>25.618553385370983</v>
       </c>
       <c r="B4" s="0">
-        <v>131.8414700683559</v>
+        <v>135.93147780256623</v>
       </c>
       <c r="C4" s="0">
-        <v>0.39197518163517098</v>
+        <v>0.42718729788386356</v>
       </c>
       <c r="D4" s="0">
-        <v>-88203.110633269403</v>
+        <v>-89623.258790606706</v>
       </c>
       <c r="E4" s="0">
-        <v>2154.5799812466066</v>
+        <v>2202.3119983048127</v>
       </c>
       <c r="F4" s="0">
-        <v>-228832.81415083623</v>
+        <v>-239714.30125701483</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>25.960741923814112</v>
+        <v>25.756368310454423</v>
       </c>
       <c r="B5" s="0">
-        <v>112.47659188403132</v>
+        <v>121.84677821758635</v>
       </c>
       <c r="C5" s="0">
-        <v>0.34084085776009038</v>
+        <v>0.39548545565116999</v>
       </c>
       <c r="D5" s="0">
-        <v>-75324.164824820327</v>
+        <v>-80874.27751679653</v>
       </c>
       <c r="E5" s="0">
-        <v>1885.7221950709479</v>
+        <v>2010.2785509216076</v>
       </c>
       <c r="F5" s="0">
-        <v>-166322.14711560388</v>
+        <v>-193638.66185013676</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>25.566435838742741</v>
+        <v>25.8829071834597</v>
       </c>
       <c r="B6" s="0">
-        <v>107.85170971149407</v>
+        <v>129.69797905839431</v>
       </c>
       <c r="C6" s="0">
-        <v>0.33121191859707666</v>
+        <v>0.39870977931111495</v>
       </c>
       <c r="D6" s="0">
-        <v>-71176.933366901212</v>
+        <v>-86439.72850348652</v>
       </c>
       <c r="E6" s="0">
-        <v>1812.5285920596377</v>
+        <v>2122.2664595147444</v>
       </c>
       <c r="F6" s="0">
-        <v>-150521.14517632904</v>
+        <v>-220532.75096585695</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>22</v>
+        <v>25.618553385370983</v>
       </c>
       <c r="B7" s="0">
-        <v>100</v>
+        <v>135.93147780256623</v>
       </c>
       <c r="C7" s="0">
-        <v>0.29999999999999999</v>
+        <v>0.42718729788386356</v>
       </c>
       <c r="D7" s="0">
-        <v>-56899.335000000006</v>
+        <v>-89623.258790606706</v>
       </c>
       <c r="E7" s="0">
-        <v>1621.816</v>
+        <v>2202.3119983048127</v>
       </c>
       <c r="F7" s="0">
-        <v>-110796.55875900001</v>
+        <v>-239714.30125701483</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>24.500376774307068</v>
+        <v>25.682593715061952</v>
       </c>
       <c r="B8" s="0">
-        <v>100.82513908020285</v>
+        <v>111.96927201492835</v>
       </c>
       <c r="C8" s="0">
-        <v>0.30259883355898065</v>
+        <v>0.37641414892540781</v>
       </c>
       <c r="D8" s="0">
-        <v>-63842.864865067197</v>
+        <v>-74189.700060444899</v>
       </c>
       <c r="E8" s="0">
-        <v>1690.822383299721</v>
+        <v>1871.625087867702</v>
       </c>
       <c r="F8" s="0">
-        <v>-125879.52400896262</v>
+        <v>-163005.97822984413</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>24.177483839159212</v>
+        <v>25.605704878238168</v>
       </c>
       <c r="B9" s="0">
-        <v>100.49090689764989</v>
+        <v>110.92928128259632</v>
       </c>
       <c r="C9" s="0">
-        <v>0.30137259089471941</v>
+        <v>0.36817208146373365</v>
       </c>
       <c r="D9" s="0">
-        <v>-62800.240809446121</v>
+        <v>-73291.01208007583</v>
       </c>
       <c r="E9" s="0">
-        <v>1678.7623795088832</v>
+        <v>1855.5466591491959</v>
       </c>
       <c r="F9" s="0">
-        <v>-123346.2749032557</v>
+        <v>-159495.65984129821</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>23.803950205544464</v>
+        <v>25.553579504126002</v>
       </c>
       <c r="B10" s="0">
-        <v>100</v>
+        <v>131.65851548025063</v>
       </c>
       <c r="C10" s="0">
-        <v>0.29999999999999999</v>
+        <v>0.33946165360563119</v>
       </c>
       <c r="D10" s="0">
-        <v>-61537.814124014418</v>
+        <v>-86617.821795030744</v>
       </c>
       <c r="E10" s="0">
-        <v>1663.360973233689</v>
+        <v>2142.9987806236763</v>
       </c>
       <c r="F10" s="0">
-        <v>-120196.30226442617</v>
+        <v>-224280.67094260713</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>25.563697421476657</v>
+        <v>24.470486141913241</v>
       </c>
       <c r="B11" s="0">
-        <v>100</v>
+        <v>108.85339849603808</v>
       </c>
       <c r="C11" s="0">
-        <v>0.31158422445065737</v>
+        <v>0.4709111763710514</v>
       </c>
       <c r="D11" s="0">
-        <v>-66062.792667532471</v>
+        <v>-68765.503044241661</v>
       </c>
       <c r="E11" s="0">
-        <v>1703.6796672609848</v>
+        <v>1798.7005519920397</v>
       </c>
       <c r="F11" s="0">
-        <v>-129365.68817207748</v>
+        <v>-146565.13893950562</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>23.826708577564752</v>
+        <v>25.750689346546043</v>
       </c>
       <c r="B12" s="0">
-        <v>100</v>
+        <v>117.40611967378695</v>
       </c>
       <c r="C12" s="0">
-        <v>0.29999999999999999</v>
+        <v>0.47900716724525155</v>
       </c>
       <c r="D12" s="0">
-        <v>-61596.332498406475</v>
+        <v>-77948.594584322869</v>
       </c>
       <c r="E12" s="0">
-        <v>1663.8850985413162</v>
+        <v>1946.9208902495245</v>
       </c>
       <c r="F12" s="0">
-        <v>-120314.88805406397</v>
+        <v>-179727.20098407147</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>25.815623266204064</v>
+        <v>25.8829071834597</v>
       </c>
       <c r="B13" s="0">
-        <v>103.64328095698325</v>
+        <v>129.69797905839431</v>
       </c>
       <c r="C13" s="0">
-        <v>0.32145033188879929</v>
+        <v>0.39870977931111495</v>
       </c>
       <c r="D13" s="0">
-        <v>-69103.424531349403</v>
+        <v>-86439.72850348652</v>
       </c>
       <c r="E13" s="0">
-        <v>1759.9457321553862</v>
+        <v>2122.2664595147444</v>
       </c>
       <c r="F13" s="0">
-        <v>-140385.7308066074</v>
+        <v>-220532.75096585695</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>25.582334289548761</v>
+        <v>25.919392196733387</v>
       </c>
       <c r="B14" s="0">
-        <v>107.28065463927706</v>
+        <v>127.72560980531588</v>
       </c>
       <c r="C14" s="0">
-        <v>0.32953095870710175</v>
+        <v>0.41509101354197586</v>
       </c>
       <c r="D14" s="0">
-        <v>-70849.314655643335</v>
+        <v>-85260.771434765455</v>
       </c>
       <c r="E14" s="0">
-        <v>1804.9872915367052</v>
+        <v>2095.3962421611759</v>
       </c>
       <c r="F14" s="0">
-        <v>-149024.98483518843</v>
+        <v>-214180.42323207686</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>24.798152696818768</v>
+        <v>25.682593715061952</v>
       </c>
       <c r="B15" s="0">
-        <v>111.57595562103141</v>
+        <v>111.96927201492835</v>
       </c>
       <c r="C15" s="0">
-        <v>0.33324711547581093</v>
+        <v>0.37641414892540781</v>
       </c>
       <c r="D15" s="0">
-        <v>-71397.516167122594</v>
+        <v>-74189.700060444899</v>
       </c>
       <c r="E15" s="0">
-        <v>1846.5654566038179</v>
+        <v>1871.625087867702</v>
       </c>
       <c r="F15" s="0">
-        <v>-156123.13773936126</v>
+        <v>-163005.97822984413</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>26</v>
+        <v>25.605704878238168</v>
       </c>
       <c r="B16" s="0">
-        <v>123.30949284918394</v>
+        <v>110.92928128259632</v>
       </c>
       <c r="C16" s="0">
-        <v>0.37567513747291126</v>
+        <v>0.36817208146373365</v>
       </c>
       <c r="D16" s="0">
-        <v>-82603.358915790741</v>
+        <v>-73291.01208007583</v>
       </c>
       <c r="E16" s="0">
-        <v>2036.5773116318937</v>
+        <v>1855.5466591491959</v>
       </c>
       <c r="F16" s="0">
-        <v>-200251.44021959158</v>
+        <v>-159495.65984129821</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>24.864937625439577</v>
+        <v>25.682593715061952</v>
       </c>
       <c r="B17" s="0">
-        <v>102.51610621758296</v>
+        <v>111.96927201492835</v>
       </c>
       <c r="C17" s="0">
-        <v>0.30781439044035375</v>
+        <v>0.37641414892540781</v>
       </c>
       <c r="D17" s="0">
-        <v>-65857.6253799556</v>
+        <v>-74189.700060444899</v>
       </c>
       <c r="E17" s="0">
-        <v>1722.628887198159</v>
+        <v>1871.625087867702</v>
       </c>
       <c r="F17" s="0">
-        <v>-132138.92030516063</v>
+        <v>-163005.97822984413</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>24.79445506498999</v>
+        <v>24.470486141913241</v>
       </c>
       <c r="B18" s="0">
-        <v>102.11552161774422</v>
+        <v>108.85339849603808</v>
       </c>
       <c r="C18" s="0">
-        <v>0.30628033121591353</v>
+        <v>0.4709111763710514</v>
       </c>
       <c r="D18" s="0">
-        <v>-65419.184643337234</v>
+        <v>-68765.503044241661</v>
       </c>
       <c r="E18" s="0">
-        <v>1715.4651302781022</v>
+        <v>1798.7005519920397</v>
       </c>
       <c r="F18" s="0">
-        <v>-130724.0694070836</v>
+        <v>-146565.13893950562</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>26</v>
+        <v>25.556305370846339</v>
       </c>
       <c r="B19" s="0">
-        <v>130.24419903431152</v>
+        <v>114.57979332813709</v>
       </c>
       <c r="C19" s="0">
-        <v>0.33797064344440736</v>
+        <v>0.31515895258397691</v>
       </c>
       <c r="D19" s="0">
-        <v>-87189.736308538035</v>
+        <v>-75522.922106385318</v>
       </c>
       <c r="E19" s="0">
-        <v>2133.6476544077996</v>
+        <v>1906.1042819842369</v>
       </c>
       <c r="F19" s="0">
-        <v>-223431.62590128073</v>
+        <v>-169839.82536300496</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>26</v>
+        <v>25.605704878238168</v>
       </c>
       <c r="B20" s="0">
-        <v>138.77414272964197</v>
+        <v>110.92928128259632</v>
       </c>
       <c r="C20" s="0">
-        <v>0.41122209000322812</v>
+        <v>0.36817208146373365</v>
       </c>
       <c r="D20" s="0">
-        <v>-92832.782148622937</v>
+        <v>-73291.01208007583</v>
       </c>
       <c r="E20" s="0">
-        <v>2250.8968107637652</v>
+        <v>1855.5466591491959</v>
       </c>
       <c r="F20" s="0">
-        <v>-253684.37360991447</v>
+        <v>-159495.65984129821</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>25.915869961183937</v>
+        <v>25.756368310454423</v>
       </c>
       <c r="B21" s="0">
-        <v>132.93190402715649</v>
+        <v>121.84677821758635</v>
       </c>
       <c r="C21" s="0">
-        <v>0.39441913127316269</v>
+        <v>0.39548545565116999</v>
       </c>
       <c r="D21" s="0">
-        <v>-88681.456586814427</v>
+        <v>-80874.27751679653</v>
       </c>
       <c r="E21" s="0">
-        <v>2168.0542952032501</v>
+        <v>2010.2785509216076</v>
       </c>
       <c r="F21" s="0">
-        <v>-231981.62771728719</v>
+        <v>-193638.66185013676</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>26</v>
+        <v>25.919392196733387</v>
       </c>
       <c r="B22" s="0">
-        <v>132.1863735709251</v>
+        <v>127.72560980531588</v>
       </c>
       <c r="C22" s="0">
-        <v>0.38014593733343877</v>
+        <v>0.41509101354197586</v>
       </c>
       <c r="D22" s="0">
-        <v>-88474.943926797307</v>
+        <v>-85260.771434765455</v>
       </c>
       <c r="E22" s="0">
-        <v>2159.8855686826037</v>
+        <v>2095.3962421611759</v>
       </c>
       <c r="F22" s="0">
-        <v>-230150.94757436542</v>
+        <v>-214180.42323207686</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>25.845855019266924</v>
+        <v>24.470486141913241</v>
       </c>
       <c r="B23" s="0">
-        <v>111.98366213217814</v>
+        <v>108.85339849603808</v>
       </c>
       <c r="C23" s="0">
-        <v>0.33936570652243503</v>
+        <v>0.4709111763710514</v>
       </c>
       <c r="D23" s="0">
-        <v>-74668.161063478765</v>
+        <v>-68765.503044241661</v>
       </c>
       <c r="E23" s="0">
-        <v>1876.25114932772</v>
+        <v>1798.7005519920397</v>
       </c>
       <c r="F23" s="0">
-        <v>-164115.08419688541</v>
+        <v>-146565.13893950562</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>24.765857513254485</v>
+        <v>24.453876449612522</v>
       </c>
       <c r="B24" s="0">
-        <v>101.7271477868814</v>
+        <v>100.89878945382742</v>
       </c>
       <c r="C24" s="0">
-        <v>0.30499133694368913</v>
+        <v>0.38677470788105578</v>
       </c>
       <c r="D24" s="0">
-        <v>-65099.402987098809</v>
+        <v>-63769.290317293096</v>
       </c>
       <c r="E24" s="0">
-        <v>1709.4313085296549</v>
+        <v>1689.2617387950761</v>
       </c>
       <c r="F24" s="0">
-        <v>-129576.21547100264</v>
+        <v>-125816.82017019449</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>25.012791437279049</v>
+        <v>25.605704878238168</v>
       </c>
       <c r="B25" s="0">
-        <v>102.97922589063948</v>
+        <v>110.92928128259632</v>
       </c>
       <c r="C25" s="0">
-        <v>0.30887245424145116</v>
+        <v>0.36817208146373365</v>
       </c>
       <c r="D25" s="0">
-        <v>-66541.973752512058</v>
+        <v>-73291.01208007583</v>
       </c>
       <c r="E25" s="0">
-        <v>1732.4522999531641</v>
+        <v>1855.5466591491959</v>
       </c>
       <c r="F25" s="0">
-        <v>-134153.97332683054</v>
+        <v>-159495.65984129821</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>26</v>
+        <v>25.8829071834597</v>
       </c>
       <c r="B26" s="0">
-        <v>133.57373607811664</v>
+        <v>129.69797905839431</v>
       </c>
       <c r="C26" s="0">
-        <v>0.39629949482921134</v>
+        <v>0.39870977931111495</v>
       </c>
       <c r="D26" s="0">
-        <v>-89392.821479613907</v>
+        <v>-86439.72850348652</v>
       </c>
       <c r="E26" s="0">
-        <v>2178.8794665687924</v>
+        <v>2122.2664595147444</v>
       </c>
       <c r="F26" s="0">
-        <v>-235011.78219299499</v>
+        <v>-220532.75096585695</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>26</v>
+        <v>25.919392196733387</v>
       </c>
       <c r="B27" s="0">
-        <v>123.30949284918394</v>
+        <v>127.72560980531588</v>
       </c>
       <c r="C27" s="0">
-        <v>0.37567513747291126</v>
+        <v>0.41509101354197586</v>
       </c>
       <c r="D27" s="0">
-        <v>-82603.358915790741</v>
+        <v>-85260.771434765455</v>
       </c>
       <c r="E27" s="0">
-        <v>2036.5773116318937</v>
+        <v>2095.3962421611759</v>
       </c>
       <c r="F27" s="0">
-        <v>-200251.44021959158</v>
+        <v>-214180.42323207686</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>25.776098036283138</v>
+        <v>25.553579504126002</v>
       </c>
       <c r="B28" s="0">
-        <v>121.82984473593753</v>
+        <v>131.65851548025063</v>
       </c>
       <c r="C28" s="0">
-        <v>0.3712746464380256</v>
+        <v>0.33946165360563119</v>
       </c>
       <c r="D28" s="0">
-        <v>-80924.539285330844</v>
+        <v>-86617.821795030744</v>
       </c>
       <c r="E28" s="0">
-        <v>2010.9328614621766</v>
+        <v>2142.9987806236763</v>
       </c>
       <c r="F28" s="0">
-        <v>-193737.50684555239</v>
+        <v>-224280.67094260713</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>24.79445506498999</v>
+        <v>25.750689346546043</v>
       </c>
       <c r="B29" s="0">
-        <v>102.11552161774422</v>
+        <v>117.40611967378695</v>
       </c>
       <c r="C29" s="0">
-        <v>0.30628033121591353</v>
+        <v>0.47900716724525155</v>
       </c>
       <c r="D29" s="0">
-        <v>-65419.184643337234</v>
+        <v>-77948.594584322869</v>
       </c>
       <c r="E29" s="0">
-        <v>1715.4651302781022</v>
+        <v>1946.9208902495245</v>
       </c>
       <c r="F29" s="0">
-        <v>-130724.0694070836</v>
+        <v>-179727.20098407147</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>25.767914613404095</v>
+        <v>25.682593715061952</v>
       </c>
       <c r="B30" s="0">
-        <v>127.41696352722077</v>
+        <v>111.96927201492835</v>
       </c>
       <c r="C30" s="0">
-        <v>0.37868427977654806</v>
+        <v>0.37641414892540781</v>
       </c>
       <c r="D30" s="0">
-        <v>-84561.609893981178</v>
+        <v>-74189.700060444899</v>
       </c>
       <c r="E30" s="0">
-        <v>2088.2721232246827</v>
+        <v>1871.625087867702</v>
       </c>
       <c r="F30" s="0">
-        <v>-211863.63612588128</v>
+        <v>-163005.97822984413</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>24.817629338758014</v>
+        <v>25.553579504126002</v>
       </c>
       <c r="B31" s="0">
-        <v>102.2077490209733</v>
+        <v>131.65851548025063</v>
       </c>
       <c r="C31" s="0">
-        <v>0.30655789681123063</v>
+        <v>0.33946165360563119</v>
       </c>
       <c r="D31" s="0">
-        <v>-65538.252162259829</v>
+        <v>-86617.821795030744</v>
       </c>
       <c r="E31" s="0">
-        <v>1717.2758040784599</v>
+        <v>2142.9987806236763</v>
       </c>
       <c r="F31" s="0">
-        <v>-131086.73763638426</v>
+        <v>-224280.67094260713</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>24.091446215109514</v>
+        <v>25.696042467488898</v>
       </c>
       <c r="B32" s="0">
-        <v>100</v>
+        <v>104.14005484012439</v>
       </c>
       <c r="C32" s="0">
-        <v>0.29999999999999999</v>
+        <v>0.39702352439547373</v>
       </c>
       <c r="D32" s="0">
-        <v>-62277.049738448943</v>
+        <v>-69110.640563072171</v>
       </c>
       <c r="E32" s="0">
-        <v>1669.9820063339721</v>
+        <v>1762.738137335368</v>
       </c>
       <c r="F32" s="0">
-        <v>-121694.3418114376</v>
+        <v>-141060.28279096275</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>25.960741923814112</v>
+        <v>25.605704878238168</v>
       </c>
       <c r="B33" s="0">
-        <v>112.47659188403132</v>
+        <v>110.92928128259632</v>
       </c>
       <c r="C33" s="0">
-        <v>0.34084085776009038</v>
+        <v>0.36817208146373365</v>
       </c>
       <c r="D33" s="0">
-        <v>-75324.164824820327</v>
+        <v>-73291.01208007583</v>
       </c>
       <c r="E33" s="0">
-        <v>1885.7221950709479</v>
+        <v>1855.5466591491959</v>
       </c>
       <c r="F33" s="0">
-        <v>-166322.14711560388</v>
+        <v>-159495.65984129821</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>26</v>
+        <v>25.556305370846339</v>
       </c>
       <c r="B34" s="0">
-        <v>133.57373607811664</v>
+        <v>114.57979332813709</v>
       </c>
       <c r="C34" s="0">
-        <v>0.39629949482921134</v>
+        <v>0.31515895258397691</v>
       </c>
       <c r="D34" s="0">
-        <v>-89392.821479613907</v>
+        <v>-75522.922106385318</v>
       </c>
       <c r="E34" s="0">
-        <v>2178.8794665687924</v>
+        <v>1906.1042819842369</v>
       </c>
       <c r="F34" s="0">
-        <v>-235011.78219299499</v>
+        <v>-169839.82536300496</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>24.79445506498999</v>
+        <v>24.453876449612522</v>
       </c>
       <c r="B35" s="0">
-        <v>102.11552161774422</v>
+        <v>100.89878945382742</v>
       </c>
       <c r="C35" s="0">
-        <v>0.30628033121591353</v>
+        <v>0.38677470788105578</v>
       </c>
       <c r="D35" s="0">
-        <v>-65419.184643337234</v>
+        <v>-63769.290317293096</v>
       </c>
       <c r="E35" s="0">
-        <v>1715.4651302781022</v>
+        <v>1689.2617387950761</v>
       </c>
       <c r="F35" s="0">
-        <v>-130724.0694070836</v>
+        <v>-125816.82017019449</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>26</v>
+        <v>22.746929212114072</v>
       </c>
       <c r="B36" s="0">
-        <v>140</v>
+        <v>101.67559507604604</v>
       </c>
       <c r="C36" s="0">
-        <v>0.5</v>
+        <v>0.43337692961180319</v>
       </c>
       <c r="D36" s="0">
-        <v>-93644.825000000012</v>
+        <v>-59791.363716217165</v>
       </c>
       <c r="E36" s="0">
-        <v>2266.3400000000001</v>
+        <v>1659.9104341176069</v>
       </c>
       <c r="F36" s="0">
-        <v>-258189.64637499998</v>
+        <v>-118568.62983205088</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>25.960741923814112</v>
+        <v>25.750689346546043</v>
       </c>
       <c r="B37" s="0">
-        <v>112.47659188403132</v>
+        <v>117.40611967378695</v>
       </c>
       <c r="C37" s="0">
-        <v>0.34084085776009038</v>
+        <v>0.47900716724525155</v>
       </c>
       <c r="D37" s="0">
-        <v>-75324.164824820327</v>
+        <v>-77948.594584322869</v>
       </c>
       <c r="E37" s="0">
-        <v>1885.7221950709479</v>
+        <v>1946.9208902495245</v>
       </c>
       <c r="F37" s="0">
-        <v>-166322.14711560388</v>
+        <v>-179727.20098407147</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>26</v>
+        <v>25.682593715061952</v>
       </c>
       <c r="B38" s="0">
-        <v>123.11652984719713</v>
+        <v>111.96927201492835</v>
       </c>
       <c r="C38" s="0">
-        <v>0.37515673832248242</v>
+        <v>0.37641414892540781</v>
       </c>
       <c r="D38" s="0">
-        <v>-82475.71839160817</v>
+        <v>-74189.700060444899</v>
       </c>
       <c r="E38" s="0">
-        <v>2033.9044467210019</v>
+        <v>1871.625087867702</v>
       </c>
       <c r="F38" s="0">
-        <v>-199624.5880938386</v>
+        <v>-163005.97822984413</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>25.181779988745912</v>
+        <v>25.553579504126002</v>
       </c>
       <c r="B39" s="0">
-        <v>105.66993167323744</v>
+        <v>131.65851548025063</v>
       </c>
       <c r="C39" s="0">
-        <v>0.31817692700808514</v>
+        <v>0.33946165360563119</v>
       </c>
       <c r="D39" s="0">
-        <v>-68713.159228639866</v>
+        <v>-86617.821795030744</v>
       </c>
       <c r="E39" s="0">
-        <v>1773.5776222512134</v>
+        <v>2142.9987806236763</v>
       </c>
       <c r="F39" s="0">
-        <v>-142247.86853350193</v>
+        <v>-224280.67094260713</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>25.957240843969895</v>
+        <v>25.618553385370983</v>
       </c>
       <c r="B40" s="0">
-        <v>111.35903950289826</v>
+        <v>135.93147780256623</v>
       </c>
       <c r="C40" s="0">
-        <v>0.33888943031255864</v>
+        <v>0.42718729788386356</v>
       </c>
       <c r="D40" s="0">
-        <v>-74576.046456356053</v>
+        <v>-89623.258790606706</v>
       </c>
       <c r="E40" s="0">
-        <v>1870.1426737698928</v>
+        <v>2202.3119983048127</v>
       </c>
       <c r="F40" s="0">
-        <v>-163007.32509880053</v>
+        <v>-239714.30125701483</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>24.817629338758014</v>
+        <v>25.756368310454423</v>
       </c>
       <c r="B41" s="0">
-        <v>102.2077490209733</v>
+        <v>121.84677821758635</v>
       </c>
       <c r="C41" s="0">
-        <v>0.30655789681123063</v>
+        <v>0.39548545565116999</v>
       </c>
       <c r="D41" s="0">
-        <v>-65538.252162259829</v>
+        <v>-80874.27751679653</v>
       </c>
       <c r="E41" s="0">
-        <v>1717.2758040784599</v>
+        <v>2010.2785509216076</v>
       </c>
       <c r="F41" s="0">
-        <v>-131086.73763638426</v>
+        <v>-193638.66185013676</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>26</v>
+        <v>25.8829071834597</v>
       </c>
       <c r="B42" s="0">
-        <v>114.5167257643447</v>
+        <v>129.69797905839431</v>
       </c>
       <c r="C42" s="0">
-        <v>0.34266584072727874</v>
+        <v>0.39870977931111495</v>
       </c>
       <c r="D42" s="0">
-        <v>-76787.020478294085</v>
+        <v>-86439.72850348652</v>
       </c>
       <c r="E42" s="0">
-        <v>1914.9513563081148</v>
+        <v>2122.2664595147444</v>
       </c>
       <c r="F42" s="0">
-        <v>-172685.38568964577</v>
+        <v>-220532.75096585695</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>26</v>
+        <v>22.746929212114072</v>
       </c>
       <c r="B43" s="0">
-        <v>133.57373607811664</v>
+        <v>101.67559507604604</v>
       </c>
       <c r="C43" s="0">
-        <v>0.39629949482921134</v>
+        <v>0.43337692961180319</v>
       </c>
       <c r="D43" s="0">
-        <v>-89392.821479613907</v>
+        <v>-59791.363716217165</v>
       </c>
       <c r="E43" s="0">
-        <v>2178.8794665687924</v>
+        <v>1659.9104341176069</v>
       </c>
       <c r="F43" s="0">
-        <v>-235011.78219299499</v>
+        <v>-118568.62983205088</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>25.859367647961051</v>
+        <v>25.620987519841727</v>
       </c>
       <c r="B44" s="0">
-        <v>121.11310880263503</v>
+        <v>125.64647255985861</v>
       </c>
       <c r="C44" s="0">
-        <v>0.36496630110841599</v>
+        <v>0.38119036813335921</v>
       </c>
       <c r="D44" s="0">
-        <v>-80713.293820300692</v>
+        <v>-82927.369782510374</v>
       </c>
       <c r="E44" s="0">
-        <v>2003.0013551952406</v>
+        <v>2060.233508344952</v>
       </c>
       <c r="F44" s="0">
-        <v>-192099.13219150651</v>
+        <v>-204802.08007602533</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>26</v>
+        <v>24.470486141913241</v>
       </c>
       <c r="B45" s="0">
-        <v>113.32142911143836</v>
+        <v>108.85339849603808</v>
       </c>
       <c r="C45" s="0">
-        <v>0.33826928731642791</v>
+        <v>0.4709111763710514</v>
       </c>
       <c r="D45" s="0">
-        <v>-75996.34344724167</v>
+        <v>-68765.503044241661</v>
       </c>
       <c r="E45" s="0">
-        <v>1898.4157828630439</v>
+        <v>1798.7005519920397</v>
       </c>
       <c r="F45" s="0">
-        <v>-169095.56353565105</v>
+        <v>-146565.13893950562</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>25.691832909059549</v>
+        <v>25.556305370846339</v>
       </c>
       <c r="B46" s="0">
-        <v>110.13068715013875</v>
+        <v>114.57979332813709</v>
       </c>
       <c r="C46" s="0">
-        <v>0.33283338490613107</v>
+        <v>0.31515895258397691</v>
       </c>
       <c r="D46" s="0">
-        <v>-73013.975659789488</v>
+        <v>-75522.922106385318</v>
       </c>
       <c r="E46" s="0">
-        <v>1847.065119021958</v>
+        <v>1906.1042819842369</v>
       </c>
       <c r="F46" s="0">
-        <v>-157749.50871127206</v>
+        <v>-169839.82536300496</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>26</v>
+        <v>25.756368310454423</v>
       </c>
       <c r="B47" s="0">
-        <v>140</v>
+        <v>121.84677821758635</v>
       </c>
       <c r="C47" s="0">
-        <v>0.44745101610300025</v>
+        <v>0.39548545565116999</v>
       </c>
       <c r="D47" s="0">
-        <v>-93644.107706369818</v>
+        <v>-80874.27751679653</v>
       </c>
       <c r="E47" s="0">
-        <v>2267.284830730468</v>
+        <v>2010.2785509216076</v>
       </c>
       <c r="F47" s="0">
-        <v>-258189.79444044639</v>
+        <v>-193638.66185013676</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>26</v>
+        <v>25.605704878238168</v>
       </c>
       <c r="B48" s="0">
-        <v>123.31084830966549</v>
+        <v>110.92928128259632</v>
       </c>
       <c r="C48" s="0">
-        <v>0.37553192511996231</v>
+        <v>0.36817208146373365</v>
       </c>
       <c r="D48" s="0">
-        <v>-82604.253516723038</v>
+        <v>-73291.01208007583</v>
       </c>
       <c r="E48" s="0">
-        <v>2036.5987274906934</v>
+        <v>1855.5466591491959</v>
       </c>
       <c r="F48" s="0">
-        <v>-200255.84740080024</v>
+        <v>-159495.65984129821</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>26</v>
+        <v>24.470486141913241</v>
       </c>
       <c r="B49" s="0">
-        <v>118.77298393747444</v>
+        <v>108.85339849603808</v>
       </c>
       <c r="C49" s="0">
-        <v>0.36598003414542912</v>
+        <v>0.4709111763710514</v>
       </c>
       <c r="D49" s="0">
-        <v>-79602.598123069183</v>
+        <v>-68765.503044241661</v>
       </c>
       <c r="E49" s="0">
-        <v>1973.6941557169598</v>
+        <v>1798.7005519920397</v>
       </c>
       <c r="F49" s="0">
-        <v>-185774.30962561115</v>
+        <v>-146565.13893950562</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>24.723423560383161</v>
+        <v>25.618553385370983</v>
       </c>
       <c r="B50" s="0">
-        <v>101.84793273510381</v>
+        <v>135.93147780256623</v>
       </c>
       <c r="C50" s="0">
-        <v>0.3054784271146076</v>
+        <v>0.42718729788386356</v>
       </c>
       <c r="D50" s="0">
-        <v>-65064.404518571726</v>
+        <v>-89623.258790606706</v>
       </c>
       <c r="E50" s="0">
-        <v>1710.1242074940467</v>
+        <v>2202.3119983048127</v>
       </c>
       <c r="F50" s="0">
-        <v>-129655.10259269616</v>
+        <v>-239714.30125701483</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>24.703260632614182</v>
+        <v>22.746929212114072</v>
       </c>
       <c r="B51" s="0">
-        <v>101.80556777788125</v>
+        <v>101.67559507604604</v>
       </c>
       <c r="C51" s="0">
-        <v>0.30534196982274092</v>
+        <v>0.43337692961180319</v>
       </c>
       <c r="D51" s="0">
-        <v>-64984.985736112882</v>
+        <v>-59791.363716217165</v>
       </c>
       <c r="E51" s="0">
-        <v>1709.0734358642412</v>
+        <v>1659.9104341176069</v>
       </c>
       <c r="F51" s="0">
-        <v>-129438.2389502852</v>
+        <v>-118568.62983205088</v>
       </c>
     </row>
     <row r="52">

</xml_diff>

<commit_message>
Refactor plotChart.m and remove plotChart_new.m
- Refactor plotChart.m to use separate functions for 2D and 3D plotting
- Add support for multiple figure windows showing different projections
- Improve code organization with helper functions checkfigHandle, plot2D, and plot3D
- Remove obsolete plotChart_new.m file
- Update binary files Optimal.xlsx and matlab.mat with new results
</commit_message>
<xml_diff>
--- a/Optimal.xlsx
+++ b/Optimal.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="84" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="90" uniqueCount="7">
   <si>
     <t>X1</t>
   </si>
@@ -115,1002 +115,1002 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>24.470486141913241</v>
+        <v>23.875006942982093</v>
       </c>
       <c r="B2" s="0">
-        <v>108.85339849603808</v>
+        <v>109.41263880710096</v>
       </c>
       <c r="C2" s="0">
-        <v>0.4709111763710514</v>
+        <v>0.46972176595962373</v>
       </c>
       <c r="D2" s="0">
-        <v>-68765.503044241661</v>
+        <v>-67439.888525732109</v>
       </c>
       <c r="E2" s="0">
-        <v>1798.7005519920397</v>
+        <v>1792.7814919636269</v>
       </c>
       <c r="F2" s="0">
-        <v>-146565.13893950562</v>
+        <v>-144361.53111926137</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>25.919392196733387</v>
+        <v>23.875006942982093</v>
       </c>
       <c r="B3" s="0">
-        <v>127.72560980531588</v>
+        <v>109.41263880710096</v>
       </c>
       <c r="C3" s="0">
-        <v>0.41509101354197586</v>
+        <v>0.46972176595962373</v>
       </c>
       <c r="D3" s="0">
-        <v>-85260.771434765455</v>
+        <v>-67439.888525732109</v>
       </c>
       <c r="E3" s="0">
-        <v>2095.3962421611759</v>
+        <v>1792.7814919636269</v>
       </c>
       <c r="F3" s="0">
-        <v>-214180.42323207686</v>
+        <v>-144361.53111926137</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>25.618553385370983</v>
+        <v>25.61815391394012</v>
       </c>
       <c r="B4" s="0">
-        <v>135.93147780256623</v>
+        <v>119.92344667163808</v>
       </c>
       <c r="C4" s="0">
-        <v>0.42718729788386356</v>
+        <v>0.49128623022716422</v>
       </c>
       <c r="D4" s="0">
-        <v>-89623.258790606706</v>
+        <v>-79189.893963938041</v>
       </c>
       <c r="E4" s="0">
-        <v>2202.3119983048127</v>
+        <v>1978.638666954326</v>
       </c>
       <c r="F4" s="0">
-        <v>-239714.30125701483</v>
+        <v>-186531.45901636404</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>25.756368310454423</v>
+        <v>23.874947542822227</v>
       </c>
       <c r="B5" s="0">
-        <v>121.84677821758635</v>
+        <v>119.92290742064648</v>
       </c>
       <c r="C5" s="0">
-        <v>0.39548545565116999</v>
+        <v>0.49128622530165833</v>
       </c>
       <c r="D5" s="0">
-        <v>-80874.27751679653</v>
+        <v>-73823.728846179802</v>
       </c>
       <c r="E5" s="0">
-        <v>2010.2785509216076</v>
+        <v>1938.4851287272581</v>
       </c>
       <c r="F5" s="0">
-        <v>-193638.66185013676</v>
+        <v>-173461.91217714103</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>25.8829071834597</v>
+        <v>25.224459513620715</v>
       </c>
       <c r="B6" s="0">
-        <v>129.69797905839431</v>
+        <v>100.01955122973901</v>
       </c>
       <c r="C6" s="0">
-        <v>0.39870977931111495</v>
+        <v>0.49128639015974701</v>
       </c>
       <c r="D6" s="0">
-        <v>-86439.72850348652</v>
+        <v>-65205.512786527637</v>
       </c>
       <c r="E6" s="0">
-        <v>2122.2664595147444</v>
+        <v>1692.9077353969851</v>
       </c>
       <c r="F6" s="0">
-        <v>-220532.75096585695</v>
+        <v>-127647.51180694136</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>25.618553385370983</v>
+        <v>25.712531550521202</v>
       </c>
       <c r="B7" s="0">
-        <v>135.93147780256623</v>
+        <v>109.41261405750602</v>
       </c>
       <c r="C7" s="0">
-        <v>0.42718729788386356</v>
+        <v>0.49128613091577261</v>
       </c>
       <c r="D7" s="0">
-        <v>-89623.258790606706</v>
+        <v>-72604.984444196903</v>
       </c>
       <c r="E7" s="0">
-        <v>2202.3119983048127</v>
+        <v>1834.7116123739713</v>
       </c>
       <c r="F7" s="0">
-        <v>-239714.30125701483</v>
+        <v>-155825.55759322413</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>25.682593715061952</v>
+        <v>23.875006942982093</v>
       </c>
       <c r="B8" s="0">
-        <v>111.96927201492835</v>
+        <v>109.41263880710096</v>
       </c>
       <c r="C8" s="0">
-        <v>0.37641414892540781</v>
+        <v>0.46972176595962373</v>
       </c>
       <c r="D8" s="0">
-        <v>-74189.700060444899</v>
+        <v>-67439.888525732109</v>
       </c>
       <c r="E8" s="0">
-        <v>1871.625087867702</v>
+        <v>1792.7814919636269</v>
       </c>
       <c r="F8" s="0">
-        <v>-163005.97822984413</v>
+        <v>-144361.53111926137</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>25.605704878238168</v>
+        <v>25.854488806783635</v>
       </c>
       <c r="B9" s="0">
-        <v>110.92928128259632</v>
+        <v>113.52638339802725</v>
       </c>
       <c r="C9" s="0">
-        <v>0.36817208146373365</v>
+        <v>0.49128768736562645</v>
       </c>
       <c r="D9" s="0">
-        <v>-73291.01208007583</v>
+        <v>-75709.77360533188</v>
       </c>
       <c r="E9" s="0">
-        <v>1855.5466591491959</v>
+        <v>1895.162253833972</v>
       </c>
       <c r="F9" s="0">
-        <v>-159495.65984129821</v>
+        <v>-168730.54268168294</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>25.553579504126002</v>
+        <v>25.224463182320878</v>
       </c>
       <c r="B10" s="0">
-        <v>131.65851548025063</v>
+        <v>109.41251797000442</v>
       </c>
       <c r="C10" s="0">
-        <v>0.33946165360563119</v>
+        <v>0.49128667225964967</v>
       </c>
       <c r="D10" s="0">
-        <v>-86617.821795030744</v>
+        <v>-71233.086137543374</v>
       </c>
       <c r="E10" s="0">
-        <v>2142.9987806236763</v>
+        <v>1823.4700525046828</v>
       </c>
       <c r="F10" s="0">
-        <v>-224280.67094260713</v>
+        <v>-152780.27504011022</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>24.470486141913241</v>
+        <v>25.601126505734449</v>
       </c>
       <c r="B11" s="0">
-        <v>108.85339849603808</v>
+        <v>100.01981785075569</v>
       </c>
       <c r="C11" s="0">
-        <v>0.4709111763710514</v>
+        <v>0.49128640717886446</v>
       </c>
       <c r="D11" s="0">
-        <v>-68765.503044241661</v>
+        <v>-66174.393853088506</v>
       </c>
       <c r="E11" s="0">
-        <v>1798.7005519920397</v>
+        <v>1701.5860819514926</v>
       </c>
       <c r="F11" s="0">
-        <v>-146565.13893950562</v>
+        <v>-129611.64249073368</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>25.750689346546043</v>
+        <v>23.874944903946343</v>
       </c>
       <c r="B12" s="0">
-        <v>117.40611967378695</v>
+        <v>119.92337605130746</v>
       </c>
       <c r="C12" s="0">
-        <v>0.47900716724525155</v>
+        <v>0.49128766841904919</v>
       </c>
       <c r="D12" s="0">
-        <v>-77948.594584322869</v>
+        <v>-73824.005379312599</v>
       </c>
       <c r="E12" s="0">
-        <v>1946.9208902495245</v>
+        <v>1938.4915559728834</v>
       </c>
       <c r="F12" s="0">
-        <v>-179727.20098407147</v>
+        <v>-173463.24946300231</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>25.8829071834597</v>
+        <v>23.874947542822227</v>
       </c>
       <c r="B13" s="0">
-        <v>129.69797905839431</v>
+        <v>119.92290742064648</v>
       </c>
       <c r="C13" s="0">
-        <v>0.39870977931111495</v>
+        <v>0.49128622530165833</v>
       </c>
       <c r="D13" s="0">
-        <v>-86439.72850348652</v>
+        <v>-73823.728846179802</v>
       </c>
       <c r="E13" s="0">
-        <v>2122.2664595147444</v>
+        <v>1938.4851287272581</v>
       </c>
       <c r="F13" s="0">
-        <v>-220532.75096585695</v>
+        <v>-173461.91217714103</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>25.919392196733387</v>
+        <v>25.224455268661256</v>
       </c>
       <c r="B14" s="0">
-        <v>127.72560980531588</v>
+        <v>124.89968618097143</v>
       </c>
       <c r="C14" s="0">
-        <v>0.41509101354197586</v>
+        <v>0.49128623968856905</v>
       </c>
       <c r="D14" s="0">
-        <v>-85260.771434765455</v>
+        <v>-81171.336800739431</v>
       </c>
       <c r="E14" s="0">
-        <v>2095.3962421611759</v>
+        <v>2038.7415161631711</v>
       </c>
       <c r="F14" s="0">
-        <v>-214180.42323207686</v>
+        <v>-199147.52189131209</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>25.682593715061952</v>
+        <v>25.224461090432516</v>
       </c>
       <c r="B15" s="0">
-        <v>111.96927201492835</v>
+        <v>132.16657154812918</v>
       </c>
       <c r="C15" s="0">
-        <v>0.37641414892540781</v>
+        <v>0.49128610456938188</v>
       </c>
       <c r="D15" s="0">
-        <v>-74189.700060444899</v>
+        <v>-85834.590573524052</v>
       </c>
       <c r="E15" s="0">
-        <v>1871.625087867702</v>
+        <v>2139.751359271499</v>
       </c>
       <c r="F15" s="0">
-        <v>-163005.97822984413</v>
+        <v>-223018.88539772257</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>25.605704878238168</v>
+        <v>25.618153097884537</v>
       </c>
       <c r="B16" s="0">
-        <v>110.92928128259632</v>
+        <v>124.89982348896177</v>
       </c>
       <c r="C16" s="0">
-        <v>0.36817208146373365</v>
+        <v>0.4912875358984885</v>
       </c>
       <c r="D16" s="0">
-        <v>-73291.01208007583</v>
+        <v>-82433.124705897892</v>
       </c>
       <c r="E16" s="0">
-        <v>1855.5466591491959</v>
+        <v>2047.8102624453945</v>
       </c>
       <c r="F16" s="0">
-        <v>-159495.65984129821</v>
+        <v>-202349.5850209436</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>25.682593715061952</v>
+        <v>25.61815391394012</v>
       </c>
       <c r="B17" s="0">
-        <v>111.96927201492835</v>
+        <v>119.92344667163808</v>
       </c>
       <c r="C17" s="0">
-        <v>0.37641414892540781</v>
+        <v>0.49128623022716422</v>
       </c>
       <c r="D17" s="0">
-        <v>-74189.700060444899</v>
+        <v>-79189.893963938041</v>
       </c>
       <c r="E17" s="0">
-        <v>1871.625087867702</v>
+        <v>1978.638666954326</v>
       </c>
       <c r="F17" s="0">
-        <v>-163005.97822984413</v>
+        <v>-186531.45901636404</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>24.470486141913241</v>
+        <v>25.601125681965666</v>
       </c>
       <c r="B18" s="0">
-        <v>108.85339849603808</v>
+        <v>100.01936674002421</v>
       </c>
       <c r="C18" s="0">
-        <v>0.4709111763710514</v>
+        <v>0.49128624323855974</v>
       </c>
       <c r="D18" s="0">
-        <v>-68765.503044241661</v>
+        <v>-66174.097927188937</v>
       </c>
       <c r="E18" s="0">
-        <v>1798.7005519920397</v>
+        <v>1701.5797954885766</v>
       </c>
       <c r="F18" s="0">
-        <v>-146565.13893950562</v>
+        <v>-129610.46762477436</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>25.556305370846339</v>
+        <v>25.854481104765942</v>
       </c>
       <c r="B19" s="0">
-        <v>114.57979332813709</v>
+        <v>132.16649660815901</v>
       </c>
       <c r="C19" s="0">
-        <v>0.31515895258397691</v>
+        <v>0.49128621147357765</v>
       </c>
       <c r="D19" s="0">
-        <v>-75522.922106385318</v>
+        <v>-87970.061900369721</v>
       </c>
       <c r="E19" s="0">
-        <v>1906.1042819842369</v>
+        <v>2154.2596766138749</v>
       </c>
       <c r="F19" s="0">
-        <v>-169839.82536300496</v>
+        <v>-228756.1409334963</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>25.605704878238168</v>
+        <v>25.854488806783635</v>
       </c>
       <c r="B20" s="0">
-        <v>110.92928128259632</v>
+        <v>113.52638339802725</v>
       </c>
       <c r="C20" s="0">
-        <v>0.36817208146373365</v>
+        <v>0.49128768736562645</v>
       </c>
       <c r="D20" s="0">
-        <v>-73291.01208007583</v>
+        <v>-75709.77360533188</v>
       </c>
       <c r="E20" s="0">
-        <v>1855.5466591491959</v>
+        <v>1895.162253833972</v>
       </c>
       <c r="F20" s="0">
-        <v>-159495.65984129821</v>
+        <v>-168730.54268168294</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>25.756368310454423</v>
+        <v>25.712525614235773</v>
       </c>
       <c r="B21" s="0">
-        <v>121.84677821758635</v>
+        <v>113.52603542201737</v>
       </c>
       <c r="C21" s="0">
-        <v>0.39548545565116999</v>
+        <v>0.49128735928019113</v>
       </c>
       <c r="D21" s="0">
-        <v>-80874.27751679653</v>
+        <v>-75295.666319463504</v>
       </c>
       <c r="E21" s="0">
-        <v>2010.2785509216076</v>
+        <v>1891.8880105420335</v>
       </c>
       <c r="F21" s="0">
-        <v>-193638.66185013676</v>
+        <v>-167775.89293842294</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>25.919392196733387</v>
+        <v>25.61814424404588</v>
       </c>
       <c r="B22" s="0">
-        <v>127.72560980531588</v>
+        <v>113.52623549877508</v>
       </c>
       <c r="C22" s="0">
-        <v>0.41509101354197586</v>
+        <v>0.49128752114779695</v>
       </c>
       <c r="D22" s="0">
-        <v>-85260.771434765455</v>
+        <v>-75020.637993018332</v>
       </c>
       <c r="E22" s="0">
-        <v>2095.3962421611759</v>
+        <v>1889.7171857431131</v>
       </c>
       <c r="F22" s="0">
-        <v>-214180.42323207686</v>
+        <v>-167142.4914544365</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>24.470486141913241</v>
+        <v>25.224461090432516</v>
       </c>
       <c r="B23" s="0">
-        <v>108.85339849603808</v>
+        <v>132.16657154812918</v>
       </c>
       <c r="C23" s="0">
-        <v>0.4709111763710514</v>
+        <v>0.49128610456938188</v>
       </c>
       <c r="D23" s="0">
-        <v>-68765.503044241661</v>
+        <v>-85834.590573524052</v>
       </c>
       <c r="E23" s="0">
-        <v>1798.7005519920397</v>
+        <v>2139.751359271499</v>
       </c>
       <c r="F23" s="0">
-        <v>-146565.13893950562</v>
+        <v>-223018.88539772257</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>24.453876449612522</v>
+        <v>25.224451821106776</v>
       </c>
       <c r="B24" s="0">
-        <v>100.89878945382742</v>
+        <v>132.1658771138473</v>
       </c>
       <c r="C24" s="0">
-        <v>0.38677470788105578</v>
+        <v>0.49128764059098046</v>
       </c>
       <c r="D24" s="0">
-        <v>-63769.290317293096</v>
+        <v>-85834.113549653193</v>
       </c>
       <c r="E24" s="0">
-        <v>1689.2617387950761</v>
+        <v>2139.7414655447405</v>
       </c>
       <c r="F24" s="0">
-        <v>-125816.82017019449</v>
+        <v>-223016.45526407374</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>25.605704878238168</v>
+        <v>23.875006942982093</v>
       </c>
       <c r="B25" s="0">
-        <v>110.92928128259632</v>
+        <v>109.41263880710096</v>
       </c>
       <c r="C25" s="0">
-        <v>0.36817208146373365</v>
+        <v>0.46972176595962373</v>
       </c>
       <c r="D25" s="0">
-        <v>-73291.01208007583</v>
+        <v>-67439.888525732109</v>
       </c>
       <c r="E25" s="0">
-        <v>1855.5466591491959</v>
+        <v>1792.7814919636269</v>
       </c>
       <c r="F25" s="0">
-        <v>-159495.65984129821</v>
+        <v>-144361.53111926137</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>25.8829071834597</v>
+        <v>25.601126505734449</v>
       </c>
       <c r="B26" s="0">
-        <v>129.69797905839431</v>
+        <v>100.01981785075569</v>
       </c>
       <c r="C26" s="0">
-        <v>0.39870977931111495</v>
+        <v>0.49128640717886446</v>
       </c>
       <c r="D26" s="0">
-        <v>-86439.72850348652</v>
+        <v>-66174.393853088506</v>
       </c>
       <c r="E26" s="0">
-        <v>2122.2664595147444</v>
+        <v>1701.5860819514926</v>
       </c>
       <c r="F26" s="0">
-        <v>-220532.75096585695</v>
+        <v>-129611.64249073368</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>25.919392196733387</v>
+        <v>25.601125681965666</v>
       </c>
       <c r="B27" s="0">
-        <v>127.72560980531588</v>
+        <v>100.01936674002421</v>
       </c>
       <c r="C27" s="0">
-        <v>0.41509101354197586</v>
+        <v>0.49128624323855974</v>
       </c>
       <c r="D27" s="0">
-        <v>-85260.771434765455</v>
+        <v>-66174.097927188937</v>
       </c>
       <c r="E27" s="0">
-        <v>2095.3962421611759</v>
+        <v>1701.5797954885766</v>
       </c>
       <c r="F27" s="0">
-        <v>-214180.42323207686</v>
+        <v>-129610.46762477436</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>25.553579504126002</v>
+        <v>23.874944903946343</v>
       </c>
       <c r="B28" s="0">
-        <v>131.65851548025063</v>
+        <v>119.92337605130746</v>
       </c>
       <c r="C28" s="0">
-        <v>0.33946165360563119</v>
+        <v>0.49128766841904919</v>
       </c>
       <c r="D28" s="0">
-        <v>-86617.821795030744</v>
+        <v>-73824.005379312599</v>
       </c>
       <c r="E28" s="0">
-        <v>2142.9987806236763</v>
+        <v>1938.4915559728834</v>
       </c>
       <c r="F28" s="0">
-        <v>-224280.67094260713</v>
+        <v>-173463.24946300231</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>25.750689346546043</v>
+        <v>25.854491743977551</v>
       </c>
       <c r="B29" s="0">
-        <v>117.40611967378695</v>
+        <v>109.41223618051394</v>
       </c>
       <c r="C29" s="0">
-        <v>0.47900716724525155</v>
+        <v>0.49128628533875596</v>
       </c>
       <c r="D29" s="0">
-        <v>-77948.594584322869</v>
+        <v>-73003.750076056967</v>
       </c>
       <c r="E29" s="0">
-        <v>1946.9208902495245</v>
+        <v>1837.9757003625559</v>
       </c>
       <c r="F29" s="0">
-        <v>-179727.20098407147</v>
+        <v>-156710.15059551509</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>25.682593715061952</v>
+        <v>25.618153097884537</v>
       </c>
       <c r="B30" s="0">
-        <v>111.96927201492835</v>
+        <v>124.89982348896177</v>
       </c>
       <c r="C30" s="0">
-        <v>0.37641414892540781</v>
+        <v>0.4912875358984885</v>
       </c>
       <c r="D30" s="0">
-        <v>-74189.700060444899</v>
+        <v>-82433.124705897892</v>
       </c>
       <c r="E30" s="0">
-        <v>1871.625087867702</v>
+        <v>2047.8102624453945</v>
       </c>
       <c r="F30" s="0">
-        <v>-163005.97822984413</v>
+        <v>-202349.5850209436</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>25.553579504126002</v>
+        <v>25.618149936820124</v>
       </c>
       <c r="B31" s="0">
-        <v>131.65851548025063</v>
+        <v>119.92340383371194</v>
       </c>
       <c r="C31" s="0">
-        <v>0.33946165360563119</v>
+        <v>0.49128638615123266</v>
       </c>
       <c r="D31" s="0">
-        <v>-86617.821795030744</v>
+        <v>-79189.853805345512</v>
       </c>
       <c r="E31" s="0">
-        <v>2142.9987806236763</v>
+        <v>1978.6379771105644</v>
       </c>
       <c r="F31" s="0">
-        <v>-224280.67094260713</v>
+        <v>-186531.29580526281</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>25.696042467488898</v>
+        <v>25.85445982289632</v>
       </c>
       <c r="B32" s="0">
-        <v>104.14005484012439</v>
+        <v>119.92350664750568</v>
       </c>
       <c r="C32" s="0">
-        <v>0.39702352439547373</v>
+        <v>0.49128768140335788</v>
       </c>
       <c r="D32" s="0">
-        <v>-69110.640563072171</v>
+        <v>-79917.316689540443</v>
       </c>
       <c r="E32" s="0">
-        <v>1762.738137335368</v>
+        <v>1984.0815996099989</v>
       </c>
       <c r="F32" s="0">
-        <v>-141060.28279096275</v>
+        <v>-188303.12004191964</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>25.605704878238168</v>
+        <v>25.618152863259823</v>
       </c>
       <c r="B33" s="0">
-        <v>110.92928128259632</v>
+        <v>136.10512151331841</v>
       </c>
       <c r="C33" s="0">
-        <v>0.36817208146373365</v>
+        <v>0.4912861457984144</v>
       </c>
       <c r="D33" s="0">
-        <v>-73291.01208007583</v>
+        <v>-89735.905853243443</v>
       </c>
       <c r="E33" s="0">
-        <v>1855.5466591491959</v>
+        <v>2203.5639245745442</v>
       </c>
       <c r="F33" s="0">
-        <v>-159495.65984129821</v>
+        <v>-240323.62677455996</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>25.556305370846339</v>
+        <v>25.618153238722648</v>
       </c>
       <c r="B34" s="0">
-        <v>114.57979332813709</v>
+        <v>136.10530457568424</v>
       </c>
       <c r="C34" s="0">
-        <v>0.31515895258397691</v>
+        <v>0.49128626646661977</v>
       </c>
       <c r="D34" s="0">
-        <v>-75522.922106385318</v>
+        <v>-89736.026471652527</v>
       </c>
       <c r="E34" s="0">
-        <v>1906.1042819842369</v>
+        <v>2203.5664756187239</v>
       </c>
       <c r="F34" s="0">
-        <v>-169839.82536300496</v>
+        <v>-240324.27744536861</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>24.453876449612522</v>
+        <v>25.854490710176915</v>
       </c>
       <c r="B35" s="0">
-        <v>100.89878945382742</v>
+        <v>136.10522450456983</v>
       </c>
       <c r="C35" s="0">
-        <v>0.38677470788105578</v>
+        <v>0.49128762983616314</v>
       </c>
       <c r="D35" s="0">
-        <v>-63769.290317293096</v>
+        <v>-90560.746447152967</v>
       </c>
       <c r="E35" s="0">
-        <v>1689.2617387950761</v>
+        <v>2209.0081900844407</v>
       </c>
       <c r="F35" s="0">
-        <v>-125816.82017019449</v>
+        <v>-242606.59284989868</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>22.746929212114072</v>
+        <v>25.712531849715972</v>
       </c>
       <c r="B36" s="0">
-        <v>101.67559507604604</v>
+        <v>136.10500941319125</v>
       </c>
       <c r="C36" s="0">
-        <v>0.43337692961180319</v>
+        <v>0.49128615369210937</v>
       </c>
       <c r="D36" s="0">
-        <v>-59791.363716217165</v>
+        <v>-90065.196717595682</v>
       </c>
       <c r="E36" s="0">
-        <v>1659.9104341176069</v>
+        <v>2205.735914298933</v>
       </c>
       <c r="F36" s="0">
-        <v>-118568.62983205088</v>
+        <v>-241234.76033456274</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>25.750689346546043</v>
+        <v>25.618141575828098</v>
       </c>
       <c r="B37" s="0">
-        <v>117.40611967378695</v>
+        <v>136.10528920949929</v>
       </c>
       <c r="C37" s="0">
-        <v>0.47900716724525155</v>
+        <v>0.49128626220529353</v>
       </c>
       <c r="D37" s="0">
-        <v>-77948.594584322869</v>
+        <v>-89735.975755785694</v>
       </c>
       <c r="E37" s="0">
-        <v>1946.9208902495245</v>
+        <v>2203.5659935089102</v>
       </c>
       <c r="F37" s="0">
-        <v>-179727.20098407147</v>
+        <v>-240324.11048978425</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>25.682593715061952</v>
+        <v>25.224446653666991</v>
       </c>
       <c r="B38" s="0">
-        <v>111.96927201492835</v>
+        <v>134.21966882959916</v>
       </c>
       <c r="C38" s="0">
-        <v>0.37641414892540781</v>
+        <v>0.49128607181745276</v>
       </c>
       <c r="D38" s="0">
-        <v>-74189.700060444899</v>
+        <v>-87152.034536242383</v>
       </c>
       <c r="E38" s="0">
-        <v>1871.625087867702</v>
+        <v>2168.2890795941012</v>
       </c>
       <c r="F38" s="0">
-        <v>-163005.97822984413</v>
+        <v>-230007.79738395623</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>25.553579504126002</v>
+        <v>25.854469424339616</v>
       </c>
       <c r="B39" s="0">
-        <v>131.65851548025063</v>
+        <v>132.16648355471114</v>
       </c>
       <c r="C39" s="0">
-        <v>0.33946165360563119</v>
+        <v>0.49128748399330657</v>
       </c>
       <c r="D39" s="0">
-        <v>-86617.821795030744</v>
+        <v>-87970.013739955437</v>
       </c>
       <c r="E39" s="0">
-        <v>2142.9987806236763</v>
+        <v>2154.2592032908265</v>
       </c>
       <c r="F39" s="0">
-        <v>-224280.67094260713</v>
+        <v>-228755.98933049801</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>25.618553385370983</v>
+        <v>25.854476872103522</v>
       </c>
       <c r="B40" s="0">
-        <v>135.93147780256623</v>
+        <v>132.16634503828544</v>
       </c>
       <c r="C40" s="0">
-        <v>0.42718729788386356</v>
+        <v>0.49128606881190878</v>
       </c>
       <c r="D40" s="0">
-        <v>-89623.258790606706</v>
+        <v>-87969.94785811675</v>
       </c>
       <c r="E40" s="0">
-        <v>2202.3119983048127</v>
+        <v>2154.2574748794736</v>
       </c>
       <c r="F40" s="0">
-        <v>-239714.30125701483</v>
+        <v>-228755.57723137201</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>25.756368310454423</v>
+        <v>25.224464846320679</v>
       </c>
       <c r="B41" s="0">
-        <v>121.84677821758635</v>
+        <v>132.16576405889214</v>
       </c>
       <c r="C41" s="0">
-        <v>0.39548545565116999</v>
+        <v>0.49128768276914009</v>
       </c>
       <c r="D41" s="0">
-        <v>-80874.27751679653</v>
+        <v>-85834.085151823718</v>
       </c>
       <c r="E41" s="0">
-        <v>2010.2785509216076</v>
+        <v>2139.7401932931771</v>
       </c>
       <c r="F41" s="0">
-        <v>-193638.66185013676</v>
+        <v>-223016.1919967712</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>25.8829071834597</v>
+        <v>25.618154901458492</v>
       </c>
       <c r="B42" s="0">
-        <v>129.69797905839431</v>
+        <v>124.89955852928965</v>
       </c>
       <c r="C42" s="0">
-        <v>0.39870977931111495</v>
+        <v>0.49128659578019829</v>
       </c>
       <c r="D42" s="0">
-        <v>-86439.72850348652</v>
+        <v>-82432.957791983237</v>
       </c>
       <c r="E42" s="0">
-        <v>2122.2664595147444</v>
+        <v>2047.8066379455877</v>
       </c>
       <c r="F42" s="0">
-        <v>-220532.75096585695</v>
+        <v>-202348.7403435061</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>22.746929212114072</v>
+        <v>25.224457167100017</v>
       </c>
       <c r="B43" s="0">
-        <v>101.67559507604604</v>
+        <v>124.89979492531337</v>
       </c>
       <c r="C43" s="0">
-        <v>0.43337692961180319</v>
+        <v>0.49128746254065059</v>
       </c>
       <c r="D43" s="0">
-        <v>-59791.363716217165</v>
+        <v>-81171.412683782619</v>
       </c>
       <c r="E43" s="0">
-        <v>1659.9104341176069</v>
+        <v>2038.7430494436885</v>
       </c>
       <c r="F43" s="0">
-        <v>-118568.62983205088</v>
+        <v>-199147.88443845845</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>25.620987519841727</v>
+        <v>25.712526358825286</v>
       </c>
       <c r="B44" s="0">
-        <v>125.64647255985861</v>
+        <v>119.9234638988224</v>
       </c>
       <c r="C44" s="0">
-        <v>0.38119036813335921</v>
+        <v>0.49128747522275901</v>
       </c>
       <c r="D44" s="0">
-        <v>-82927.369782510374</v>
+        <v>-79480.397081549381</v>
       </c>
       <c r="E44" s="0">
-        <v>2060.233508344952</v>
+        <v>1980.8122814328726</v>
       </c>
       <c r="F44" s="0">
-        <v>-204802.08007602533</v>
+        <v>-187238.9779896054</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>24.470486141913241</v>
+        <v>25.224454393768845</v>
       </c>
       <c r="B45" s="0">
-        <v>108.85339849603808</v>
+        <v>119.92296724081029</v>
       </c>
       <c r="C45" s="0">
-        <v>0.4709111763710514</v>
+        <v>0.49128748426137475</v>
       </c>
       <c r="D45" s="0">
-        <v>-68765.503044241661</v>
+        <v>-77977.723106737234</v>
       </c>
       <c r="E45" s="0">
-        <v>1798.7005519920397</v>
+        <v>1969.5650803687404</v>
       </c>
       <c r="F45" s="0">
-        <v>-146565.13893950562</v>
+        <v>-183578.61250759405</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>25.556305370846339</v>
+        <v>25.22447538390697</v>
       </c>
       <c r="B46" s="0">
-        <v>114.57979332813709</v>
+        <v>136.10557606294233</v>
       </c>
       <c r="C46" s="0">
-        <v>0.31515895258397691</v>
+        <v>0.49128740841170299</v>
       </c>
       <c r="D46" s="0">
-        <v>-75522.922106385318</v>
+        <v>-88362.34020298117</v>
       </c>
       <c r="E46" s="0">
-        <v>1906.1042819842369</v>
+        <v>2194.5038277630333</v>
       </c>
       <c r="F46" s="0">
-        <v>-169839.82536300496</v>
+        <v>-236522.99149003005</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>25.756368310454423</v>
+        <v>25.85447205251505</v>
       </c>
       <c r="B47" s="0">
-        <v>121.84677821758635</v>
+        <v>132.16651101412711</v>
       </c>
       <c r="C47" s="0">
-        <v>0.39548545565116999</v>
+        <v>0.49128736098724024</v>
       </c>
       <c r="D47" s="0">
-        <v>-80874.27751679653</v>
+        <v>-87970.040707848908</v>
       </c>
       <c r="E47" s="0">
-        <v>2010.2785509216076</v>
+        <v>2154.2596477152383</v>
       </c>
       <c r="F47" s="0">
-        <v>-193638.66185013676</v>
+        <v>-228756.10840614911</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>25.605704878238168</v>
+        <v>25.224492579728832</v>
       </c>
       <c r="B48" s="0">
-        <v>110.92928128259632</v>
+        <v>132.16640075832268</v>
       </c>
       <c r="C48" s="0">
-        <v>0.36817208146373365</v>
+        <v>0.49128638480306946</v>
       </c>
       <c r="D48" s="0">
-        <v>-73291.01208007583</v>
+        <v>-85834.587715993621</v>
       </c>
       <c r="E48" s="0">
-        <v>1855.5466591491959</v>
+        <v>2139.7497054530813</v>
       </c>
       <c r="F48" s="0">
-        <v>-159495.65984129821</v>
+        <v>-223018.59525675667</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>24.470486141913241</v>
+        <v>24.852730264801959</v>
       </c>
       <c r="B49" s="0">
-        <v>108.85339849603808</v>
+        <v>132.16639478769378</v>
       </c>
       <c r="C49" s="0">
-        <v>0.4709111763710514</v>
+        <v>0.49128762426799916</v>
       </c>
       <c r="D49" s="0">
-        <v>-68765.503044241661</v>
+        <v>-84574.457212525871</v>
       </c>
       <c r="E49" s="0">
-        <v>1798.7005519920397</v>
+        <v>2131.1879140629944</v>
       </c>
       <c r="F49" s="0">
-        <v>-146565.13893950562</v>
+        <v>-219632.99023224477</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>25.618553385370983</v>
+        <v>25.854493352718652</v>
       </c>
       <c r="B50" s="0">
-        <v>135.93147780256623</v>
+        <v>124.89977064302131</v>
       </c>
       <c r="C50" s="0">
-        <v>0.42718729788386356</v>
+        <v>0.49128747218902469</v>
       </c>
       <c r="D50" s="0">
-        <v>-89623.258790606706</v>
+        <v>-83190.499371275306</v>
       </c>
       <c r="E50" s="0">
-        <v>2202.3119983048127</v>
+        <v>2053.2524451011486</v>
       </c>
       <c r="F50" s="0">
-        <v>-239714.30125701483</v>
+        <v>-204271.3754316238</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>22.746929212114072</v>
+        <v>25.712527513888848</v>
       </c>
       <c r="B51" s="0">
-        <v>101.67559507604604</v>
+        <v>124.8997707999258</v>
       </c>
       <c r="C51" s="0">
-        <v>0.43337692961180319</v>
+        <v>0.4912874560972334</v>
       </c>
       <c r="D51" s="0">
-        <v>-59791.363716217165</v>
+        <v>-82735.53584791279</v>
       </c>
       <c r="E51" s="0">
-        <v>1659.9104341176069</v>
+        <v>2049.9829743032005</v>
       </c>
       <c r="F51" s="0">
-        <v>-118568.62983205088</v>
+        <v>-203116.88399926829</v>
       </c>
     </row>
     <row r="52">

</xml_diff>